<commit_message>
Update with new SvPortal API
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/CDBMeta.xlsx
+++ b/Excel_and_CSV/CDBMeta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F56E976-E039-48A9-B162-5119626058AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F83AEB4-00E4-4A23-82C1-0FD29A8B85B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="248">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -696,24 +696,6 @@
     <t>Corral Souls</t>
   </si>
   <si>
-    <t>LW (Ghost) Shadow</t>
-  </si>
-  <si>
-    <t>Tochella, Noble Necromancer</t>
-  </si>
-  <si>
-    <t>7YjpS</t>
-  </si>
-  <si>
-    <t>7JQpC</t>
-  </si>
-  <si>
-    <t>Suzy, Hexcaster</t>
-  </si>
-  <si>
-    <t>LW (Evo) Shadow</t>
-  </si>
-  <si>
     <t>7TLa2</t>
   </si>
   <si>
@@ -781,6 +763,18 @@
   </si>
   <si>
     <t>Badb Catha, Trine Goddess</t>
+  </si>
+  <si>
+    <t>Ghost Shadow</t>
+  </si>
+  <si>
+    <t>Opulent Strategist</t>
+  </si>
+  <si>
+    <t>7XaZy</t>
+  </si>
+  <si>
+    <t>Hybrid Shadow</t>
   </si>
 </sst>
 </file>
@@ -1080,10 +1074,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I1025"/>
+  <dimension ref="A1:I1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1200,10 +1194,10 @@
         <v>212</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1442,22 +1436,22 @@
     </row>
     <row r="14" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>6</v>
@@ -1500,16 +1494,16 @@
         <v>7</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>6</v>
@@ -1520,100 +1514,100 @@
     </row>
     <row r="17" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>111</v>
+        <v>49</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>111</v>
+        <v>159</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>159</v>
+        <v>111</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>160</v>
+        <v>112</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>162</v>
+        <v>111</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>6</v>
+        <v>112</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>6</v>
@@ -1622,24 +1616,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>11</v>
+        <v>178</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>44</v>
+        <v>180</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>45</v>
+        <v>179</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>44</v>
+        <v>181</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>45</v>
+        <v>182</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>6</v>
@@ -1648,24 +1642,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>12</v>
+    <row r="22" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>91</v>
+      <c r="C22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>6</v>
@@ -1676,48 +1670,48 @@
     </row>
     <row r="23" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F24" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>184</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>6</v>
@@ -1728,22 +1722,22 @@
     </row>
     <row r="25" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>113</v>
+        <v>48</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>114</v>
+        <v>49</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>117</v>
+        <v>183</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>116</v>
+        <v>184</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>6</v>
@@ -1754,22 +1748,22 @@
     </row>
     <row r="26" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>183</v>
+        <v>117</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>184</v>
+        <v>116</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>6</v>
@@ -1780,22 +1774,22 @@
     </row>
     <row r="27" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>118</v>
+        <v>183</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>119</v>
+        <v>184</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>6</v>
@@ -1815,7 +1809,7 @@
         <v>103</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>118</v>
@@ -1832,22 +1826,22 @@
     </row>
     <row r="29" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>185</v>
+        <v>13</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>186</v>
+        <v>103</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>187</v>
+        <v>104</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>188</v>
+        <v>118</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>189</v>
+        <v>119</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>6</v>
@@ -1858,22 +1852,22 @@
     </row>
     <row r="30" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>149</v>
+        <v>186</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>148</v>
+        <v>187</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>6</v>
@@ -1896,10 +1890,10 @@
         <v>148</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>234</v>
+        <v>183</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>233</v>
+        <v>184</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>6</v>
@@ -1910,22 +1904,22 @@
     </row>
     <row r="32" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>190</v>
+        <v>147</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>85</v>
+        <v>149</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>86</v>
+        <v>148</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>192</v>
+        <v>228</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>191</v>
+        <v>227</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>6</v>
@@ -1934,24 +1928,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>84</v>
+        <v>190</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>130</v>
+        <v>85</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>130</v>
+        <v>192</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>131</v>
+        <v>191</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>6</v>
@@ -1960,7 +1954,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>84</v>
       </c>
@@ -1971,169 +1965,169 @@
         <v>130</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>130</v>
       </c>
       <c r="F34" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+      <c r="E35" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>100</v>
+      <c r="C36" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="C37" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="H37" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G37" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>164</v>
+        <v>93</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>166</v>
+        <v>6</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>229</v>
+        <v>164</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>133</v>
+        <v>217</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>134</v>
+        <v>218</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>6</v>
+        <v>166</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>231</v>
+        <v>133</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>230</v>
+        <v>134</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>231</v>
+        <v>133</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>230</v>
+        <v>134</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>6</v>
@@ -2142,24 +2136,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>6</v>
@@ -2168,24 +2162,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>135</v>
+        <v>225</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>136</v>
+        <v>226</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>225</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>6</v>
@@ -2194,24 +2188,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>226</v>
+        <v>247</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>59</v>
+        <v>194</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>58</v>
+        <v>193</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>225</v>
+        <v>135</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>224</v>
+        <v>136</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>6</v>
@@ -2220,18 +2214,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>221</v>
+        <v>244</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>135</v>
+        <v>194</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>136</v>
+        <v>193</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>194</v>
@@ -2246,24 +2240,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>194</v>
+        <v>135</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>193</v>
+        <v>136</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>194</v>
+        <v>135</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>193</v>
+        <v>136</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>6</v>
@@ -2272,24 +2266,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>242</v>
+        <v>52</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>135</v>
+        <v>49</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>136</v>
+        <v>50</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>222</v>
+        <v>54</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>223</v>
+        <v>53</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>6</v>
@@ -2298,24 +2292,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>242</v>
+    <row r="47" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>135</v>
+        <v>31</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>136</v>
+        <v>32</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>135</v>
+        <v>195</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>6</v>
@@ -2323,25 +2317,26 @@
       <c r="H47" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>52</v>
+      <c r="I47" s="3"/>
+    </row>
+    <row r="48" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>49</v>
+        <v>197</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>50</v>
+        <v>198</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>54</v>
+        <v>120</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>6</v>
@@ -2349,25 +2344,26 @@
       <c r="H48" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I48" s="3"/>
+    </row>
+    <row r="49" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>195</v>
+        <v>73</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>196</v>
+        <v>74</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>6</v>
@@ -2377,24 +2373,24 @@
       </c>
       <c r="I49" s="3"/>
     </row>
-    <row r="50" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>35</v>
+        <v>199</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>120</v>
+        <v>203</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>121</v>
+        <v>202</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>6</v>
@@ -2406,22 +2402,22 @@
     </row>
     <row r="51" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>71</v>
+        <v>214</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>72</v>
+        <v>213</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>73</v>
+        <v>214</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>74</v>
+        <v>213</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>6</v>
@@ -2433,22 +2429,22 @@
     </row>
     <row r="52" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>199</v>
+        <v>56</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>201</v>
+        <v>49</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>203</v>
+        <v>42</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>202</v>
+        <v>43</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>6</v>
@@ -2456,26 +2452,25 @@
       <c r="H52" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I52" s="3"/>
     </row>
     <row r="53" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>17</v>
+        <v>204</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>6</v>
@@ -2483,26 +2478,25 @@
       <c r="H53" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I53" s="3"/>
     </row>
     <row r="54" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>49</v>
+        <v>122</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>42</v>
+        <v>216</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>43</v>
+        <v>215</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>6</v>
@@ -2511,24 +2505,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>204</v>
+        <v>19</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>205</v>
+        <v>37</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>208</v>
+        <v>38</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>6</v>
@@ -2537,24 +2531,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>122</v>
+        <v>40</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>123</v>
+        <v>41</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>216</v>
+        <v>42</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>215</v>
+        <v>43</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>6</v>
@@ -2563,24 +2557,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>21</v>
+        <v>83</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>6</v>
@@ -2589,24 +2583,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>39</v>
+        <v>150</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>40</v>
+        <v>152</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>41</v>
+        <v>151</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>42</v>
+        <v>152</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>43</v>
+        <v>151</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>6</v>
@@ -2617,22 +2611,22 @@
     </row>
     <row r="59" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>83</v>
+        <v>153</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>76</v>
+        <v>152</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>77</v>
+        <v>153</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>6</v>
@@ -2643,22 +2637,22 @@
     </row>
     <row r="60" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>150</v>
+        <v>55</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>152</v>
+        <v>49</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>151</v>
+        <v>50</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>152</v>
+        <v>46</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>151</v>
+        <v>47</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>6</v>
@@ -2669,22 +2663,22 @@
     </row>
     <row r="61" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>150</v>
+        <v>78</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>153</v>
+        <v>80</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>153</v>
+        <v>80</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>6</v>
@@ -2695,22 +2689,22 @@
     </row>
     <row r="62" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>49</v>
+        <v>106</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>6</v>
@@ -2721,48 +2715,48 @@
     </row>
     <row r="63" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>78</v>
+        <v>231</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>79</v>
+        <v>233</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>80</v>
+        <v>232</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>79</v>
+        <v>234</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>80</v>
+        <v>235</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>24</v>
+        <v>140</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>25</v>
+        <v>141</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>6</v>
@@ -2771,94 +2765,53 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>237</v>
+        <v>26</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>241</v>
+      <c r="C65" t="s">
+        <v>128</v>
+      </c>
+      <c r="D65" t="s">
+        <v>129</v>
+      </c>
+      <c r="E65" t="s">
+        <v>210</v>
+      </c>
+      <c r="F65" t="s">
+        <v>209</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>6</v>
-      </c>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
     </row>
     <row r="67" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C67" t="s">
-        <v>128</v>
-      </c>
-      <c r="D67" t="s">
-        <v>129</v>
-      </c>
-      <c r="E67" t="s">
-        <v>210</v>
-      </c>
-      <c r="F67" t="s">
-        <v>209</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H67" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-    </row>
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+    </row>
+    <row r="68" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="69" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
@@ -2869,12 +2822,21 @@
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
     </row>
-    <row r="70" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+    </row>
+    <row r="71" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
@@ -2890,43 +2852,29 @@
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
     </row>
-    <row r="73" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
     </row>
-    <row r="74" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-    </row>
-    <row r="75" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3"/>
-    </row>
+    <row r="74" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="76" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="77" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="78" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="79" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="80" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="81" spans="2:2" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="82" spans="2:2" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="81" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B81" s="7"/>
+    </row>
+    <row r="82" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B82" s="7"/>
+    </row>
     <row r="83" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B83" s="7"/>
     </row>
@@ -5749,12 +5697,6 @@
     </row>
     <row r="1023" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B1023" s="7"/>
-    </row>
-    <row r="1024" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B1024" s="7"/>
-    </row>
-    <row r="1025" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B1025" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5766,7 +5708,7 @@
           <x14:formula1>
             <xm:f>Class!$A$2:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>B83:B1025 B71:B75 J64:J65 R64:R65 Z64:Z65 AH64:AH65 AP64:AP65 AX64:AX65 BF64:BF65 BN64:BN65 BV64:BV65 CD64:CD65 CL64:CL65 CT64:CT65 DB64:DB65 DJ64:DJ65 DR64:DR65 DZ64:DZ65 EH64:EH65 EP64:EP65 EX64:EX65 FF64:FF65 FN64:FN65 FV64:FV65 GD64:GD65 GL64:GL65 GT64:GT65 HB64:HB65 HJ64:HJ65 HR64:HR65 HZ64:HZ65 IH64:IH65 IP64:IP65 IX64:IX65 JF64:JF65 JN64:JN65 JV64:JV65 KD64:KD65 KL64:KL65 KT64:KT65 LB64:LB65 LJ64:LJ65 LR64:LR65 LZ64:LZ65 MH64:MH65 MP64:MP65 MX64:MX65 NF64:NF65 NN64:NN65 NV64:NV65 OD64:OD65 OL64:OL65 OT64:OT65 PB64:PB65 PJ64:PJ65 PR64:PR65 PZ64:PZ65 QH64:QH65 QP64:QP65 QX64:QX65 RF64:RF65 RN64:RN65 RV64:RV65 SD64:SD65 SL64:SL65 ST64:ST65 TB64:TB65 TJ64:TJ65 TR64:TR65 TZ64:TZ65 UH64:UH65 UP64:UP65 UX64:UX65 VF64:VF65 VN64:VN65 VV64:VV65 WD64:WD65 WL64:WL65 WT64:WT65 XB64:XB65 XJ64:XJ65 XR64:XR65 XZ64:XZ65 YH64:YH65 YP64:YP65 YX64:YX65 ZF64:ZF65 ZN64:ZN65 ZV64:ZV65 AAD64:AAD65 AAL64:AAL65 AAT64:AAT65 ABB64:ABB65 ABJ64:ABJ65 ABR64:ABR65 ABZ64:ABZ65 ACH64:ACH65 ACP64:ACP65 ACX64:ACX65 ADF64:ADF65 ADN64:ADN65 ADV64:ADV65 AED64:AED65 AEL64:AEL65 AET64:AET65 AFB64:AFB65 AFJ64:AFJ65 AFR64:AFR65 AFZ64:AFZ65 AGH64:AGH65 AGP64:AGP65 AGX64:AGX65 AHF64:AHF65 AHN64:AHN65 AHV64:AHV65 AID64:AID65 AIL64:AIL65 AIT64:AIT65 AJB64:AJB65 AJJ64:AJJ65 AJR64:AJR65 AJZ64:AJZ65 AKH64:AKH65 AKP64:AKP65 AKX64:AKX65 ALF64:ALF65 ALN64:ALN65 ALV64:ALV65 AMD64:AMD65 AML64:AML65 AMT64:AMT65 ANB64:ANB65 ANJ64:ANJ65 ANR64:ANR65 ANZ64:ANZ65 AOH64:AOH65 AOP64:AOP65 AOX64:AOX65 APF64:APF65 APN64:APN65 APV64:APV65 AQD64:AQD65 AQL64:AQL65 AQT64:AQT65 ARB64:ARB65 ARJ64:ARJ65 ARR64:ARR65 ARZ64:ARZ65 ASH64:ASH65 ASP64:ASP65 ASX64:ASX65 ATF64:ATF65 ATN64:ATN65 ATV64:ATV65 AUD64:AUD65 AUL64:AUL65 AUT64:AUT65 AVB64:AVB65 AVJ64:AVJ65 AVR64:AVR65 AVZ64:AVZ65 AWH64:AWH65 AWP64:AWP65 AWX64:AWX65 AXF64:AXF65 AXN64:AXN65 AXV64:AXV65 AYD64:AYD65 AYL64:AYL65 AYT64:AYT65 AZB64:AZB65 AZJ64:AZJ65 AZR64:AZR65 AZZ64:AZZ65 BAH64:BAH65 BAP64:BAP65 BAX64:BAX65 BBF64:BBF65 BBN64:BBN65 BBV64:BBV65 BCD64:BCD65 BCL64:BCL65 BCT64:BCT65 BDB64:BDB65 BDJ64:BDJ65 BDR64:BDR65 BDZ64:BDZ65 BEH64:BEH65 BEP64:BEP65 BEX64:BEX65 BFF64:BFF65 BFN64:BFN65 BFV64:BFV65 BGD64:BGD65 BGL64:BGL65 BGT64:BGT65 BHB64:BHB65 BHJ64:BHJ65 BHR64:BHR65 BHZ64:BHZ65 BIH64:BIH65 BIP64:BIP65 BIX64:BIX65 BJF64:BJF65 BJN64:BJN65 BJV64:BJV65 BKD64:BKD65 BKL64:BKL65 BKT64:BKT65 BLB64:BLB65 BLJ64:BLJ65 BLR64:BLR65 BLZ64:BLZ65 BMH64:BMH65 BMP64:BMP65 BMX64:BMX65 BNF64:BNF65 BNN64:BNN65 BNV64:BNV65 BOD64:BOD65 BOL64:BOL65 BOT64:BOT65 BPB64:BPB65 BPJ64:BPJ65 BPR64:BPR65 BPZ64:BPZ65 BQH64:BQH65 BQP64:BQP65 BQX64:BQX65 BRF64:BRF65 BRN64:BRN65 BRV64:BRV65 BSD64:BSD65 BSL64:BSL65 BST64:BST65 BTB64:BTB65 BTJ64:BTJ65 BTR64:BTR65 BTZ64:BTZ65 BUH64:BUH65 BUP64:BUP65 BUX64:BUX65 BVF64:BVF65 BVN64:BVN65 BVV64:BVV65 BWD64:BWD65 BWL64:BWL65 BWT64:BWT65 BXB64:BXB65 BXJ64:BXJ65 BXR64:BXR65 BXZ64:BXZ65 BYH64:BYH65 BYP64:BYP65 BYX64:BYX65 BZF64:BZF65 BZN64:BZN65 BZV64:BZV65 CAD64:CAD65 CAL64:CAL65 CAT64:CAT65 CBB64:CBB65 CBJ64:CBJ65 CBR64:CBR65 CBZ64:CBZ65 CCH64:CCH65 CCP64:CCP65 CCX64:CCX65 CDF64:CDF65 CDN64:CDN65 CDV64:CDV65 CED64:CED65 CEL64:CEL65 CET64:CET65 CFB64:CFB65 CFJ64:CFJ65 CFR64:CFR65 CFZ64:CFZ65 CGH64:CGH65 CGP64:CGP65 CGX64:CGX65 CHF64:CHF65 CHN64:CHN65 CHV64:CHV65 CID64:CID65 CIL64:CIL65 CIT64:CIT65 CJB64:CJB65 CJJ64:CJJ65 CJR64:CJR65 CJZ64:CJZ65 CKH64:CKH65 CKP64:CKP65 CKX64:CKX65 CLF64:CLF65 CLN64:CLN65 CLV64:CLV65 CMD64:CMD65 CML64:CML65 CMT64:CMT65 CNB64:CNB65 CNJ64:CNJ65 CNR64:CNR65 CNZ64:CNZ65 COH64:COH65 COP64:COP65 COX64:COX65 CPF64:CPF65 CPN64:CPN65 CPV64:CPV65 CQD64:CQD65 CQL64:CQL65 CQT64:CQT65 CRB64:CRB65 CRJ64:CRJ65 CRR64:CRR65 CRZ64:CRZ65 CSH64:CSH65 CSP64:CSP65 CSX64:CSX65 CTF64:CTF65 CTN64:CTN65 CTV64:CTV65 CUD64:CUD65 CUL64:CUL65 CUT64:CUT65 CVB64:CVB65 CVJ64:CVJ65 CVR64:CVR65 CVZ64:CVZ65 CWH64:CWH65 CWP64:CWP65 CWX64:CWX65 CXF64:CXF65 CXN64:CXN65 CXV64:CXV65 CYD64:CYD65 CYL64:CYL65 CYT64:CYT65 CZB64:CZB65 CZJ64:CZJ65 CZR64:CZR65 CZZ64:CZZ65 DAH64:DAH65 DAP64:DAP65 DAX64:DAX65 DBF64:DBF65 DBN64:DBN65 DBV64:DBV65 DCD64:DCD65 DCL64:DCL65 DCT64:DCT65 DDB64:DDB65 DDJ64:DDJ65 DDR64:DDR65 DDZ64:DDZ65 DEH64:DEH65 DEP64:DEP65 DEX64:DEX65 DFF64:DFF65 DFN64:DFN65 DFV64:DFV65 DGD64:DGD65 DGL64:DGL65 DGT64:DGT65 DHB64:DHB65 DHJ64:DHJ65 DHR64:DHR65 DHZ64:DHZ65 DIH64:DIH65 DIP64:DIP65 DIX64:DIX65 DJF64:DJF65 DJN64:DJN65 DJV64:DJV65 DKD64:DKD65 DKL64:DKL65 DKT64:DKT65 DLB64:DLB65 DLJ64:DLJ65 DLR64:DLR65 DLZ64:DLZ65 DMH64:DMH65 DMP64:DMP65 DMX64:DMX65 DNF64:DNF65 DNN64:DNN65 DNV64:DNV65 DOD64:DOD65 DOL64:DOL65 DOT64:DOT65 DPB64:DPB65 DPJ64:DPJ65 DPR64:DPR65 DPZ64:DPZ65 DQH64:DQH65 DQP64:DQP65 DQX64:DQX65 DRF64:DRF65 DRN64:DRN65 DRV64:DRV65 DSD64:DSD65 DSL64:DSL65 DST64:DST65 DTB64:DTB65 DTJ64:DTJ65 DTR64:DTR65 DTZ64:DTZ65 DUH64:DUH65 DUP64:DUP65 DUX64:DUX65 DVF64:DVF65 DVN64:DVN65 DVV64:DVV65 DWD64:DWD65 DWL64:DWL65 DWT64:DWT65 DXB64:DXB65 DXJ64:DXJ65 DXR64:DXR65 DXZ64:DXZ65 DYH64:DYH65 DYP64:DYP65 DYX64:DYX65 DZF64:DZF65 DZN64:DZN65 DZV64:DZV65 EAD64:EAD65 EAL64:EAL65 EAT64:EAT65 EBB64:EBB65 EBJ64:EBJ65 EBR64:EBR65 EBZ64:EBZ65 ECH64:ECH65 ECP64:ECP65 ECX64:ECX65 EDF64:EDF65 EDN64:EDN65 EDV64:EDV65 EED64:EED65 EEL64:EEL65 EET64:EET65 EFB64:EFB65 EFJ64:EFJ65 EFR64:EFR65 EFZ64:EFZ65 EGH64:EGH65 EGP64:EGP65 EGX64:EGX65 EHF64:EHF65 EHN64:EHN65 EHV64:EHV65 EID64:EID65 EIL64:EIL65 EIT64:EIT65 EJB64:EJB65 EJJ64:EJJ65 EJR64:EJR65 EJZ64:EJZ65 EKH64:EKH65 EKP64:EKP65 EKX64:EKX65 ELF64:ELF65 ELN64:ELN65 ELV64:ELV65 EMD64:EMD65 EML64:EML65 EMT64:EMT65 ENB64:ENB65 ENJ64:ENJ65 ENR64:ENR65 ENZ64:ENZ65 EOH64:EOH65 EOP64:EOP65 EOX64:EOX65 EPF64:EPF65 EPN64:EPN65 EPV64:EPV65 EQD64:EQD65 EQL64:EQL65 EQT64:EQT65 ERB64:ERB65 ERJ64:ERJ65 ERR64:ERR65 ERZ64:ERZ65 ESH64:ESH65 ESP64:ESP65 ESX64:ESX65 ETF64:ETF65 ETN64:ETN65 ETV64:ETV65 EUD64:EUD65 EUL64:EUL65 EUT64:EUT65 EVB64:EVB65 EVJ64:EVJ65 EVR64:EVR65 EVZ64:EVZ65 EWH64:EWH65 EWP64:EWP65 EWX64:EWX65 EXF64:EXF65 EXN64:EXN65 EXV64:EXV65 EYD64:EYD65 EYL64:EYL65 EYT64:EYT65 EZB64:EZB65 EZJ64:EZJ65 EZR64:EZR65 EZZ64:EZZ65 FAH64:FAH65 FAP64:FAP65 FAX64:FAX65 FBF64:FBF65 FBN64:FBN65 FBV64:FBV65 FCD64:FCD65 FCL64:FCL65 FCT64:FCT65 FDB64:FDB65 FDJ64:FDJ65 FDR64:FDR65 FDZ64:FDZ65 FEH64:FEH65 FEP64:FEP65 FEX64:FEX65 FFF64:FFF65 FFN64:FFN65 FFV64:FFV65 FGD64:FGD65 FGL64:FGL65 FGT64:FGT65 FHB64:FHB65 FHJ64:FHJ65 FHR64:FHR65 FHZ64:FHZ65 FIH64:FIH65 FIP64:FIP65 FIX64:FIX65 FJF64:FJF65 FJN64:FJN65 FJV64:FJV65 FKD64:FKD65 FKL64:FKL65 FKT64:FKT65 FLB64:FLB65 FLJ64:FLJ65 FLR64:FLR65 FLZ64:FLZ65 FMH64:FMH65 FMP64:FMP65 FMX64:FMX65 FNF64:FNF65 FNN64:FNN65 FNV64:FNV65 FOD64:FOD65 FOL64:FOL65 FOT64:FOT65 FPB64:FPB65 FPJ64:FPJ65 FPR64:FPR65 FPZ64:FPZ65 FQH64:FQH65 FQP64:FQP65 FQX64:FQX65 FRF64:FRF65 FRN64:FRN65 FRV64:FRV65 FSD64:FSD65 FSL64:FSL65 FST64:FST65 FTB64:FTB65 FTJ64:FTJ65 FTR64:FTR65 FTZ64:FTZ65 FUH64:FUH65 FUP64:FUP65 FUX64:FUX65 FVF64:FVF65 FVN64:FVN65 FVV64:FVV65 FWD64:FWD65 FWL64:FWL65 FWT64:FWT65 FXB64:FXB65 FXJ64:FXJ65 FXR64:FXR65 FXZ64:FXZ65 FYH64:FYH65 FYP64:FYP65 FYX64:FYX65 FZF64:FZF65 FZN64:FZN65 FZV64:FZV65 GAD64:GAD65 GAL64:GAL65 GAT64:GAT65 GBB64:GBB65 GBJ64:GBJ65 GBR64:GBR65 GBZ64:GBZ65 GCH64:GCH65 GCP64:GCP65 GCX64:GCX65 GDF64:GDF65 GDN64:GDN65 GDV64:GDV65 GED64:GED65 GEL64:GEL65 GET64:GET65 GFB64:GFB65 GFJ64:GFJ65 GFR64:GFR65 GFZ64:GFZ65 GGH64:GGH65 GGP64:GGP65 GGX64:GGX65 GHF64:GHF65 GHN64:GHN65 GHV64:GHV65 GID64:GID65 GIL64:GIL65 GIT64:GIT65 GJB64:GJB65 GJJ64:GJJ65 GJR64:GJR65 GJZ64:GJZ65 GKH64:GKH65 GKP64:GKP65 GKX64:GKX65 GLF64:GLF65 GLN64:GLN65 GLV64:GLV65 GMD64:GMD65 GML64:GML65 GMT64:GMT65 GNB64:GNB65 GNJ64:GNJ65 GNR64:GNR65 GNZ64:GNZ65 GOH64:GOH65 GOP64:GOP65 GOX64:GOX65 GPF64:GPF65 GPN64:GPN65 GPV64:GPV65 GQD64:GQD65 GQL64:GQL65 GQT64:GQT65 GRB64:GRB65 GRJ64:GRJ65 GRR64:GRR65 GRZ64:GRZ65 GSH64:GSH65 GSP64:GSP65 GSX64:GSX65 GTF64:GTF65 GTN64:GTN65 GTV64:GTV65 GUD64:GUD65 GUL64:GUL65 GUT64:GUT65 GVB64:GVB65 GVJ64:GVJ65 GVR64:GVR65 GVZ64:GVZ65 GWH64:GWH65 GWP64:GWP65 GWX64:GWX65 GXF64:GXF65 GXN64:GXN65 GXV64:GXV65 GYD64:GYD65 GYL64:GYL65 GYT64:GYT65 GZB64:GZB65 GZJ64:GZJ65 GZR64:GZR65 GZZ64:GZZ65 HAH64:HAH65 HAP64:HAP65 HAX64:HAX65 HBF64:HBF65 HBN64:HBN65 HBV64:HBV65 HCD64:HCD65 HCL64:HCL65 HCT64:HCT65 HDB64:HDB65 HDJ64:HDJ65 HDR64:HDR65 HDZ64:HDZ65 HEH64:HEH65 HEP64:HEP65 HEX64:HEX65 HFF64:HFF65 HFN64:HFN65 HFV64:HFV65 HGD64:HGD65 HGL64:HGL65 HGT64:HGT65 HHB64:HHB65 HHJ64:HHJ65 HHR64:HHR65 HHZ64:HHZ65 HIH64:HIH65 HIP64:HIP65 HIX64:HIX65 HJF64:HJF65 HJN64:HJN65 HJV64:HJV65 HKD64:HKD65 HKL64:HKL65 HKT64:HKT65 HLB64:HLB65 HLJ64:HLJ65 HLR64:HLR65 HLZ64:HLZ65 HMH64:HMH65 HMP64:HMP65 HMX64:HMX65 HNF64:HNF65 HNN64:HNN65 HNV64:HNV65 HOD64:HOD65 HOL64:HOL65 HOT64:HOT65 HPB64:HPB65 HPJ64:HPJ65 HPR64:HPR65 HPZ64:HPZ65 HQH64:HQH65 HQP64:HQP65 HQX64:HQX65 HRF64:HRF65 HRN64:HRN65 HRV64:HRV65 HSD64:HSD65 HSL64:HSL65 HST64:HST65 HTB64:HTB65 HTJ64:HTJ65 HTR64:HTR65 HTZ64:HTZ65 HUH64:HUH65 HUP64:HUP65 HUX64:HUX65 HVF64:HVF65 HVN64:HVN65 HVV64:HVV65 HWD64:HWD65 HWL64:HWL65 HWT64:HWT65 HXB64:HXB65 HXJ64:HXJ65 HXR64:HXR65 HXZ64:HXZ65 HYH64:HYH65 HYP64:HYP65 HYX64:HYX65 HZF64:HZF65 HZN64:HZN65 HZV64:HZV65 IAD64:IAD65 IAL64:IAL65 IAT64:IAT65 IBB64:IBB65 IBJ64:IBJ65 IBR64:IBR65 IBZ64:IBZ65 ICH64:ICH65 ICP64:ICP65 ICX64:ICX65 IDF64:IDF65 IDN64:IDN65 IDV64:IDV65 IED64:IED65 IEL64:IEL65 IET64:IET65 IFB64:IFB65 IFJ64:IFJ65 IFR64:IFR65 IFZ64:IFZ65 IGH64:IGH65 IGP64:IGP65 IGX64:IGX65 IHF64:IHF65 IHN64:IHN65 IHV64:IHV65 IID64:IID65 IIL64:IIL65 IIT64:IIT65 IJB64:IJB65 IJJ64:IJJ65 IJR64:IJR65 IJZ64:IJZ65 IKH64:IKH65 IKP64:IKP65 IKX64:IKX65 ILF64:ILF65 ILN64:ILN65 ILV64:ILV65 IMD64:IMD65 IML64:IML65 IMT64:IMT65 INB64:INB65 INJ64:INJ65 INR64:INR65 INZ64:INZ65 IOH64:IOH65 IOP64:IOP65 IOX64:IOX65 IPF64:IPF65 IPN64:IPN65 IPV64:IPV65 IQD64:IQD65 IQL64:IQL65 IQT64:IQT65 IRB64:IRB65 IRJ64:IRJ65 IRR64:IRR65 IRZ64:IRZ65 ISH64:ISH65 ISP64:ISP65 ISX64:ISX65 ITF64:ITF65 ITN64:ITN65 ITV64:ITV65 IUD64:IUD65 IUL64:IUL65 IUT64:IUT65 IVB64:IVB65 IVJ64:IVJ65 IVR64:IVR65 IVZ64:IVZ65 IWH64:IWH65 IWP64:IWP65 IWX64:IWX65 IXF64:IXF65 IXN64:IXN65 IXV64:IXV65 IYD64:IYD65 IYL64:IYL65 IYT64:IYT65 IZB64:IZB65 IZJ64:IZJ65 IZR64:IZR65 IZZ64:IZZ65 JAH64:JAH65 JAP64:JAP65 JAX64:JAX65 JBF64:JBF65 JBN64:JBN65 JBV64:JBV65 JCD64:JCD65 JCL64:JCL65 JCT64:JCT65 JDB64:JDB65 JDJ64:JDJ65 JDR64:JDR65 JDZ64:JDZ65 JEH64:JEH65 JEP64:JEP65 JEX64:JEX65 JFF64:JFF65 JFN64:JFN65 JFV64:JFV65 JGD64:JGD65 JGL64:JGL65 JGT64:JGT65 JHB64:JHB65 JHJ64:JHJ65 JHR64:JHR65 JHZ64:JHZ65 JIH64:JIH65 JIP64:JIP65 JIX64:JIX65 JJF64:JJF65 JJN64:JJN65 JJV64:JJV65 JKD64:JKD65 JKL64:JKL65 JKT64:JKT65 JLB64:JLB65 JLJ64:JLJ65 JLR64:JLR65 JLZ64:JLZ65 JMH64:JMH65 JMP64:JMP65 JMX64:JMX65 JNF64:JNF65 JNN64:JNN65 JNV64:JNV65 JOD64:JOD65 JOL64:JOL65 JOT64:JOT65 JPB64:JPB65 JPJ64:JPJ65 JPR64:JPR65 JPZ64:JPZ65 JQH64:JQH65 JQP64:JQP65 JQX64:JQX65 JRF64:JRF65 JRN64:JRN65 JRV64:JRV65 JSD64:JSD65 JSL64:JSL65 JST64:JST65 JTB64:JTB65 JTJ64:JTJ65 JTR64:JTR65 JTZ64:JTZ65 JUH64:JUH65 JUP64:JUP65 JUX64:JUX65 JVF64:JVF65 JVN64:JVN65 JVV64:JVV65 JWD64:JWD65 JWL64:JWL65 JWT64:JWT65 JXB64:JXB65 JXJ64:JXJ65 JXR64:JXR65 JXZ64:JXZ65 JYH64:JYH65 JYP64:JYP65 JYX64:JYX65 JZF64:JZF65 JZN64:JZN65 JZV64:JZV65 KAD64:KAD65 KAL64:KAL65 KAT64:KAT65 KBB64:KBB65 KBJ64:KBJ65 KBR64:KBR65 KBZ64:KBZ65 KCH64:KCH65 KCP64:KCP65 KCX64:KCX65 KDF64:KDF65 KDN64:KDN65 KDV64:KDV65 KED64:KED65 KEL64:KEL65 KET64:KET65 KFB64:KFB65 KFJ64:KFJ65 KFR64:KFR65 KFZ64:KFZ65 KGH64:KGH65 KGP64:KGP65 KGX64:KGX65 KHF64:KHF65 KHN64:KHN65 KHV64:KHV65 KID64:KID65 KIL64:KIL65 KIT64:KIT65 KJB64:KJB65 KJJ64:KJJ65 KJR64:KJR65 KJZ64:KJZ65 KKH64:KKH65 KKP64:KKP65 KKX64:KKX65 KLF64:KLF65 KLN64:KLN65 KLV64:KLV65 KMD64:KMD65 KML64:KML65 KMT64:KMT65 KNB64:KNB65 KNJ64:KNJ65 KNR64:KNR65 KNZ64:KNZ65 KOH64:KOH65 KOP64:KOP65 KOX64:KOX65 KPF64:KPF65 KPN64:KPN65 KPV64:KPV65 KQD64:KQD65 KQL64:KQL65 KQT64:KQT65 KRB64:KRB65 KRJ64:KRJ65 KRR64:KRR65 KRZ64:KRZ65 KSH64:KSH65 KSP64:KSP65 KSX64:KSX65 KTF64:KTF65 KTN64:KTN65 KTV64:KTV65 KUD64:KUD65 KUL64:KUL65 KUT64:KUT65 KVB64:KVB65 KVJ64:KVJ65 KVR64:KVR65 KVZ64:KVZ65 KWH64:KWH65 KWP64:KWP65 KWX64:KWX65 KXF64:KXF65 KXN64:KXN65 KXV64:KXV65 KYD64:KYD65 KYL64:KYL65 KYT64:KYT65 KZB64:KZB65 KZJ64:KZJ65 KZR64:KZR65 KZZ64:KZZ65 LAH64:LAH65 LAP64:LAP65 LAX64:LAX65 LBF64:LBF65 LBN64:LBN65 LBV64:LBV65 LCD64:LCD65 LCL64:LCL65 LCT64:LCT65 LDB64:LDB65 LDJ64:LDJ65 LDR64:LDR65 LDZ64:LDZ65 LEH64:LEH65 LEP64:LEP65 LEX64:LEX65 LFF64:LFF65 LFN64:LFN65 LFV64:LFV65 LGD64:LGD65 LGL64:LGL65 LGT64:LGT65 LHB64:LHB65 LHJ64:LHJ65 LHR64:LHR65 LHZ64:LHZ65 LIH64:LIH65 LIP64:LIP65 LIX64:LIX65 LJF64:LJF65 LJN64:LJN65 LJV64:LJV65 LKD64:LKD65 LKL64:LKL65 LKT64:LKT65 LLB64:LLB65 LLJ64:LLJ65 LLR64:LLR65 LLZ64:LLZ65 LMH64:LMH65 LMP64:LMP65 LMX64:LMX65 LNF64:LNF65 LNN64:LNN65 LNV64:LNV65 LOD64:LOD65 LOL64:LOL65 LOT64:LOT65 LPB64:LPB65 LPJ64:LPJ65 LPR64:LPR65 LPZ64:LPZ65 LQH64:LQH65 LQP64:LQP65 LQX64:LQX65 LRF64:LRF65 LRN64:LRN65 LRV64:LRV65 LSD64:LSD65 LSL64:LSL65 LST64:LST65 LTB64:LTB65 LTJ64:LTJ65 LTR64:LTR65 LTZ64:LTZ65 LUH64:LUH65 LUP64:LUP65 LUX64:LUX65 LVF64:LVF65 LVN64:LVN65 LVV64:LVV65 LWD64:LWD65 LWL64:LWL65 LWT64:LWT65 LXB64:LXB65 LXJ64:LXJ65 LXR64:LXR65 LXZ64:LXZ65 LYH64:LYH65 LYP64:LYP65 LYX64:LYX65 LZF64:LZF65 LZN64:LZN65 LZV64:LZV65 MAD64:MAD65 MAL64:MAL65 MAT64:MAT65 MBB64:MBB65 MBJ64:MBJ65 MBR64:MBR65 MBZ64:MBZ65 MCH64:MCH65 MCP64:MCP65 MCX64:MCX65 MDF64:MDF65 MDN64:MDN65 MDV64:MDV65 MED64:MED65 MEL64:MEL65 MET64:MET65 MFB64:MFB65 MFJ64:MFJ65 MFR64:MFR65 MFZ64:MFZ65 MGH64:MGH65 MGP64:MGP65 MGX64:MGX65 MHF64:MHF65 MHN64:MHN65 MHV64:MHV65 MID64:MID65 MIL64:MIL65 MIT64:MIT65 MJB64:MJB65 MJJ64:MJJ65 MJR64:MJR65 MJZ64:MJZ65 MKH64:MKH65 MKP64:MKP65 MKX64:MKX65 MLF64:MLF65 MLN64:MLN65 MLV64:MLV65 MMD64:MMD65 MML64:MML65 MMT64:MMT65 MNB64:MNB65 MNJ64:MNJ65 MNR64:MNR65 MNZ64:MNZ65 MOH64:MOH65 MOP64:MOP65 MOX64:MOX65 MPF64:MPF65 MPN64:MPN65 MPV64:MPV65 MQD64:MQD65 MQL64:MQL65 MQT64:MQT65 MRB64:MRB65 MRJ64:MRJ65 MRR64:MRR65 MRZ64:MRZ65 MSH64:MSH65 MSP64:MSP65 MSX64:MSX65 MTF64:MTF65 MTN64:MTN65 MTV64:MTV65 MUD64:MUD65 MUL64:MUL65 MUT64:MUT65 MVB64:MVB65 MVJ64:MVJ65 MVR64:MVR65 MVZ64:MVZ65 MWH64:MWH65 MWP64:MWP65 MWX64:MWX65 MXF64:MXF65 MXN64:MXN65 MXV64:MXV65 MYD64:MYD65 MYL64:MYL65 MYT64:MYT65 MZB64:MZB65 MZJ64:MZJ65 MZR64:MZR65 MZZ64:MZZ65 NAH64:NAH65 NAP64:NAP65 NAX64:NAX65 NBF64:NBF65 NBN64:NBN65 NBV64:NBV65 NCD64:NCD65 NCL64:NCL65 NCT64:NCT65 NDB64:NDB65 NDJ64:NDJ65 NDR64:NDR65 NDZ64:NDZ65 NEH64:NEH65 NEP64:NEP65 NEX64:NEX65 NFF64:NFF65 NFN64:NFN65 NFV64:NFV65 NGD64:NGD65 NGL64:NGL65 NGT64:NGT65 NHB64:NHB65 NHJ64:NHJ65 NHR64:NHR65 NHZ64:NHZ65 NIH64:NIH65 NIP64:NIP65 NIX64:NIX65 NJF64:NJF65 NJN64:NJN65 NJV64:NJV65 NKD64:NKD65 NKL64:NKL65 NKT64:NKT65 NLB64:NLB65 NLJ64:NLJ65 NLR64:NLR65 NLZ64:NLZ65 NMH64:NMH65 NMP64:NMP65 NMX64:NMX65 NNF64:NNF65 NNN64:NNN65 NNV64:NNV65 NOD64:NOD65 NOL64:NOL65 NOT64:NOT65 NPB64:NPB65 NPJ64:NPJ65 NPR64:NPR65 NPZ64:NPZ65 NQH64:NQH65 NQP64:NQP65 NQX64:NQX65 NRF64:NRF65 NRN64:NRN65 NRV64:NRV65 NSD64:NSD65 NSL64:NSL65 NST64:NST65 NTB64:NTB65 NTJ64:NTJ65 NTR64:NTR65 NTZ64:NTZ65 NUH64:NUH65 NUP64:NUP65 NUX64:NUX65 NVF64:NVF65 NVN64:NVN65 NVV64:NVV65 NWD64:NWD65 NWL64:NWL65 NWT64:NWT65 NXB64:NXB65 NXJ64:NXJ65 NXR64:NXR65 NXZ64:NXZ65 NYH64:NYH65 NYP64:NYP65 NYX64:NYX65 NZF64:NZF65 NZN64:NZN65 NZV64:NZV65 OAD64:OAD65 OAL64:OAL65 OAT64:OAT65 OBB64:OBB65 OBJ64:OBJ65 OBR64:OBR65 OBZ64:OBZ65 OCH64:OCH65 OCP64:OCP65 OCX64:OCX65 ODF64:ODF65 ODN64:ODN65 ODV64:ODV65 OED64:OED65 OEL64:OEL65 OET64:OET65 OFB64:OFB65 OFJ64:OFJ65 OFR64:OFR65 OFZ64:OFZ65 OGH64:OGH65 OGP64:OGP65 OGX64:OGX65 OHF64:OHF65 OHN64:OHN65 OHV64:OHV65 OID64:OID65 OIL64:OIL65 OIT64:OIT65 OJB64:OJB65 OJJ64:OJJ65 OJR64:OJR65 OJZ64:OJZ65 OKH64:OKH65 OKP64:OKP65 OKX64:OKX65 OLF64:OLF65 OLN64:OLN65 OLV64:OLV65 OMD64:OMD65 OML64:OML65 OMT64:OMT65 ONB64:ONB65 ONJ64:ONJ65 ONR64:ONR65 ONZ64:ONZ65 OOH64:OOH65 OOP64:OOP65 OOX64:OOX65 OPF64:OPF65 OPN64:OPN65 OPV64:OPV65 OQD64:OQD65 OQL64:OQL65 OQT64:OQT65 ORB64:ORB65 ORJ64:ORJ65 ORR64:ORR65 ORZ64:ORZ65 OSH64:OSH65 OSP64:OSP65 OSX64:OSX65 OTF64:OTF65 OTN64:OTN65 OTV64:OTV65 OUD64:OUD65 OUL64:OUL65 OUT64:OUT65 OVB64:OVB65 OVJ64:OVJ65 OVR64:OVR65 OVZ64:OVZ65 OWH64:OWH65 OWP64:OWP65 OWX64:OWX65 OXF64:OXF65 OXN64:OXN65 OXV64:OXV65 OYD64:OYD65 OYL64:OYL65 OYT64:OYT65 OZB64:OZB65 OZJ64:OZJ65 OZR64:OZR65 OZZ64:OZZ65 PAH64:PAH65 PAP64:PAP65 PAX64:PAX65 PBF64:PBF65 PBN64:PBN65 PBV64:PBV65 PCD64:PCD65 PCL64:PCL65 PCT64:PCT65 PDB64:PDB65 PDJ64:PDJ65 PDR64:PDR65 PDZ64:PDZ65 PEH64:PEH65 PEP64:PEP65 PEX64:PEX65 PFF64:PFF65 PFN64:PFN65 PFV64:PFV65 PGD64:PGD65 PGL64:PGL65 PGT64:PGT65 PHB64:PHB65 PHJ64:PHJ65 PHR64:PHR65 PHZ64:PHZ65 PIH64:PIH65 PIP64:PIP65 PIX64:PIX65 PJF64:PJF65 PJN64:PJN65 PJV64:PJV65 PKD64:PKD65 PKL64:PKL65 PKT64:PKT65 PLB64:PLB65 PLJ64:PLJ65 PLR64:PLR65 PLZ64:PLZ65 PMH64:PMH65 PMP64:PMP65 PMX64:PMX65 PNF64:PNF65 PNN64:PNN65 PNV64:PNV65 POD64:POD65 POL64:POL65 POT64:POT65 PPB64:PPB65 PPJ64:PPJ65 PPR64:PPR65 PPZ64:PPZ65 PQH64:PQH65 PQP64:PQP65 PQX64:PQX65 PRF64:PRF65 PRN64:PRN65 PRV64:PRV65 PSD64:PSD65 PSL64:PSL65 PST64:PST65 PTB64:PTB65 PTJ64:PTJ65 PTR64:PTR65 PTZ64:PTZ65 PUH64:PUH65 PUP64:PUP65 PUX64:PUX65 PVF64:PVF65 PVN64:PVN65 PVV64:PVV65 PWD64:PWD65 PWL64:PWL65 PWT64:PWT65 PXB64:PXB65 PXJ64:PXJ65 PXR64:PXR65 PXZ64:PXZ65 PYH64:PYH65 PYP64:PYP65 PYX64:PYX65 PZF64:PZF65 PZN64:PZN65 PZV64:PZV65 QAD64:QAD65 QAL64:QAL65 QAT64:QAT65 QBB64:QBB65 QBJ64:QBJ65 QBR64:QBR65 QBZ64:QBZ65 QCH64:QCH65 QCP64:QCP65 QCX64:QCX65 QDF64:QDF65 QDN64:QDN65 QDV64:QDV65 QED64:QED65 QEL64:QEL65 QET64:QET65 QFB64:QFB65 QFJ64:QFJ65 QFR64:QFR65 QFZ64:QFZ65 QGH64:QGH65 QGP64:QGP65 QGX64:QGX65 QHF64:QHF65 QHN64:QHN65 QHV64:QHV65 QID64:QID65 QIL64:QIL65 QIT64:QIT65 QJB64:QJB65 QJJ64:QJJ65 QJR64:QJR65 QJZ64:QJZ65 QKH64:QKH65 QKP64:QKP65 QKX64:QKX65 QLF64:QLF65 QLN64:QLN65 QLV64:QLV65 QMD64:QMD65 QML64:QML65 QMT64:QMT65 QNB64:QNB65 QNJ64:QNJ65 QNR64:QNR65 QNZ64:QNZ65 QOH64:QOH65 QOP64:QOP65 QOX64:QOX65 QPF64:QPF65 QPN64:QPN65 QPV64:QPV65 QQD64:QQD65 QQL64:QQL65 QQT64:QQT65 QRB64:QRB65 QRJ64:QRJ65 QRR64:QRR65 QRZ64:QRZ65 QSH64:QSH65 QSP64:QSP65 QSX64:QSX65 QTF64:QTF65 QTN64:QTN65 QTV64:QTV65 QUD64:QUD65 QUL64:QUL65 QUT64:QUT65 QVB64:QVB65 QVJ64:QVJ65 QVR64:QVR65 QVZ64:QVZ65 QWH64:QWH65 QWP64:QWP65 QWX64:QWX65 QXF64:QXF65 QXN64:QXN65 QXV64:QXV65 QYD64:QYD65 QYL64:QYL65 QYT64:QYT65 QZB64:QZB65 QZJ64:QZJ65 QZR64:QZR65 QZZ64:QZZ65 RAH64:RAH65 RAP64:RAP65 RAX64:RAX65 RBF64:RBF65 RBN64:RBN65 RBV64:RBV65 RCD64:RCD65 RCL64:RCL65 RCT64:RCT65 RDB64:RDB65 RDJ64:RDJ65 RDR64:RDR65 RDZ64:RDZ65 REH64:REH65 REP64:REP65 REX64:REX65 RFF64:RFF65 RFN64:RFN65 RFV64:RFV65 RGD64:RGD65 RGL64:RGL65 RGT64:RGT65 RHB64:RHB65 RHJ64:RHJ65 RHR64:RHR65 RHZ64:RHZ65 RIH64:RIH65 RIP64:RIP65 RIX64:RIX65 RJF64:RJF65 RJN64:RJN65 RJV64:RJV65 RKD64:RKD65 RKL64:RKL65 RKT64:RKT65 RLB64:RLB65 RLJ64:RLJ65 RLR64:RLR65 RLZ64:RLZ65 RMH64:RMH65 RMP64:RMP65 RMX64:RMX65 RNF64:RNF65 RNN64:RNN65 RNV64:RNV65 ROD64:ROD65 ROL64:ROL65 ROT64:ROT65 RPB64:RPB65 RPJ64:RPJ65 RPR64:RPR65 RPZ64:RPZ65 RQH64:RQH65 RQP64:RQP65 RQX64:RQX65 RRF64:RRF65 RRN64:RRN65 RRV64:RRV65 RSD64:RSD65 RSL64:RSL65 RST64:RST65 RTB64:RTB65 RTJ64:RTJ65 RTR64:RTR65 RTZ64:RTZ65 RUH64:RUH65 RUP64:RUP65 RUX64:RUX65 RVF64:RVF65 RVN64:RVN65 RVV64:RVV65 RWD64:RWD65 RWL64:RWL65 RWT64:RWT65 RXB64:RXB65 RXJ64:RXJ65 RXR64:RXR65 RXZ64:RXZ65 RYH64:RYH65 RYP64:RYP65 RYX64:RYX65 RZF64:RZF65 RZN64:RZN65 RZV64:RZV65 SAD64:SAD65 SAL64:SAL65 SAT64:SAT65 SBB64:SBB65 SBJ64:SBJ65 SBR64:SBR65 SBZ64:SBZ65 SCH64:SCH65 SCP64:SCP65 SCX64:SCX65 SDF64:SDF65 SDN64:SDN65 SDV64:SDV65 SED64:SED65 SEL64:SEL65 SET64:SET65 SFB64:SFB65 SFJ64:SFJ65 SFR64:SFR65 SFZ64:SFZ65 SGH64:SGH65 SGP64:SGP65 SGX64:SGX65 SHF64:SHF65 SHN64:SHN65 SHV64:SHV65 SID64:SID65 SIL64:SIL65 SIT64:SIT65 SJB64:SJB65 SJJ64:SJJ65 SJR64:SJR65 SJZ64:SJZ65 SKH64:SKH65 SKP64:SKP65 SKX64:SKX65 SLF64:SLF65 SLN64:SLN65 SLV64:SLV65 SMD64:SMD65 SML64:SML65 SMT64:SMT65 SNB64:SNB65 SNJ64:SNJ65 SNR64:SNR65 SNZ64:SNZ65 SOH64:SOH65 SOP64:SOP65 SOX64:SOX65 SPF64:SPF65 SPN64:SPN65 SPV64:SPV65 SQD64:SQD65 SQL64:SQL65 SQT64:SQT65 SRB64:SRB65 SRJ64:SRJ65 SRR64:SRR65 SRZ64:SRZ65 SSH64:SSH65 SSP64:SSP65 SSX64:SSX65 STF64:STF65 STN64:STN65 STV64:STV65 SUD64:SUD65 SUL64:SUL65 SUT64:SUT65 SVB64:SVB65 SVJ64:SVJ65 SVR64:SVR65 SVZ64:SVZ65 SWH64:SWH65 SWP64:SWP65 SWX64:SWX65 SXF64:SXF65 SXN64:SXN65 SXV64:SXV65 SYD64:SYD65 SYL64:SYL65 SYT64:SYT65 SZB64:SZB65 SZJ64:SZJ65 SZR64:SZR65 SZZ64:SZZ65 TAH64:TAH65 TAP64:TAP65 TAX64:TAX65 TBF64:TBF65 TBN64:TBN65 TBV64:TBV65 TCD64:TCD65 TCL64:TCL65 TCT64:TCT65 TDB64:TDB65 TDJ64:TDJ65 TDR64:TDR65 TDZ64:TDZ65 TEH64:TEH65 TEP64:TEP65 TEX64:TEX65 TFF64:TFF65 TFN64:TFN65 TFV64:TFV65 TGD64:TGD65 TGL64:TGL65 TGT64:TGT65 THB64:THB65 THJ64:THJ65 THR64:THR65 THZ64:THZ65 TIH64:TIH65 TIP64:TIP65 TIX64:TIX65 TJF64:TJF65 TJN64:TJN65 TJV64:TJV65 TKD64:TKD65 TKL64:TKL65 TKT64:TKT65 TLB64:TLB65 TLJ64:TLJ65 TLR64:TLR65 TLZ64:TLZ65 TMH64:TMH65 TMP64:TMP65 TMX64:TMX65 TNF64:TNF65 TNN64:TNN65 TNV64:TNV65 TOD64:TOD65 TOL64:TOL65 TOT64:TOT65 TPB64:TPB65 TPJ64:TPJ65 TPR64:TPR65 TPZ64:TPZ65 TQH64:TQH65 TQP64:TQP65 TQX64:TQX65 TRF64:TRF65 TRN64:TRN65 TRV64:TRV65 TSD64:TSD65 TSL64:TSL65 TST64:TST65 TTB64:TTB65 TTJ64:TTJ65 TTR64:TTR65 TTZ64:TTZ65 TUH64:TUH65 TUP64:TUP65 TUX64:TUX65 TVF64:TVF65 TVN64:TVN65 TVV64:TVV65 TWD64:TWD65 TWL64:TWL65 TWT64:TWT65 TXB64:TXB65 TXJ64:TXJ65 TXR64:TXR65 TXZ64:TXZ65 TYH64:TYH65 TYP64:TYP65 TYX64:TYX65 TZF64:TZF65 TZN64:TZN65 TZV64:TZV65 UAD64:UAD65 UAL64:UAL65 UAT64:UAT65 UBB64:UBB65 UBJ64:UBJ65 UBR64:UBR65 UBZ64:UBZ65 UCH64:UCH65 UCP64:UCP65 UCX64:UCX65 UDF64:UDF65 UDN64:UDN65 UDV64:UDV65 UED64:UED65 UEL64:UEL65 UET64:UET65 UFB64:UFB65 UFJ64:UFJ65 UFR64:UFR65 UFZ64:UFZ65 UGH64:UGH65 UGP64:UGP65 UGX64:UGX65 UHF64:UHF65 UHN64:UHN65 UHV64:UHV65 UID64:UID65 UIL64:UIL65 UIT64:UIT65 UJB64:UJB65 UJJ64:UJJ65 UJR64:UJR65 UJZ64:UJZ65 UKH64:UKH65 UKP64:UKP65 UKX64:UKX65 ULF64:ULF65 ULN64:ULN65 ULV64:ULV65 UMD64:UMD65 UML64:UML65 UMT64:UMT65 UNB64:UNB65 UNJ64:UNJ65 UNR64:UNR65 UNZ64:UNZ65 UOH64:UOH65 UOP64:UOP65 UOX64:UOX65 UPF64:UPF65 UPN64:UPN65 UPV64:UPV65 UQD64:UQD65 UQL64:UQL65 UQT64:UQT65 URB64:URB65 URJ64:URJ65 URR64:URR65 URZ64:URZ65 USH64:USH65 USP64:USP65 USX64:USX65 UTF64:UTF65 UTN64:UTN65 UTV64:UTV65 UUD64:UUD65 UUL64:UUL65 UUT64:UUT65 UVB64:UVB65 UVJ64:UVJ65 UVR64:UVR65 UVZ64:UVZ65 UWH64:UWH65 UWP64:UWP65 UWX64:UWX65 UXF64:UXF65 UXN64:UXN65 UXV64:UXV65 UYD64:UYD65 UYL64:UYL65 UYT64:UYT65 UZB64:UZB65 UZJ64:UZJ65 UZR64:UZR65 UZZ64:UZZ65 VAH64:VAH65 VAP64:VAP65 VAX64:VAX65 VBF64:VBF65 VBN64:VBN65 VBV64:VBV65 VCD64:VCD65 VCL64:VCL65 VCT64:VCT65 VDB64:VDB65 VDJ64:VDJ65 VDR64:VDR65 VDZ64:VDZ65 VEH64:VEH65 VEP64:VEP65 VEX64:VEX65 VFF64:VFF65 VFN64:VFN65 VFV64:VFV65 VGD64:VGD65 VGL64:VGL65 VGT64:VGT65 VHB64:VHB65 VHJ64:VHJ65 VHR64:VHR65 VHZ64:VHZ65 VIH64:VIH65 VIP64:VIP65 VIX64:VIX65 VJF64:VJF65 VJN64:VJN65 VJV64:VJV65 VKD64:VKD65 VKL64:VKL65 VKT64:VKT65 VLB64:VLB65 VLJ64:VLJ65 VLR64:VLR65 VLZ64:VLZ65 VMH64:VMH65 VMP64:VMP65 VMX64:VMX65 VNF64:VNF65 VNN64:VNN65 VNV64:VNV65 VOD64:VOD65 VOL64:VOL65 VOT64:VOT65 VPB64:VPB65 VPJ64:VPJ65 VPR64:VPR65 VPZ64:VPZ65 VQH64:VQH65 VQP64:VQP65 VQX64:VQX65 VRF64:VRF65 VRN64:VRN65 VRV64:VRV65 VSD64:VSD65 VSL64:VSL65 VST64:VST65 VTB64:VTB65 VTJ64:VTJ65 VTR64:VTR65 VTZ64:VTZ65 VUH64:VUH65 VUP64:VUP65 VUX64:VUX65 VVF64:VVF65 VVN64:VVN65 VVV64:VVV65 VWD64:VWD65 VWL64:VWL65 VWT64:VWT65 VXB64:VXB65 VXJ64:VXJ65 VXR64:VXR65 VXZ64:VXZ65 VYH64:VYH65 VYP64:VYP65 VYX64:VYX65 VZF64:VZF65 VZN64:VZN65 VZV64:VZV65 WAD64:WAD65 WAL64:WAL65 WAT64:WAT65 WBB64:WBB65 WBJ64:WBJ65 WBR64:WBR65 WBZ64:WBZ65 WCH64:WCH65 WCP64:WCP65 WCX64:WCX65 WDF64:WDF65 WDN64:WDN65 WDV64:WDV65 WED64:WED65 WEL64:WEL65 WET64:WET65 WFB64:WFB65 WFJ64:WFJ65 WFR64:WFR65 WFZ64:WFZ65 WGH64:WGH65 WGP64:WGP65 WGX64:WGX65 WHF64:WHF65 WHN64:WHN65 WHV64:WHV65 WID64:WID65 WIL64:WIL65 WIT64:WIT65 WJB64:WJB65 WJJ64:WJJ65 WJR64:WJR65 WJZ64:WJZ65 WKH64:WKH65 WKP64:WKP65 WKX64:WKX65 WLF64:WLF65 WLN64:WLN65 WLV64:WLV65 WMD64:WMD65 WML64:WML65 WMT64:WMT65 WNB64:WNB65 WNJ64:WNJ65 WNR64:WNR65 WNZ64:WNZ65 WOH64:WOH65 WOP64:WOP65 WOX64:WOX65 WPF64:WPF65 WPN64:WPN65 WPV64:WPV65 WQD64:WQD65 WQL64:WQL65 WQT64:WQT65 WRB64:WRB65 WRJ64:WRJ65 WRR64:WRR65 WRZ64:WRZ65 WSH64:WSH65 WSP64:WSP65 WSX64:WSX65 WTF64:WTF65 WTN64:WTN65 WTV64:WTV65 WUD64:WUD65 WUL64:WUL65 WUT64:WUT65 WVB64:WVB65 WVJ64:WVJ65 WVR64:WVR65 WVZ64:WVZ65 WWH64:WWH65 WWP64:WWP65 WWX64:WWX65 WXF64:WXF65 WXN64:WXN65 WXV64:WXV65 WYD64:WYD65 WYL64:WYL65 WYT64:WYT65 WZB64:WZB65 WZJ64:WZJ65 WZR64:WZR65 WZZ64:WZZ65 XAH64:XAH65 XAP64:XAP65 XAX64:XAX65 XBF64:XBF65 XBN64:XBN65 XBV64:XBV65 XCD64:XCD65 XCL64:XCL65 XCT64:XCT65 XDB64:XDB65 XDJ64:XDJ65 XDR64:XDR65 XDZ64:XDZ65 XEH64:XEH65 XEP64:XEP65 XEX64:XEX65 B3:B69</xm:sqref>
+          <xm:sqref>B81:B1023 B69:B73 J62:J63 R62:R63 Z62:Z63 AH62:AH63 AP62:AP63 AX62:AX63 BF62:BF63 BN62:BN63 BV62:BV63 CD62:CD63 CL62:CL63 CT62:CT63 DB62:DB63 DJ62:DJ63 DR62:DR63 DZ62:DZ63 EH62:EH63 EP62:EP63 EX62:EX63 FF62:FF63 FN62:FN63 FV62:FV63 GD62:GD63 GL62:GL63 GT62:GT63 HB62:HB63 HJ62:HJ63 HR62:HR63 HZ62:HZ63 IH62:IH63 IP62:IP63 IX62:IX63 JF62:JF63 JN62:JN63 JV62:JV63 KD62:KD63 KL62:KL63 KT62:KT63 LB62:LB63 LJ62:LJ63 LR62:LR63 LZ62:LZ63 MH62:MH63 MP62:MP63 MX62:MX63 NF62:NF63 NN62:NN63 NV62:NV63 OD62:OD63 OL62:OL63 OT62:OT63 PB62:PB63 PJ62:PJ63 PR62:PR63 PZ62:PZ63 QH62:QH63 QP62:QP63 QX62:QX63 RF62:RF63 RN62:RN63 RV62:RV63 SD62:SD63 SL62:SL63 ST62:ST63 TB62:TB63 TJ62:TJ63 TR62:TR63 TZ62:TZ63 UH62:UH63 UP62:UP63 UX62:UX63 VF62:VF63 VN62:VN63 VV62:VV63 WD62:WD63 WL62:WL63 WT62:WT63 XB62:XB63 XJ62:XJ63 XR62:XR63 XZ62:XZ63 YH62:YH63 YP62:YP63 YX62:YX63 ZF62:ZF63 ZN62:ZN63 ZV62:ZV63 AAD62:AAD63 AAL62:AAL63 AAT62:AAT63 ABB62:ABB63 ABJ62:ABJ63 ABR62:ABR63 ABZ62:ABZ63 ACH62:ACH63 ACP62:ACP63 ACX62:ACX63 ADF62:ADF63 ADN62:ADN63 ADV62:ADV63 AED62:AED63 AEL62:AEL63 AET62:AET63 AFB62:AFB63 AFJ62:AFJ63 AFR62:AFR63 AFZ62:AFZ63 AGH62:AGH63 AGP62:AGP63 AGX62:AGX63 AHF62:AHF63 AHN62:AHN63 AHV62:AHV63 AID62:AID63 AIL62:AIL63 AIT62:AIT63 AJB62:AJB63 AJJ62:AJJ63 AJR62:AJR63 AJZ62:AJZ63 AKH62:AKH63 AKP62:AKP63 AKX62:AKX63 ALF62:ALF63 ALN62:ALN63 ALV62:ALV63 AMD62:AMD63 AML62:AML63 AMT62:AMT63 ANB62:ANB63 ANJ62:ANJ63 ANR62:ANR63 ANZ62:ANZ63 AOH62:AOH63 AOP62:AOP63 AOX62:AOX63 APF62:APF63 APN62:APN63 APV62:APV63 AQD62:AQD63 AQL62:AQL63 AQT62:AQT63 ARB62:ARB63 ARJ62:ARJ63 ARR62:ARR63 ARZ62:ARZ63 ASH62:ASH63 ASP62:ASP63 ASX62:ASX63 ATF62:ATF63 ATN62:ATN63 ATV62:ATV63 AUD62:AUD63 AUL62:AUL63 AUT62:AUT63 AVB62:AVB63 AVJ62:AVJ63 AVR62:AVR63 AVZ62:AVZ63 AWH62:AWH63 AWP62:AWP63 AWX62:AWX63 AXF62:AXF63 AXN62:AXN63 AXV62:AXV63 AYD62:AYD63 AYL62:AYL63 AYT62:AYT63 AZB62:AZB63 AZJ62:AZJ63 AZR62:AZR63 AZZ62:AZZ63 BAH62:BAH63 BAP62:BAP63 BAX62:BAX63 BBF62:BBF63 BBN62:BBN63 BBV62:BBV63 BCD62:BCD63 BCL62:BCL63 BCT62:BCT63 BDB62:BDB63 BDJ62:BDJ63 BDR62:BDR63 BDZ62:BDZ63 BEH62:BEH63 BEP62:BEP63 BEX62:BEX63 BFF62:BFF63 BFN62:BFN63 BFV62:BFV63 BGD62:BGD63 BGL62:BGL63 BGT62:BGT63 BHB62:BHB63 BHJ62:BHJ63 BHR62:BHR63 BHZ62:BHZ63 BIH62:BIH63 BIP62:BIP63 BIX62:BIX63 BJF62:BJF63 BJN62:BJN63 BJV62:BJV63 BKD62:BKD63 BKL62:BKL63 BKT62:BKT63 BLB62:BLB63 BLJ62:BLJ63 BLR62:BLR63 BLZ62:BLZ63 BMH62:BMH63 BMP62:BMP63 BMX62:BMX63 BNF62:BNF63 BNN62:BNN63 BNV62:BNV63 BOD62:BOD63 BOL62:BOL63 BOT62:BOT63 BPB62:BPB63 BPJ62:BPJ63 BPR62:BPR63 BPZ62:BPZ63 BQH62:BQH63 BQP62:BQP63 BQX62:BQX63 BRF62:BRF63 BRN62:BRN63 BRV62:BRV63 BSD62:BSD63 BSL62:BSL63 BST62:BST63 BTB62:BTB63 BTJ62:BTJ63 BTR62:BTR63 BTZ62:BTZ63 BUH62:BUH63 BUP62:BUP63 BUX62:BUX63 BVF62:BVF63 BVN62:BVN63 BVV62:BVV63 BWD62:BWD63 BWL62:BWL63 BWT62:BWT63 BXB62:BXB63 BXJ62:BXJ63 BXR62:BXR63 BXZ62:BXZ63 BYH62:BYH63 BYP62:BYP63 BYX62:BYX63 BZF62:BZF63 BZN62:BZN63 BZV62:BZV63 CAD62:CAD63 CAL62:CAL63 CAT62:CAT63 CBB62:CBB63 CBJ62:CBJ63 CBR62:CBR63 CBZ62:CBZ63 CCH62:CCH63 CCP62:CCP63 CCX62:CCX63 CDF62:CDF63 CDN62:CDN63 CDV62:CDV63 CED62:CED63 CEL62:CEL63 CET62:CET63 CFB62:CFB63 CFJ62:CFJ63 CFR62:CFR63 CFZ62:CFZ63 CGH62:CGH63 CGP62:CGP63 CGX62:CGX63 CHF62:CHF63 CHN62:CHN63 CHV62:CHV63 CID62:CID63 CIL62:CIL63 CIT62:CIT63 CJB62:CJB63 CJJ62:CJJ63 CJR62:CJR63 CJZ62:CJZ63 CKH62:CKH63 CKP62:CKP63 CKX62:CKX63 CLF62:CLF63 CLN62:CLN63 CLV62:CLV63 CMD62:CMD63 CML62:CML63 CMT62:CMT63 CNB62:CNB63 CNJ62:CNJ63 CNR62:CNR63 CNZ62:CNZ63 COH62:COH63 COP62:COP63 COX62:COX63 CPF62:CPF63 CPN62:CPN63 CPV62:CPV63 CQD62:CQD63 CQL62:CQL63 CQT62:CQT63 CRB62:CRB63 CRJ62:CRJ63 CRR62:CRR63 CRZ62:CRZ63 CSH62:CSH63 CSP62:CSP63 CSX62:CSX63 CTF62:CTF63 CTN62:CTN63 CTV62:CTV63 CUD62:CUD63 CUL62:CUL63 CUT62:CUT63 CVB62:CVB63 CVJ62:CVJ63 CVR62:CVR63 CVZ62:CVZ63 CWH62:CWH63 CWP62:CWP63 CWX62:CWX63 CXF62:CXF63 CXN62:CXN63 CXV62:CXV63 CYD62:CYD63 CYL62:CYL63 CYT62:CYT63 CZB62:CZB63 CZJ62:CZJ63 CZR62:CZR63 CZZ62:CZZ63 DAH62:DAH63 DAP62:DAP63 DAX62:DAX63 DBF62:DBF63 DBN62:DBN63 DBV62:DBV63 DCD62:DCD63 DCL62:DCL63 DCT62:DCT63 DDB62:DDB63 DDJ62:DDJ63 DDR62:DDR63 DDZ62:DDZ63 DEH62:DEH63 DEP62:DEP63 DEX62:DEX63 DFF62:DFF63 DFN62:DFN63 DFV62:DFV63 DGD62:DGD63 DGL62:DGL63 DGT62:DGT63 DHB62:DHB63 DHJ62:DHJ63 DHR62:DHR63 DHZ62:DHZ63 DIH62:DIH63 DIP62:DIP63 DIX62:DIX63 DJF62:DJF63 DJN62:DJN63 DJV62:DJV63 DKD62:DKD63 DKL62:DKL63 DKT62:DKT63 DLB62:DLB63 DLJ62:DLJ63 DLR62:DLR63 DLZ62:DLZ63 DMH62:DMH63 DMP62:DMP63 DMX62:DMX63 DNF62:DNF63 DNN62:DNN63 DNV62:DNV63 DOD62:DOD63 DOL62:DOL63 DOT62:DOT63 DPB62:DPB63 DPJ62:DPJ63 DPR62:DPR63 DPZ62:DPZ63 DQH62:DQH63 DQP62:DQP63 DQX62:DQX63 DRF62:DRF63 DRN62:DRN63 DRV62:DRV63 DSD62:DSD63 DSL62:DSL63 DST62:DST63 DTB62:DTB63 DTJ62:DTJ63 DTR62:DTR63 DTZ62:DTZ63 DUH62:DUH63 DUP62:DUP63 DUX62:DUX63 DVF62:DVF63 DVN62:DVN63 DVV62:DVV63 DWD62:DWD63 DWL62:DWL63 DWT62:DWT63 DXB62:DXB63 DXJ62:DXJ63 DXR62:DXR63 DXZ62:DXZ63 DYH62:DYH63 DYP62:DYP63 DYX62:DYX63 DZF62:DZF63 DZN62:DZN63 DZV62:DZV63 EAD62:EAD63 EAL62:EAL63 EAT62:EAT63 EBB62:EBB63 EBJ62:EBJ63 EBR62:EBR63 EBZ62:EBZ63 ECH62:ECH63 ECP62:ECP63 ECX62:ECX63 EDF62:EDF63 EDN62:EDN63 EDV62:EDV63 EED62:EED63 EEL62:EEL63 EET62:EET63 EFB62:EFB63 EFJ62:EFJ63 EFR62:EFR63 EFZ62:EFZ63 EGH62:EGH63 EGP62:EGP63 EGX62:EGX63 EHF62:EHF63 EHN62:EHN63 EHV62:EHV63 EID62:EID63 EIL62:EIL63 EIT62:EIT63 EJB62:EJB63 EJJ62:EJJ63 EJR62:EJR63 EJZ62:EJZ63 EKH62:EKH63 EKP62:EKP63 EKX62:EKX63 ELF62:ELF63 ELN62:ELN63 ELV62:ELV63 EMD62:EMD63 EML62:EML63 EMT62:EMT63 ENB62:ENB63 ENJ62:ENJ63 ENR62:ENR63 ENZ62:ENZ63 EOH62:EOH63 EOP62:EOP63 EOX62:EOX63 EPF62:EPF63 EPN62:EPN63 EPV62:EPV63 EQD62:EQD63 EQL62:EQL63 EQT62:EQT63 ERB62:ERB63 ERJ62:ERJ63 ERR62:ERR63 ERZ62:ERZ63 ESH62:ESH63 ESP62:ESP63 ESX62:ESX63 ETF62:ETF63 ETN62:ETN63 ETV62:ETV63 EUD62:EUD63 EUL62:EUL63 EUT62:EUT63 EVB62:EVB63 EVJ62:EVJ63 EVR62:EVR63 EVZ62:EVZ63 EWH62:EWH63 EWP62:EWP63 EWX62:EWX63 EXF62:EXF63 EXN62:EXN63 EXV62:EXV63 EYD62:EYD63 EYL62:EYL63 EYT62:EYT63 EZB62:EZB63 EZJ62:EZJ63 EZR62:EZR63 EZZ62:EZZ63 FAH62:FAH63 FAP62:FAP63 FAX62:FAX63 FBF62:FBF63 FBN62:FBN63 FBV62:FBV63 FCD62:FCD63 FCL62:FCL63 FCT62:FCT63 FDB62:FDB63 FDJ62:FDJ63 FDR62:FDR63 FDZ62:FDZ63 FEH62:FEH63 FEP62:FEP63 FEX62:FEX63 FFF62:FFF63 FFN62:FFN63 FFV62:FFV63 FGD62:FGD63 FGL62:FGL63 FGT62:FGT63 FHB62:FHB63 FHJ62:FHJ63 FHR62:FHR63 FHZ62:FHZ63 FIH62:FIH63 FIP62:FIP63 FIX62:FIX63 FJF62:FJF63 FJN62:FJN63 FJV62:FJV63 FKD62:FKD63 FKL62:FKL63 FKT62:FKT63 FLB62:FLB63 FLJ62:FLJ63 FLR62:FLR63 FLZ62:FLZ63 FMH62:FMH63 FMP62:FMP63 FMX62:FMX63 FNF62:FNF63 FNN62:FNN63 FNV62:FNV63 FOD62:FOD63 FOL62:FOL63 FOT62:FOT63 FPB62:FPB63 FPJ62:FPJ63 FPR62:FPR63 FPZ62:FPZ63 FQH62:FQH63 FQP62:FQP63 FQX62:FQX63 FRF62:FRF63 FRN62:FRN63 FRV62:FRV63 FSD62:FSD63 FSL62:FSL63 FST62:FST63 FTB62:FTB63 FTJ62:FTJ63 FTR62:FTR63 FTZ62:FTZ63 FUH62:FUH63 FUP62:FUP63 FUX62:FUX63 FVF62:FVF63 FVN62:FVN63 FVV62:FVV63 FWD62:FWD63 FWL62:FWL63 FWT62:FWT63 FXB62:FXB63 FXJ62:FXJ63 FXR62:FXR63 FXZ62:FXZ63 FYH62:FYH63 FYP62:FYP63 FYX62:FYX63 FZF62:FZF63 FZN62:FZN63 FZV62:FZV63 GAD62:GAD63 GAL62:GAL63 GAT62:GAT63 GBB62:GBB63 GBJ62:GBJ63 GBR62:GBR63 GBZ62:GBZ63 GCH62:GCH63 GCP62:GCP63 GCX62:GCX63 GDF62:GDF63 GDN62:GDN63 GDV62:GDV63 GED62:GED63 GEL62:GEL63 GET62:GET63 GFB62:GFB63 GFJ62:GFJ63 GFR62:GFR63 GFZ62:GFZ63 GGH62:GGH63 GGP62:GGP63 GGX62:GGX63 GHF62:GHF63 GHN62:GHN63 GHV62:GHV63 GID62:GID63 GIL62:GIL63 GIT62:GIT63 GJB62:GJB63 GJJ62:GJJ63 GJR62:GJR63 GJZ62:GJZ63 GKH62:GKH63 GKP62:GKP63 GKX62:GKX63 GLF62:GLF63 GLN62:GLN63 GLV62:GLV63 GMD62:GMD63 GML62:GML63 GMT62:GMT63 GNB62:GNB63 GNJ62:GNJ63 GNR62:GNR63 GNZ62:GNZ63 GOH62:GOH63 GOP62:GOP63 GOX62:GOX63 GPF62:GPF63 GPN62:GPN63 GPV62:GPV63 GQD62:GQD63 GQL62:GQL63 GQT62:GQT63 GRB62:GRB63 GRJ62:GRJ63 GRR62:GRR63 GRZ62:GRZ63 GSH62:GSH63 GSP62:GSP63 GSX62:GSX63 GTF62:GTF63 GTN62:GTN63 GTV62:GTV63 GUD62:GUD63 GUL62:GUL63 GUT62:GUT63 GVB62:GVB63 GVJ62:GVJ63 GVR62:GVR63 GVZ62:GVZ63 GWH62:GWH63 GWP62:GWP63 GWX62:GWX63 GXF62:GXF63 GXN62:GXN63 GXV62:GXV63 GYD62:GYD63 GYL62:GYL63 GYT62:GYT63 GZB62:GZB63 GZJ62:GZJ63 GZR62:GZR63 GZZ62:GZZ63 HAH62:HAH63 HAP62:HAP63 HAX62:HAX63 HBF62:HBF63 HBN62:HBN63 HBV62:HBV63 HCD62:HCD63 HCL62:HCL63 HCT62:HCT63 HDB62:HDB63 HDJ62:HDJ63 HDR62:HDR63 HDZ62:HDZ63 HEH62:HEH63 HEP62:HEP63 HEX62:HEX63 HFF62:HFF63 HFN62:HFN63 HFV62:HFV63 HGD62:HGD63 HGL62:HGL63 HGT62:HGT63 HHB62:HHB63 HHJ62:HHJ63 HHR62:HHR63 HHZ62:HHZ63 HIH62:HIH63 HIP62:HIP63 HIX62:HIX63 HJF62:HJF63 HJN62:HJN63 HJV62:HJV63 HKD62:HKD63 HKL62:HKL63 HKT62:HKT63 HLB62:HLB63 HLJ62:HLJ63 HLR62:HLR63 HLZ62:HLZ63 HMH62:HMH63 HMP62:HMP63 HMX62:HMX63 HNF62:HNF63 HNN62:HNN63 HNV62:HNV63 HOD62:HOD63 HOL62:HOL63 HOT62:HOT63 HPB62:HPB63 HPJ62:HPJ63 HPR62:HPR63 HPZ62:HPZ63 HQH62:HQH63 HQP62:HQP63 HQX62:HQX63 HRF62:HRF63 HRN62:HRN63 HRV62:HRV63 HSD62:HSD63 HSL62:HSL63 HST62:HST63 HTB62:HTB63 HTJ62:HTJ63 HTR62:HTR63 HTZ62:HTZ63 HUH62:HUH63 HUP62:HUP63 HUX62:HUX63 HVF62:HVF63 HVN62:HVN63 HVV62:HVV63 HWD62:HWD63 HWL62:HWL63 HWT62:HWT63 HXB62:HXB63 HXJ62:HXJ63 HXR62:HXR63 HXZ62:HXZ63 HYH62:HYH63 HYP62:HYP63 HYX62:HYX63 HZF62:HZF63 HZN62:HZN63 HZV62:HZV63 IAD62:IAD63 IAL62:IAL63 IAT62:IAT63 IBB62:IBB63 IBJ62:IBJ63 IBR62:IBR63 IBZ62:IBZ63 ICH62:ICH63 ICP62:ICP63 ICX62:ICX63 IDF62:IDF63 IDN62:IDN63 IDV62:IDV63 IED62:IED63 IEL62:IEL63 IET62:IET63 IFB62:IFB63 IFJ62:IFJ63 IFR62:IFR63 IFZ62:IFZ63 IGH62:IGH63 IGP62:IGP63 IGX62:IGX63 IHF62:IHF63 IHN62:IHN63 IHV62:IHV63 IID62:IID63 IIL62:IIL63 IIT62:IIT63 IJB62:IJB63 IJJ62:IJJ63 IJR62:IJR63 IJZ62:IJZ63 IKH62:IKH63 IKP62:IKP63 IKX62:IKX63 ILF62:ILF63 ILN62:ILN63 ILV62:ILV63 IMD62:IMD63 IML62:IML63 IMT62:IMT63 INB62:INB63 INJ62:INJ63 INR62:INR63 INZ62:INZ63 IOH62:IOH63 IOP62:IOP63 IOX62:IOX63 IPF62:IPF63 IPN62:IPN63 IPV62:IPV63 IQD62:IQD63 IQL62:IQL63 IQT62:IQT63 IRB62:IRB63 IRJ62:IRJ63 IRR62:IRR63 IRZ62:IRZ63 ISH62:ISH63 ISP62:ISP63 ISX62:ISX63 ITF62:ITF63 ITN62:ITN63 ITV62:ITV63 IUD62:IUD63 IUL62:IUL63 IUT62:IUT63 IVB62:IVB63 IVJ62:IVJ63 IVR62:IVR63 IVZ62:IVZ63 IWH62:IWH63 IWP62:IWP63 IWX62:IWX63 IXF62:IXF63 IXN62:IXN63 IXV62:IXV63 IYD62:IYD63 IYL62:IYL63 IYT62:IYT63 IZB62:IZB63 IZJ62:IZJ63 IZR62:IZR63 IZZ62:IZZ63 JAH62:JAH63 JAP62:JAP63 JAX62:JAX63 JBF62:JBF63 JBN62:JBN63 JBV62:JBV63 JCD62:JCD63 JCL62:JCL63 JCT62:JCT63 JDB62:JDB63 JDJ62:JDJ63 JDR62:JDR63 JDZ62:JDZ63 JEH62:JEH63 JEP62:JEP63 JEX62:JEX63 JFF62:JFF63 JFN62:JFN63 JFV62:JFV63 JGD62:JGD63 JGL62:JGL63 JGT62:JGT63 JHB62:JHB63 JHJ62:JHJ63 JHR62:JHR63 JHZ62:JHZ63 JIH62:JIH63 JIP62:JIP63 JIX62:JIX63 JJF62:JJF63 JJN62:JJN63 JJV62:JJV63 JKD62:JKD63 JKL62:JKL63 JKT62:JKT63 JLB62:JLB63 JLJ62:JLJ63 JLR62:JLR63 JLZ62:JLZ63 JMH62:JMH63 JMP62:JMP63 JMX62:JMX63 JNF62:JNF63 JNN62:JNN63 JNV62:JNV63 JOD62:JOD63 JOL62:JOL63 JOT62:JOT63 JPB62:JPB63 JPJ62:JPJ63 JPR62:JPR63 JPZ62:JPZ63 JQH62:JQH63 JQP62:JQP63 JQX62:JQX63 JRF62:JRF63 JRN62:JRN63 JRV62:JRV63 JSD62:JSD63 JSL62:JSL63 JST62:JST63 JTB62:JTB63 JTJ62:JTJ63 JTR62:JTR63 JTZ62:JTZ63 JUH62:JUH63 JUP62:JUP63 JUX62:JUX63 JVF62:JVF63 JVN62:JVN63 JVV62:JVV63 JWD62:JWD63 JWL62:JWL63 JWT62:JWT63 JXB62:JXB63 JXJ62:JXJ63 JXR62:JXR63 JXZ62:JXZ63 JYH62:JYH63 JYP62:JYP63 JYX62:JYX63 JZF62:JZF63 JZN62:JZN63 JZV62:JZV63 KAD62:KAD63 KAL62:KAL63 KAT62:KAT63 KBB62:KBB63 KBJ62:KBJ63 KBR62:KBR63 KBZ62:KBZ63 KCH62:KCH63 KCP62:KCP63 KCX62:KCX63 KDF62:KDF63 KDN62:KDN63 KDV62:KDV63 KED62:KED63 KEL62:KEL63 KET62:KET63 KFB62:KFB63 KFJ62:KFJ63 KFR62:KFR63 KFZ62:KFZ63 KGH62:KGH63 KGP62:KGP63 KGX62:KGX63 KHF62:KHF63 KHN62:KHN63 KHV62:KHV63 KID62:KID63 KIL62:KIL63 KIT62:KIT63 KJB62:KJB63 KJJ62:KJJ63 KJR62:KJR63 KJZ62:KJZ63 KKH62:KKH63 KKP62:KKP63 KKX62:KKX63 KLF62:KLF63 KLN62:KLN63 KLV62:KLV63 KMD62:KMD63 KML62:KML63 KMT62:KMT63 KNB62:KNB63 KNJ62:KNJ63 KNR62:KNR63 KNZ62:KNZ63 KOH62:KOH63 KOP62:KOP63 KOX62:KOX63 KPF62:KPF63 KPN62:KPN63 KPV62:KPV63 KQD62:KQD63 KQL62:KQL63 KQT62:KQT63 KRB62:KRB63 KRJ62:KRJ63 KRR62:KRR63 KRZ62:KRZ63 KSH62:KSH63 KSP62:KSP63 KSX62:KSX63 KTF62:KTF63 KTN62:KTN63 KTV62:KTV63 KUD62:KUD63 KUL62:KUL63 KUT62:KUT63 KVB62:KVB63 KVJ62:KVJ63 KVR62:KVR63 KVZ62:KVZ63 KWH62:KWH63 KWP62:KWP63 KWX62:KWX63 KXF62:KXF63 KXN62:KXN63 KXV62:KXV63 KYD62:KYD63 KYL62:KYL63 KYT62:KYT63 KZB62:KZB63 KZJ62:KZJ63 KZR62:KZR63 KZZ62:KZZ63 LAH62:LAH63 LAP62:LAP63 LAX62:LAX63 LBF62:LBF63 LBN62:LBN63 LBV62:LBV63 LCD62:LCD63 LCL62:LCL63 LCT62:LCT63 LDB62:LDB63 LDJ62:LDJ63 LDR62:LDR63 LDZ62:LDZ63 LEH62:LEH63 LEP62:LEP63 LEX62:LEX63 LFF62:LFF63 LFN62:LFN63 LFV62:LFV63 LGD62:LGD63 LGL62:LGL63 LGT62:LGT63 LHB62:LHB63 LHJ62:LHJ63 LHR62:LHR63 LHZ62:LHZ63 LIH62:LIH63 LIP62:LIP63 LIX62:LIX63 LJF62:LJF63 LJN62:LJN63 LJV62:LJV63 LKD62:LKD63 LKL62:LKL63 LKT62:LKT63 LLB62:LLB63 LLJ62:LLJ63 LLR62:LLR63 LLZ62:LLZ63 LMH62:LMH63 LMP62:LMP63 LMX62:LMX63 LNF62:LNF63 LNN62:LNN63 LNV62:LNV63 LOD62:LOD63 LOL62:LOL63 LOT62:LOT63 LPB62:LPB63 LPJ62:LPJ63 LPR62:LPR63 LPZ62:LPZ63 LQH62:LQH63 LQP62:LQP63 LQX62:LQX63 LRF62:LRF63 LRN62:LRN63 LRV62:LRV63 LSD62:LSD63 LSL62:LSL63 LST62:LST63 LTB62:LTB63 LTJ62:LTJ63 LTR62:LTR63 LTZ62:LTZ63 LUH62:LUH63 LUP62:LUP63 LUX62:LUX63 LVF62:LVF63 LVN62:LVN63 LVV62:LVV63 LWD62:LWD63 LWL62:LWL63 LWT62:LWT63 LXB62:LXB63 LXJ62:LXJ63 LXR62:LXR63 LXZ62:LXZ63 LYH62:LYH63 LYP62:LYP63 LYX62:LYX63 LZF62:LZF63 LZN62:LZN63 LZV62:LZV63 MAD62:MAD63 MAL62:MAL63 MAT62:MAT63 MBB62:MBB63 MBJ62:MBJ63 MBR62:MBR63 MBZ62:MBZ63 MCH62:MCH63 MCP62:MCP63 MCX62:MCX63 MDF62:MDF63 MDN62:MDN63 MDV62:MDV63 MED62:MED63 MEL62:MEL63 MET62:MET63 MFB62:MFB63 MFJ62:MFJ63 MFR62:MFR63 MFZ62:MFZ63 MGH62:MGH63 MGP62:MGP63 MGX62:MGX63 MHF62:MHF63 MHN62:MHN63 MHV62:MHV63 MID62:MID63 MIL62:MIL63 MIT62:MIT63 MJB62:MJB63 MJJ62:MJJ63 MJR62:MJR63 MJZ62:MJZ63 MKH62:MKH63 MKP62:MKP63 MKX62:MKX63 MLF62:MLF63 MLN62:MLN63 MLV62:MLV63 MMD62:MMD63 MML62:MML63 MMT62:MMT63 MNB62:MNB63 MNJ62:MNJ63 MNR62:MNR63 MNZ62:MNZ63 MOH62:MOH63 MOP62:MOP63 MOX62:MOX63 MPF62:MPF63 MPN62:MPN63 MPV62:MPV63 MQD62:MQD63 MQL62:MQL63 MQT62:MQT63 MRB62:MRB63 MRJ62:MRJ63 MRR62:MRR63 MRZ62:MRZ63 MSH62:MSH63 MSP62:MSP63 MSX62:MSX63 MTF62:MTF63 MTN62:MTN63 MTV62:MTV63 MUD62:MUD63 MUL62:MUL63 MUT62:MUT63 MVB62:MVB63 MVJ62:MVJ63 MVR62:MVR63 MVZ62:MVZ63 MWH62:MWH63 MWP62:MWP63 MWX62:MWX63 MXF62:MXF63 MXN62:MXN63 MXV62:MXV63 MYD62:MYD63 MYL62:MYL63 MYT62:MYT63 MZB62:MZB63 MZJ62:MZJ63 MZR62:MZR63 MZZ62:MZZ63 NAH62:NAH63 NAP62:NAP63 NAX62:NAX63 NBF62:NBF63 NBN62:NBN63 NBV62:NBV63 NCD62:NCD63 NCL62:NCL63 NCT62:NCT63 NDB62:NDB63 NDJ62:NDJ63 NDR62:NDR63 NDZ62:NDZ63 NEH62:NEH63 NEP62:NEP63 NEX62:NEX63 NFF62:NFF63 NFN62:NFN63 NFV62:NFV63 NGD62:NGD63 NGL62:NGL63 NGT62:NGT63 NHB62:NHB63 NHJ62:NHJ63 NHR62:NHR63 NHZ62:NHZ63 NIH62:NIH63 NIP62:NIP63 NIX62:NIX63 NJF62:NJF63 NJN62:NJN63 NJV62:NJV63 NKD62:NKD63 NKL62:NKL63 NKT62:NKT63 NLB62:NLB63 NLJ62:NLJ63 NLR62:NLR63 NLZ62:NLZ63 NMH62:NMH63 NMP62:NMP63 NMX62:NMX63 NNF62:NNF63 NNN62:NNN63 NNV62:NNV63 NOD62:NOD63 NOL62:NOL63 NOT62:NOT63 NPB62:NPB63 NPJ62:NPJ63 NPR62:NPR63 NPZ62:NPZ63 NQH62:NQH63 NQP62:NQP63 NQX62:NQX63 NRF62:NRF63 NRN62:NRN63 NRV62:NRV63 NSD62:NSD63 NSL62:NSL63 NST62:NST63 NTB62:NTB63 NTJ62:NTJ63 NTR62:NTR63 NTZ62:NTZ63 NUH62:NUH63 NUP62:NUP63 NUX62:NUX63 NVF62:NVF63 NVN62:NVN63 NVV62:NVV63 NWD62:NWD63 NWL62:NWL63 NWT62:NWT63 NXB62:NXB63 NXJ62:NXJ63 NXR62:NXR63 NXZ62:NXZ63 NYH62:NYH63 NYP62:NYP63 NYX62:NYX63 NZF62:NZF63 NZN62:NZN63 NZV62:NZV63 OAD62:OAD63 OAL62:OAL63 OAT62:OAT63 OBB62:OBB63 OBJ62:OBJ63 OBR62:OBR63 OBZ62:OBZ63 OCH62:OCH63 OCP62:OCP63 OCX62:OCX63 ODF62:ODF63 ODN62:ODN63 ODV62:ODV63 OED62:OED63 OEL62:OEL63 OET62:OET63 OFB62:OFB63 OFJ62:OFJ63 OFR62:OFR63 OFZ62:OFZ63 OGH62:OGH63 OGP62:OGP63 OGX62:OGX63 OHF62:OHF63 OHN62:OHN63 OHV62:OHV63 OID62:OID63 OIL62:OIL63 OIT62:OIT63 OJB62:OJB63 OJJ62:OJJ63 OJR62:OJR63 OJZ62:OJZ63 OKH62:OKH63 OKP62:OKP63 OKX62:OKX63 OLF62:OLF63 OLN62:OLN63 OLV62:OLV63 OMD62:OMD63 OML62:OML63 OMT62:OMT63 ONB62:ONB63 ONJ62:ONJ63 ONR62:ONR63 ONZ62:ONZ63 OOH62:OOH63 OOP62:OOP63 OOX62:OOX63 OPF62:OPF63 OPN62:OPN63 OPV62:OPV63 OQD62:OQD63 OQL62:OQL63 OQT62:OQT63 ORB62:ORB63 ORJ62:ORJ63 ORR62:ORR63 ORZ62:ORZ63 OSH62:OSH63 OSP62:OSP63 OSX62:OSX63 OTF62:OTF63 OTN62:OTN63 OTV62:OTV63 OUD62:OUD63 OUL62:OUL63 OUT62:OUT63 OVB62:OVB63 OVJ62:OVJ63 OVR62:OVR63 OVZ62:OVZ63 OWH62:OWH63 OWP62:OWP63 OWX62:OWX63 OXF62:OXF63 OXN62:OXN63 OXV62:OXV63 OYD62:OYD63 OYL62:OYL63 OYT62:OYT63 OZB62:OZB63 OZJ62:OZJ63 OZR62:OZR63 OZZ62:OZZ63 PAH62:PAH63 PAP62:PAP63 PAX62:PAX63 PBF62:PBF63 PBN62:PBN63 PBV62:PBV63 PCD62:PCD63 PCL62:PCL63 PCT62:PCT63 PDB62:PDB63 PDJ62:PDJ63 PDR62:PDR63 PDZ62:PDZ63 PEH62:PEH63 PEP62:PEP63 PEX62:PEX63 PFF62:PFF63 PFN62:PFN63 PFV62:PFV63 PGD62:PGD63 PGL62:PGL63 PGT62:PGT63 PHB62:PHB63 PHJ62:PHJ63 PHR62:PHR63 PHZ62:PHZ63 PIH62:PIH63 PIP62:PIP63 PIX62:PIX63 PJF62:PJF63 PJN62:PJN63 PJV62:PJV63 PKD62:PKD63 PKL62:PKL63 PKT62:PKT63 PLB62:PLB63 PLJ62:PLJ63 PLR62:PLR63 PLZ62:PLZ63 PMH62:PMH63 PMP62:PMP63 PMX62:PMX63 PNF62:PNF63 PNN62:PNN63 PNV62:PNV63 POD62:POD63 POL62:POL63 POT62:POT63 PPB62:PPB63 PPJ62:PPJ63 PPR62:PPR63 PPZ62:PPZ63 PQH62:PQH63 PQP62:PQP63 PQX62:PQX63 PRF62:PRF63 PRN62:PRN63 PRV62:PRV63 PSD62:PSD63 PSL62:PSL63 PST62:PST63 PTB62:PTB63 PTJ62:PTJ63 PTR62:PTR63 PTZ62:PTZ63 PUH62:PUH63 PUP62:PUP63 PUX62:PUX63 PVF62:PVF63 PVN62:PVN63 PVV62:PVV63 PWD62:PWD63 PWL62:PWL63 PWT62:PWT63 PXB62:PXB63 PXJ62:PXJ63 PXR62:PXR63 PXZ62:PXZ63 PYH62:PYH63 PYP62:PYP63 PYX62:PYX63 PZF62:PZF63 PZN62:PZN63 PZV62:PZV63 QAD62:QAD63 QAL62:QAL63 QAT62:QAT63 QBB62:QBB63 QBJ62:QBJ63 QBR62:QBR63 QBZ62:QBZ63 QCH62:QCH63 QCP62:QCP63 QCX62:QCX63 QDF62:QDF63 QDN62:QDN63 QDV62:QDV63 QED62:QED63 QEL62:QEL63 QET62:QET63 QFB62:QFB63 QFJ62:QFJ63 QFR62:QFR63 QFZ62:QFZ63 QGH62:QGH63 QGP62:QGP63 QGX62:QGX63 QHF62:QHF63 QHN62:QHN63 QHV62:QHV63 QID62:QID63 QIL62:QIL63 QIT62:QIT63 QJB62:QJB63 QJJ62:QJJ63 QJR62:QJR63 QJZ62:QJZ63 QKH62:QKH63 QKP62:QKP63 QKX62:QKX63 QLF62:QLF63 QLN62:QLN63 QLV62:QLV63 QMD62:QMD63 QML62:QML63 QMT62:QMT63 QNB62:QNB63 QNJ62:QNJ63 QNR62:QNR63 QNZ62:QNZ63 QOH62:QOH63 QOP62:QOP63 QOX62:QOX63 QPF62:QPF63 QPN62:QPN63 QPV62:QPV63 QQD62:QQD63 QQL62:QQL63 QQT62:QQT63 QRB62:QRB63 QRJ62:QRJ63 QRR62:QRR63 QRZ62:QRZ63 QSH62:QSH63 QSP62:QSP63 QSX62:QSX63 QTF62:QTF63 QTN62:QTN63 QTV62:QTV63 QUD62:QUD63 QUL62:QUL63 QUT62:QUT63 QVB62:QVB63 QVJ62:QVJ63 QVR62:QVR63 QVZ62:QVZ63 QWH62:QWH63 QWP62:QWP63 QWX62:QWX63 QXF62:QXF63 QXN62:QXN63 QXV62:QXV63 QYD62:QYD63 QYL62:QYL63 QYT62:QYT63 QZB62:QZB63 QZJ62:QZJ63 QZR62:QZR63 QZZ62:QZZ63 RAH62:RAH63 RAP62:RAP63 RAX62:RAX63 RBF62:RBF63 RBN62:RBN63 RBV62:RBV63 RCD62:RCD63 RCL62:RCL63 RCT62:RCT63 RDB62:RDB63 RDJ62:RDJ63 RDR62:RDR63 RDZ62:RDZ63 REH62:REH63 REP62:REP63 REX62:REX63 RFF62:RFF63 RFN62:RFN63 RFV62:RFV63 RGD62:RGD63 RGL62:RGL63 RGT62:RGT63 RHB62:RHB63 RHJ62:RHJ63 RHR62:RHR63 RHZ62:RHZ63 RIH62:RIH63 RIP62:RIP63 RIX62:RIX63 RJF62:RJF63 RJN62:RJN63 RJV62:RJV63 RKD62:RKD63 RKL62:RKL63 RKT62:RKT63 RLB62:RLB63 RLJ62:RLJ63 RLR62:RLR63 RLZ62:RLZ63 RMH62:RMH63 RMP62:RMP63 RMX62:RMX63 RNF62:RNF63 RNN62:RNN63 RNV62:RNV63 ROD62:ROD63 ROL62:ROL63 ROT62:ROT63 RPB62:RPB63 RPJ62:RPJ63 RPR62:RPR63 RPZ62:RPZ63 RQH62:RQH63 RQP62:RQP63 RQX62:RQX63 RRF62:RRF63 RRN62:RRN63 RRV62:RRV63 RSD62:RSD63 RSL62:RSL63 RST62:RST63 RTB62:RTB63 RTJ62:RTJ63 RTR62:RTR63 RTZ62:RTZ63 RUH62:RUH63 RUP62:RUP63 RUX62:RUX63 RVF62:RVF63 RVN62:RVN63 RVV62:RVV63 RWD62:RWD63 RWL62:RWL63 RWT62:RWT63 RXB62:RXB63 RXJ62:RXJ63 RXR62:RXR63 RXZ62:RXZ63 RYH62:RYH63 RYP62:RYP63 RYX62:RYX63 RZF62:RZF63 RZN62:RZN63 RZV62:RZV63 SAD62:SAD63 SAL62:SAL63 SAT62:SAT63 SBB62:SBB63 SBJ62:SBJ63 SBR62:SBR63 SBZ62:SBZ63 SCH62:SCH63 SCP62:SCP63 SCX62:SCX63 SDF62:SDF63 SDN62:SDN63 SDV62:SDV63 SED62:SED63 SEL62:SEL63 SET62:SET63 SFB62:SFB63 SFJ62:SFJ63 SFR62:SFR63 SFZ62:SFZ63 SGH62:SGH63 SGP62:SGP63 SGX62:SGX63 SHF62:SHF63 SHN62:SHN63 SHV62:SHV63 SID62:SID63 SIL62:SIL63 SIT62:SIT63 SJB62:SJB63 SJJ62:SJJ63 SJR62:SJR63 SJZ62:SJZ63 SKH62:SKH63 SKP62:SKP63 SKX62:SKX63 SLF62:SLF63 SLN62:SLN63 SLV62:SLV63 SMD62:SMD63 SML62:SML63 SMT62:SMT63 SNB62:SNB63 SNJ62:SNJ63 SNR62:SNR63 SNZ62:SNZ63 SOH62:SOH63 SOP62:SOP63 SOX62:SOX63 SPF62:SPF63 SPN62:SPN63 SPV62:SPV63 SQD62:SQD63 SQL62:SQL63 SQT62:SQT63 SRB62:SRB63 SRJ62:SRJ63 SRR62:SRR63 SRZ62:SRZ63 SSH62:SSH63 SSP62:SSP63 SSX62:SSX63 STF62:STF63 STN62:STN63 STV62:STV63 SUD62:SUD63 SUL62:SUL63 SUT62:SUT63 SVB62:SVB63 SVJ62:SVJ63 SVR62:SVR63 SVZ62:SVZ63 SWH62:SWH63 SWP62:SWP63 SWX62:SWX63 SXF62:SXF63 SXN62:SXN63 SXV62:SXV63 SYD62:SYD63 SYL62:SYL63 SYT62:SYT63 SZB62:SZB63 SZJ62:SZJ63 SZR62:SZR63 SZZ62:SZZ63 TAH62:TAH63 TAP62:TAP63 TAX62:TAX63 TBF62:TBF63 TBN62:TBN63 TBV62:TBV63 TCD62:TCD63 TCL62:TCL63 TCT62:TCT63 TDB62:TDB63 TDJ62:TDJ63 TDR62:TDR63 TDZ62:TDZ63 TEH62:TEH63 TEP62:TEP63 TEX62:TEX63 TFF62:TFF63 TFN62:TFN63 TFV62:TFV63 TGD62:TGD63 TGL62:TGL63 TGT62:TGT63 THB62:THB63 THJ62:THJ63 THR62:THR63 THZ62:THZ63 TIH62:TIH63 TIP62:TIP63 TIX62:TIX63 TJF62:TJF63 TJN62:TJN63 TJV62:TJV63 TKD62:TKD63 TKL62:TKL63 TKT62:TKT63 TLB62:TLB63 TLJ62:TLJ63 TLR62:TLR63 TLZ62:TLZ63 TMH62:TMH63 TMP62:TMP63 TMX62:TMX63 TNF62:TNF63 TNN62:TNN63 TNV62:TNV63 TOD62:TOD63 TOL62:TOL63 TOT62:TOT63 TPB62:TPB63 TPJ62:TPJ63 TPR62:TPR63 TPZ62:TPZ63 TQH62:TQH63 TQP62:TQP63 TQX62:TQX63 TRF62:TRF63 TRN62:TRN63 TRV62:TRV63 TSD62:TSD63 TSL62:TSL63 TST62:TST63 TTB62:TTB63 TTJ62:TTJ63 TTR62:TTR63 TTZ62:TTZ63 TUH62:TUH63 TUP62:TUP63 TUX62:TUX63 TVF62:TVF63 TVN62:TVN63 TVV62:TVV63 TWD62:TWD63 TWL62:TWL63 TWT62:TWT63 TXB62:TXB63 TXJ62:TXJ63 TXR62:TXR63 TXZ62:TXZ63 TYH62:TYH63 TYP62:TYP63 TYX62:TYX63 TZF62:TZF63 TZN62:TZN63 TZV62:TZV63 UAD62:UAD63 UAL62:UAL63 UAT62:UAT63 UBB62:UBB63 UBJ62:UBJ63 UBR62:UBR63 UBZ62:UBZ63 UCH62:UCH63 UCP62:UCP63 UCX62:UCX63 UDF62:UDF63 UDN62:UDN63 UDV62:UDV63 UED62:UED63 UEL62:UEL63 UET62:UET63 UFB62:UFB63 UFJ62:UFJ63 UFR62:UFR63 UFZ62:UFZ63 UGH62:UGH63 UGP62:UGP63 UGX62:UGX63 UHF62:UHF63 UHN62:UHN63 UHV62:UHV63 UID62:UID63 UIL62:UIL63 UIT62:UIT63 UJB62:UJB63 UJJ62:UJJ63 UJR62:UJR63 UJZ62:UJZ63 UKH62:UKH63 UKP62:UKP63 UKX62:UKX63 ULF62:ULF63 ULN62:ULN63 ULV62:ULV63 UMD62:UMD63 UML62:UML63 UMT62:UMT63 UNB62:UNB63 UNJ62:UNJ63 UNR62:UNR63 UNZ62:UNZ63 UOH62:UOH63 UOP62:UOP63 UOX62:UOX63 UPF62:UPF63 UPN62:UPN63 UPV62:UPV63 UQD62:UQD63 UQL62:UQL63 UQT62:UQT63 URB62:URB63 URJ62:URJ63 URR62:URR63 URZ62:URZ63 USH62:USH63 USP62:USP63 USX62:USX63 UTF62:UTF63 UTN62:UTN63 UTV62:UTV63 UUD62:UUD63 UUL62:UUL63 UUT62:UUT63 UVB62:UVB63 UVJ62:UVJ63 UVR62:UVR63 UVZ62:UVZ63 UWH62:UWH63 UWP62:UWP63 UWX62:UWX63 UXF62:UXF63 UXN62:UXN63 UXV62:UXV63 UYD62:UYD63 UYL62:UYL63 UYT62:UYT63 UZB62:UZB63 UZJ62:UZJ63 UZR62:UZR63 UZZ62:UZZ63 VAH62:VAH63 VAP62:VAP63 VAX62:VAX63 VBF62:VBF63 VBN62:VBN63 VBV62:VBV63 VCD62:VCD63 VCL62:VCL63 VCT62:VCT63 VDB62:VDB63 VDJ62:VDJ63 VDR62:VDR63 VDZ62:VDZ63 VEH62:VEH63 VEP62:VEP63 VEX62:VEX63 VFF62:VFF63 VFN62:VFN63 VFV62:VFV63 VGD62:VGD63 VGL62:VGL63 VGT62:VGT63 VHB62:VHB63 VHJ62:VHJ63 VHR62:VHR63 VHZ62:VHZ63 VIH62:VIH63 VIP62:VIP63 VIX62:VIX63 VJF62:VJF63 VJN62:VJN63 VJV62:VJV63 VKD62:VKD63 VKL62:VKL63 VKT62:VKT63 VLB62:VLB63 VLJ62:VLJ63 VLR62:VLR63 VLZ62:VLZ63 VMH62:VMH63 VMP62:VMP63 VMX62:VMX63 VNF62:VNF63 VNN62:VNN63 VNV62:VNV63 VOD62:VOD63 VOL62:VOL63 VOT62:VOT63 VPB62:VPB63 VPJ62:VPJ63 VPR62:VPR63 VPZ62:VPZ63 VQH62:VQH63 VQP62:VQP63 VQX62:VQX63 VRF62:VRF63 VRN62:VRN63 VRV62:VRV63 VSD62:VSD63 VSL62:VSL63 VST62:VST63 VTB62:VTB63 VTJ62:VTJ63 VTR62:VTR63 VTZ62:VTZ63 VUH62:VUH63 VUP62:VUP63 VUX62:VUX63 VVF62:VVF63 VVN62:VVN63 VVV62:VVV63 VWD62:VWD63 VWL62:VWL63 VWT62:VWT63 VXB62:VXB63 VXJ62:VXJ63 VXR62:VXR63 VXZ62:VXZ63 VYH62:VYH63 VYP62:VYP63 VYX62:VYX63 VZF62:VZF63 VZN62:VZN63 VZV62:VZV63 WAD62:WAD63 WAL62:WAL63 WAT62:WAT63 WBB62:WBB63 WBJ62:WBJ63 WBR62:WBR63 WBZ62:WBZ63 WCH62:WCH63 WCP62:WCP63 WCX62:WCX63 WDF62:WDF63 WDN62:WDN63 WDV62:WDV63 WED62:WED63 WEL62:WEL63 WET62:WET63 WFB62:WFB63 WFJ62:WFJ63 WFR62:WFR63 WFZ62:WFZ63 WGH62:WGH63 WGP62:WGP63 WGX62:WGX63 WHF62:WHF63 WHN62:WHN63 WHV62:WHV63 WID62:WID63 WIL62:WIL63 WIT62:WIT63 WJB62:WJB63 WJJ62:WJJ63 WJR62:WJR63 WJZ62:WJZ63 WKH62:WKH63 WKP62:WKP63 WKX62:WKX63 WLF62:WLF63 WLN62:WLN63 WLV62:WLV63 WMD62:WMD63 WML62:WML63 WMT62:WMT63 WNB62:WNB63 WNJ62:WNJ63 WNR62:WNR63 WNZ62:WNZ63 WOH62:WOH63 WOP62:WOP63 WOX62:WOX63 WPF62:WPF63 WPN62:WPN63 WPV62:WPV63 WQD62:WQD63 WQL62:WQL63 WQT62:WQT63 WRB62:WRB63 WRJ62:WRJ63 WRR62:WRR63 WRZ62:WRZ63 WSH62:WSH63 WSP62:WSP63 WSX62:WSX63 WTF62:WTF63 WTN62:WTN63 WTV62:WTV63 WUD62:WUD63 WUL62:WUL63 WUT62:WUT63 WVB62:WVB63 WVJ62:WVJ63 WVR62:WVR63 WVZ62:WVZ63 WWH62:WWH63 WWP62:WWP63 WWX62:WWX63 WXF62:WXF63 WXN62:WXN63 WXV62:WXV63 WYD62:WYD63 WYL62:WYL63 WYT62:WYT63 WZB62:WZB63 WZJ62:WZJ63 WZR62:WZR63 WZZ62:WZZ63 XAH62:XAH63 XAP62:XAP63 XAX62:XAX63 XBF62:XBF63 XBN62:XBN63 XBV62:XBV63 XCD62:XCD63 XCL62:XCL63 XCT62:XCT63 XDB62:XDB63 XDJ62:XDJ63 XDR62:XDR63 XDZ62:XDZ63 XEH62:XEH63 XEP62:XEP63 XEX62:XEX63 B3:B67</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
CC + Azvaldt Update
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/CDBMeta.xlsx
+++ b/Excel_and_CSV/CDBMeta.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\ShadowverseUtility\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F83AEB4-00E4-4A23-82C1-0FD29A8B85B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CFB25F-3A55-4BA9-AA93-42C8E94C4585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,9 +21,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="278">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -231,12 +232,6 @@
     <t>7PyHy</t>
   </si>
   <si>
-    <t>Night on the Town</t>
-  </si>
-  <si>
-    <t>7PwaQ</t>
-  </si>
-  <si>
     <t>Yukishima, Master Biographer</t>
   </si>
   <si>
@@ -312,9 +307,6 @@
     <t>Forbidden Archives Warden</t>
   </si>
   <si>
-    <t>F&amp;G Shadow</t>
-  </si>
-  <si>
     <t>Harnessed Flame</t>
   </si>
   <si>
@@ -411,12 +403,6 @@
     <t>7LjI2</t>
   </si>
   <si>
-    <t>7R5XS</t>
-  </si>
-  <si>
-    <t>Lakandula, Purgatory Inn</t>
-  </si>
-  <si>
     <t>Cassim, the Courageous</t>
   </si>
   <si>
@@ -525,15 +511,6 @@
     <t>7U8rS</t>
   </si>
   <si>
-    <t>Aggro BR Shadow</t>
-  </si>
-  <si>
-    <t>7Uvgc</t>
-  </si>
-  <si>
-    <t>Mordecai, Unending Duelist</t>
-  </si>
-  <si>
     <t>Kagemitsu, Lost Samurai</t>
   </si>
   <si>
@@ -684,18 +661,6 @@
     <t>Skullfane, the Defiled</t>
   </si>
   <si>
-    <t>Anisage, Lost Forsaken</t>
-  </si>
-  <si>
-    <t>7R5XI</t>
-  </si>
-  <si>
-    <t>7UrWg</t>
-  </si>
-  <si>
-    <t>Corral Souls</t>
-  </si>
-  <si>
     <t>7TLa2</t>
   </si>
   <si>
@@ -775,6 +740,132 @@
   </si>
   <si>
     <t>Hybrid Shadow</t>
+  </si>
+  <si>
+    <t>7Jrfy</t>
+  </si>
+  <si>
+    <t>Bloodsucker of the Night</t>
+  </si>
+  <si>
+    <t>Evo Wrath Blood</t>
+  </si>
+  <si>
+    <t>7Jrg6</t>
+  </si>
+  <si>
+    <t>Bloodlust Demon</t>
+  </si>
+  <si>
+    <t>QuickCoin Sword</t>
+  </si>
+  <si>
+    <t>7Vxb2</t>
+  </si>
+  <si>
+    <t>Blossoming Flower Doll</t>
+  </si>
+  <si>
+    <t>7QI-w</t>
+  </si>
+  <si>
+    <t>Story of a Lifetime</t>
+  </si>
+  <si>
+    <t>7JQpC</t>
+  </si>
+  <si>
+    <t>Suzy, Hexcaster</t>
+  </si>
+  <si>
+    <t>7MsXi</t>
+  </si>
+  <si>
+    <t>Draconic Mercenary</t>
+  </si>
+  <si>
+    <t>Discard Dragon</t>
+  </si>
+  <si>
+    <t>Pazuzu Blood</t>
+  </si>
+  <si>
+    <t>Eccentric Archdemon</t>
+  </si>
+  <si>
+    <t>Pazuzu, Noxious Gale</t>
+  </si>
+  <si>
+    <t>7Z6E6</t>
+  </si>
+  <si>
+    <t>7NdMi</t>
+  </si>
+  <si>
+    <t>7YLP6</t>
+  </si>
+  <si>
+    <t>Lumiore, Prestigious Gold</t>
+  </si>
+  <si>
+    <t>Argente, Purest Silver</t>
+  </si>
+  <si>
+    <t>7YIys</t>
+  </si>
+  <si>
+    <t>Terra Finis</t>
+  </si>
+  <si>
+    <t>7SzPA</t>
+  </si>
+  <si>
+    <t>7Zt2o</t>
+  </si>
+  <si>
+    <t>Vyrmedea, Synthetic Voice</t>
+  </si>
+  <si>
+    <t>Evo BR Shadow</t>
+  </si>
+  <si>
+    <t>7Q-CY</t>
+  </si>
+  <si>
+    <t>Inn Ghosthound</t>
+  </si>
+  <si>
+    <t>Control Rune</t>
+  </si>
+  <si>
+    <t>Meltina, Miracle Sorceress</t>
+  </si>
+  <si>
+    <t>7Xy-S</t>
+  </si>
+  <si>
+    <t>7Wpko</t>
+  </si>
+  <si>
+    <t>Uranus</t>
+  </si>
+  <si>
+    <t>Hozumi Forest</t>
+  </si>
+  <si>
+    <t>Garuel, Seraphic Leo</t>
+  </si>
+  <si>
+    <t>7WnIY</t>
+  </si>
+  <si>
+    <t>7PZtI</t>
+  </si>
+  <si>
+    <t>glhGI</t>
+  </si>
+  <si>
+    <t>Hozumi, Enchanting Hostess</t>
   </si>
 </sst>
 </file>
@@ -1074,10 +1165,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I1023"/>
+  <dimension ref="A1:I1034"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1149,22 +1240,22 @@
     </row>
     <row r="3" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>107</v>
+        <v>272</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>143</v>
+        <v>273</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>142</v>
+        <v>274</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>145</v>
+        <v>277</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>144</v>
+        <v>275</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>6</v>
@@ -1174,206 +1265,208 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>172</v>
+        <v>272</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>174</v>
+      <c r="C4" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>274</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>211</v>
+        <v>277</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>212</v>
+        <v>276</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>222</v>
+        <v>6</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>34</v>
+      <c r="C5" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>109</v>
+        <v>6</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>110</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>33</v>
+        <v>165</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>191</v>
+        <v>166</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>204</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>109</v>
+        <v>210</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>171</v>
+        <v>33</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>170</v>
+        <v>34</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>108</v>
+        <v>141</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>110</v>
+        <v>34</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>51</v>
+        <v>161</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>50</v>
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>8</v>
+        <v>163</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>6</v>
@@ -1384,22 +1477,22 @@
     </row>
     <row r="12" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>175</v>
+        <v>93</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>176</v>
+        <v>94</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>177</v>
+        <v>95</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>176</v>
+        <v>94</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>177</v>
+        <v>95</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>6</v>
@@ -1408,24 +1501,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>158</v>
+        <v>169</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>6</v>
@@ -1436,22 +1529,22 @@
     </row>
     <row r="14" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>239</v>
+        <v>149</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>241</v>
+        <v>151</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>240</v>
+        <v>150</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>243</v>
+        <v>152</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>242</v>
+        <v>153</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>6</v>
@@ -1460,50 +1553,50 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>87</v>
+        <v>227</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>167</v>
+        <v>229</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>168</v>
+        <v>228</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>230</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>87</v>
+        <v>241</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>245</v>
+        <v>64</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>246</v>
+        <v>65</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>6</v>
@@ -1514,22 +1607,22 @@
     </row>
     <row r="17" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>230</v>
+        <v>64</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>229</v>
+        <v>65</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>230</v>
+        <v>64</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>229</v>
+        <v>65</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>6</v>
@@ -1540,16 +1633,16 @@
     </row>
     <row r="18" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>49</v>
+        <v>159</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>50</v>
+        <v>160</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>159</v>
@@ -1564,50 +1657,50 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>111</v>
+        <v>233</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>112</v>
+        <v>234</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>111</v>
+        <v>233</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>161</v>
+        <v>85</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>159</v>
+        <v>218</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>160</v>
+        <v>217</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>162</v>
+        <v>218</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>163</v>
+        <v>217</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>6</v>
@@ -1618,22 +1711,22 @@
     </row>
     <row r="21" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>178</v>
+        <v>60</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>180</v>
+        <v>49</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>179</v>
+        <v>50</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>181</v>
+        <v>245</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>182</v>
+        <v>244</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>6</v>
@@ -1642,50 +1735,50 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>12</v>
+        <v>109</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>156</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>91</v>
+      <c r="C23" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>6</v>
@@ -1694,24 +1787,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>62</v>
+    <row r="24" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>69</v>
+      <c r="C24" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>6</v>
@@ -1720,128 +1813,128 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>119</v>
+        <v>50</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>248</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>6</v>
@@ -1852,22 +1945,22 @@
     </row>
     <row r="30" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>185</v>
+        <v>48</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>186</v>
+        <v>49</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>187</v>
+        <v>50</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>6</v>
@@ -1878,22 +1971,22 @@
     </row>
     <row r="31" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>183</v>
+        <v>114</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>184</v>
+        <v>113</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>6</v>
@@ -1904,22 +1997,22 @@
     </row>
     <row r="32" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>147</v>
+        <v>86</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>149</v>
+        <v>91</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>148</v>
+        <v>92</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>228</v>
+        <v>175</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>227</v>
+        <v>176</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>6</v>
@@ -1928,24 +2021,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>190</v>
+        <v>13</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>192</v>
+        <v>115</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>191</v>
+        <v>116</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>6</v>
@@ -1954,24 +2047,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>84</v>
+        <v>13</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>6</v>
@@ -1980,24 +2073,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>84</v>
+        <v>177</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>130</v>
+        <v>178</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>130</v>
+        <v>180</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>132</v>
+        <v>181</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>6</v>
@@ -2006,180 +2099,180 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>223</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>225</v>
+        <v>49</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>226</v>
+        <v>50</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>225</v>
+        <v>59</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>226</v>
+        <v>58</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>6</v>
@@ -2188,50 +2281,50 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>247</v>
+        <v>98</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>136</v>
+      <c r="C43" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>244</v>
+        <v>211</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>194</v>
+        <v>128</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>193</v>
+        <v>129</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>194</v>
+        <v>128</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>193</v>
+        <v>129</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>6</v>
@@ -2240,24 +2333,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>135</v>
+        <v>213</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>136</v>
+        <v>212</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>135</v>
+        <v>213</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>136</v>
+        <v>212</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>6</v>
@@ -2266,173 +2359,168 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I47" s="3"/>
-    </row>
-    <row r="48" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I48" s="3"/>
-    </row>
-    <row r="49" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I49" s="3"/>
-    </row>
-    <row r="50" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I50" s="3"/>
-    </row>
-    <row r="51" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I51" s="3"/>
-    </row>
-    <row r="52" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>49</v>
@@ -2441,10 +2529,10 @@
         <v>50</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>6</v>
@@ -2455,48 +2543,49 @@
     </row>
     <row r="53" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>204</v>
+        <v>35</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>207</v>
+        <v>240</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>208</v>
+        <v>118</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>6</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="I53" s="3"/>
     </row>
     <row r="54" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>36</v>
+        <v>238</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>122</v>
+        <v>189</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>123</v>
+        <v>190</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>216</v>
+        <v>240</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>6</v>
@@ -2504,25 +2593,26 @@
       <c r="H54" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="I54" s="3"/>
     </row>
     <row r="55" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>6</v>
@@ -2530,25 +2620,26 @@
       <c r="H55" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I55" s="3"/>
+    </row>
+    <row r="56" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>40</v>
+        <v>237</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>41</v>
+        <v>236</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>42</v>
+        <v>187</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>43</v>
+        <v>188</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>6</v>
@@ -2556,25 +2647,26 @@
       <c r="H56" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I56" s="3"/>
+    </row>
+    <row r="57" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>82</v>
+        <v>189</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>83</v>
+        <v>190</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>6</v>
@@ -2582,25 +2674,26 @@
       <c r="H57" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="I57" s="3"/>
     </row>
     <row r="58" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>150</v>
+        <v>68</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>152</v>
+        <v>69</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>152</v>
+        <v>71</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>151</v>
+        <v>72</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>6</v>
@@ -2608,25 +2701,26 @@
       <c r="H58" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="I58" s="3"/>
     </row>
     <row r="59" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>150</v>
+        <v>251</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>152</v>
+        <v>253</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>153</v>
+        <v>254</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>152</v>
+        <v>252</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>153</v>
+        <v>255</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>6</v>
@@ -2634,25 +2728,26 @@
       <c r="H59" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="I59" s="3"/>
     </row>
     <row r="60" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>55</v>
+        <v>191</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>49</v>
+        <v>193</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>50</v>
+        <v>192</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>46</v>
+        <v>195</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>47</v>
+        <v>194</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>6</v>
@@ -2660,25 +2755,26 @@
       <c r="H60" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="I60" s="3"/>
     </row>
     <row r="61" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>79</v>
+        <v>206</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>80</v>
+        <v>205</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>79</v>
+        <v>206</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>80</v>
+        <v>205</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>6</v>
@@ -2686,25 +2782,26 @@
       <c r="H61" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="I61" s="3"/>
     </row>
     <row r="62" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>6</v>
@@ -2715,48 +2812,48 @@
     </row>
     <row r="63" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>231</v>
+        <v>196</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>233</v>
+        <v>197</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>232</v>
+        <v>198</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>234</v>
+        <v>199</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>81</v>
+        <v>36</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>140</v>
+        <v>208</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>141</v>
+        <v>207</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>6</v>
@@ -2767,154 +2864,407 @@
     </row>
     <row r="65" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B76" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C65" t="s">
-        <v>128</v>
-      </c>
-      <c r="D65" t="s">
-        <v>129</v>
-      </c>
-      <c r="E65" t="s">
-        <v>210</v>
-      </c>
-      <c r="F65" t="s">
-        <v>209</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H65" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-    </row>
-    <row r="67" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-    </row>
-    <row r="68" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="3"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
-      <c r="H69" s="3"/>
-    </row>
-    <row r="70" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-    </row>
-    <row r="71" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3"/>
-    </row>
-    <row r="72" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
-    </row>
-    <row r="73" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
-      <c r="H73" s="3"/>
-    </row>
-    <row r="74" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="75" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="76" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="77" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="78" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+      <c r="C76" t="s">
+        <v>123</v>
+      </c>
+      <c r="D76" t="s">
+        <v>124</v>
+      </c>
+      <c r="E76" t="s">
+        <v>202</v>
+      </c>
+      <c r="F76" t="s">
+        <v>201</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+    </row>
+    <row r="78" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+    </row>
     <row r="79" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="81" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B81" s="7"/>
-    </row>
-    <row r="82" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B82" s="7"/>
-    </row>
-    <row r="83" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B83" s="7"/>
-    </row>
-    <row r="84" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B84" s="7"/>
-    </row>
-    <row r="85" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B85" s="7"/>
-    </row>
-    <row r="86" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B86" s="7"/>
-    </row>
-    <row r="87" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B87" s="7"/>
-    </row>
-    <row r="88" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B88" s="7"/>
-    </row>
-    <row r="89" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B89" s="7"/>
-    </row>
-    <row r="90" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B90" s="7"/>
-    </row>
-    <row r="91" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B91" s="7"/>
-    </row>
-    <row r="92" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+    </row>
+    <row r="81" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+    </row>
+    <row r="82" spans="1:8" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+    </row>
+    <row r="83" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+    </row>
+    <row r="84" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+      <c r="H84" s="3"/>
+    </row>
+    <row r="85" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="86" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="87" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="88" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="89" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="90" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="91" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="92" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B92" s="7"/>
     </row>
-    <row r="93" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B93" s="7"/>
     </row>
-    <row r="94" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B94" s="7"/>
     </row>
-    <row r="95" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B95" s="7"/>
     </row>
-    <row r="96" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B96" s="7"/>
     </row>
     <row r="97" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
@@ -5697,6 +6047,39 @@
     </row>
     <row r="1023" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B1023" s="7"/>
+    </row>
+    <row r="1024" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1024" s="7"/>
+    </row>
+    <row r="1025" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1025" s="7"/>
+    </row>
+    <row r="1026" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1026" s="7"/>
+    </row>
+    <row r="1027" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1027" s="7"/>
+    </row>
+    <row r="1028" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1028" s="7"/>
+    </row>
+    <row r="1029" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1029" s="7"/>
+    </row>
+    <row r="1030" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1030" s="7"/>
+    </row>
+    <row r="1031" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1031" s="7"/>
+    </row>
+    <row r="1032" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1032" s="7"/>
+    </row>
+    <row r="1033" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1033" s="7"/>
+    </row>
+    <row r="1034" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1034" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5708,7 +6091,7 @@
           <x14:formula1>
             <xm:f>Class!$A$2:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>B81:B1023 B69:B73 J62:J63 R62:R63 Z62:Z63 AH62:AH63 AP62:AP63 AX62:AX63 BF62:BF63 BN62:BN63 BV62:BV63 CD62:CD63 CL62:CL63 CT62:CT63 DB62:DB63 DJ62:DJ63 DR62:DR63 DZ62:DZ63 EH62:EH63 EP62:EP63 EX62:EX63 FF62:FF63 FN62:FN63 FV62:FV63 GD62:GD63 GL62:GL63 GT62:GT63 HB62:HB63 HJ62:HJ63 HR62:HR63 HZ62:HZ63 IH62:IH63 IP62:IP63 IX62:IX63 JF62:JF63 JN62:JN63 JV62:JV63 KD62:KD63 KL62:KL63 KT62:KT63 LB62:LB63 LJ62:LJ63 LR62:LR63 LZ62:LZ63 MH62:MH63 MP62:MP63 MX62:MX63 NF62:NF63 NN62:NN63 NV62:NV63 OD62:OD63 OL62:OL63 OT62:OT63 PB62:PB63 PJ62:PJ63 PR62:PR63 PZ62:PZ63 QH62:QH63 QP62:QP63 QX62:QX63 RF62:RF63 RN62:RN63 RV62:RV63 SD62:SD63 SL62:SL63 ST62:ST63 TB62:TB63 TJ62:TJ63 TR62:TR63 TZ62:TZ63 UH62:UH63 UP62:UP63 UX62:UX63 VF62:VF63 VN62:VN63 VV62:VV63 WD62:WD63 WL62:WL63 WT62:WT63 XB62:XB63 XJ62:XJ63 XR62:XR63 XZ62:XZ63 YH62:YH63 YP62:YP63 YX62:YX63 ZF62:ZF63 ZN62:ZN63 ZV62:ZV63 AAD62:AAD63 AAL62:AAL63 AAT62:AAT63 ABB62:ABB63 ABJ62:ABJ63 ABR62:ABR63 ABZ62:ABZ63 ACH62:ACH63 ACP62:ACP63 ACX62:ACX63 ADF62:ADF63 ADN62:ADN63 ADV62:ADV63 AED62:AED63 AEL62:AEL63 AET62:AET63 AFB62:AFB63 AFJ62:AFJ63 AFR62:AFR63 AFZ62:AFZ63 AGH62:AGH63 AGP62:AGP63 AGX62:AGX63 AHF62:AHF63 AHN62:AHN63 AHV62:AHV63 AID62:AID63 AIL62:AIL63 AIT62:AIT63 AJB62:AJB63 AJJ62:AJJ63 AJR62:AJR63 AJZ62:AJZ63 AKH62:AKH63 AKP62:AKP63 AKX62:AKX63 ALF62:ALF63 ALN62:ALN63 ALV62:ALV63 AMD62:AMD63 AML62:AML63 AMT62:AMT63 ANB62:ANB63 ANJ62:ANJ63 ANR62:ANR63 ANZ62:ANZ63 AOH62:AOH63 AOP62:AOP63 AOX62:AOX63 APF62:APF63 APN62:APN63 APV62:APV63 AQD62:AQD63 AQL62:AQL63 AQT62:AQT63 ARB62:ARB63 ARJ62:ARJ63 ARR62:ARR63 ARZ62:ARZ63 ASH62:ASH63 ASP62:ASP63 ASX62:ASX63 ATF62:ATF63 ATN62:ATN63 ATV62:ATV63 AUD62:AUD63 AUL62:AUL63 AUT62:AUT63 AVB62:AVB63 AVJ62:AVJ63 AVR62:AVR63 AVZ62:AVZ63 AWH62:AWH63 AWP62:AWP63 AWX62:AWX63 AXF62:AXF63 AXN62:AXN63 AXV62:AXV63 AYD62:AYD63 AYL62:AYL63 AYT62:AYT63 AZB62:AZB63 AZJ62:AZJ63 AZR62:AZR63 AZZ62:AZZ63 BAH62:BAH63 BAP62:BAP63 BAX62:BAX63 BBF62:BBF63 BBN62:BBN63 BBV62:BBV63 BCD62:BCD63 BCL62:BCL63 BCT62:BCT63 BDB62:BDB63 BDJ62:BDJ63 BDR62:BDR63 BDZ62:BDZ63 BEH62:BEH63 BEP62:BEP63 BEX62:BEX63 BFF62:BFF63 BFN62:BFN63 BFV62:BFV63 BGD62:BGD63 BGL62:BGL63 BGT62:BGT63 BHB62:BHB63 BHJ62:BHJ63 BHR62:BHR63 BHZ62:BHZ63 BIH62:BIH63 BIP62:BIP63 BIX62:BIX63 BJF62:BJF63 BJN62:BJN63 BJV62:BJV63 BKD62:BKD63 BKL62:BKL63 BKT62:BKT63 BLB62:BLB63 BLJ62:BLJ63 BLR62:BLR63 BLZ62:BLZ63 BMH62:BMH63 BMP62:BMP63 BMX62:BMX63 BNF62:BNF63 BNN62:BNN63 BNV62:BNV63 BOD62:BOD63 BOL62:BOL63 BOT62:BOT63 BPB62:BPB63 BPJ62:BPJ63 BPR62:BPR63 BPZ62:BPZ63 BQH62:BQH63 BQP62:BQP63 BQX62:BQX63 BRF62:BRF63 BRN62:BRN63 BRV62:BRV63 BSD62:BSD63 BSL62:BSL63 BST62:BST63 BTB62:BTB63 BTJ62:BTJ63 BTR62:BTR63 BTZ62:BTZ63 BUH62:BUH63 BUP62:BUP63 BUX62:BUX63 BVF62:BVF63 BVN62:BVN63 BVV62:BVV63 BWD62:BWD63 BWL62:BWL63 BWT62:BWT63 BXB62:BXB63 BXJ62:BXJ63 BXR62:BXR63 BXZ62:BXZ63 BYH62:BYH63 BYP62:BYP63 BYX62:BYX63 BZF62:BZF63 BZN62:BZN63 BZV62:BZV63 CAD62:CAD63 CAL62:CAL63 CAT62:CAT63 CBB62:CBB63 CBJ62:CBJ63 CBR62:CBR63 CBZ62:CBZ63 CCH62:CCH63 CCP62:CCP63 CCX62:CCX63 CDF62:CDF63 CDN62:CDN63 CDV62:CDV63 CED62:CED63 CEL62:CEL63 CET62:CET63 CFB62:CFB63 CFJ62:CFJ63 CFR62:CFR63 CFZ62:CFZ63 CGH62:CGH63 CGP62:CGP63 CGX62:CGX63 CHF62:CHF63 CHN62:CHN63 CHV62:CHV63 CID62:CID63 CIL62:CIL63 CIT62:CIT63 CJB62:CJB63 CJJ62:CJJ63 CJR62:CJR63 CJZ62:CJZ63 CKH62:CKH63 CKP62:CKP63 CKX62:CKX63 CLF62:CLF63 CLN62:CLN63 CLV62:CLV63 CMD62:CMD63 CML62:CML63 CMT62:CMT63 CNB62:CNB63 CNJ62:CNJ63 CNR62:CNR63 CNZ62:CNZ63 COH62:COH63 COP62:COP63 COX62:COX63 CPF62:CPF63 CPN62:CPN63 CPV62:CPV63 CQD62:CQD63 CQL62:CQL63 CQT62:CQT63 CRB62:CRB63 CRJ62:CRJ63 CRR62:CRR63 CRZ62:CRZ63 CSH62:CSH63 CSP62:CSP63 CSX62:CSX63 CTF62:CTF63 CTN62:CTN63 CTV62:CTV63 CUD62:CUD63 CUL62:CUL63 CUT62:CUT63 CVB62:CVB63 CVJ62:CVJ63 CVR62:CVR63 CVZ62:CVZ63 CWH62:CWH63 CWP62:CWP63 CWX62:CWX63 CXF62:CXF63 CXN62:CXN63 CXV62:CXV63 CYD62:CYD63 CYL62:CYL63 CYT62:CYT63 CZB62:CZB63 CZJ62:CZJ63 CZR62:CZR63 CZZ62:CZZ63 DAH62:DAH63 DAP62:DAP63 DAX62:DAX63 DBF62:DBF63 DBN62:DBN63 DBV62:DBV63 DCD62:DCD63 DCL62:DCL63 DCT62:DCT63 DDB62:DDB63 DDJ62:DDJ63 DDR62:DDR63 DDZ62:DDZ63 DEH62:DEH63 DEP62:DEP63 DEX62:DEX63 DFF62:DFF63 DFN62:DFN63 DFV62:DFV63 DGD62:DGD63 DGL62:DGL63 DGT62:DGT63 DHB62:DHB63 DHJ62:DHJ63 DHR62:DHR63 DHZ62:DHZ63 DIH62:DIH63 DIP62:DIP63 DIX62:DIX63 DJF62:DJF63 DJN62:DJN63 DJV62:DJV63 DKD62:DKD63 DKL62:DKL63 DKT62:DKT63 DLB62:DLB63 DLJ62:DLJ63 DLR62:DLR63 DLZ62:DLZ63 DMH62:DMH63 DMP62:DMP63 DMX62:DMX63 DNF62:DNF63 DNN62:DNN63 DNV62:DNV63 DOD62:DOD63 DOL62:DOL63 DOT62:DOT63 DPB62:DPB63 DPJ62:DPJ63 DPR62:DPR63 DPZ62:DPZ63 DQH62:DQH63 DQP62:DQP63 DQX62:DQX63 DRF62:DRF63 DRN62:DRN63 DRV62:DRV63 DSD62:DSD63 DSL62:DSL63 DST62:DST63 DTB62:DTB63 DTJ62:DTJ63 DTR62:DTR63 DTZ62:DTZ63 DUH62:DUH63 DUP62:DUP63 DUX62:DUX63 DVF62:DVF63 DVN62:DVN63 DVV62:DVV63 DWD62:DWD63 DWL62:DWL63 DWT62:DWT63 DXB62:DXB63 DXJ62:DXJ63 DXR62:DXR63 DXZ62:DXZ63 DYH62:DYH63 DYP62:DYP63 DYX62:DYX63 DZF62:DZF63 DZN62:DZN63 DZV62:DZV63 EAD62:EAD63 EAL62:EAL63 EAT62:EAT63 EBB62:EBB63 EBJ62:EBJ63 EBR62:EBR63 EBZ62:EBZ63 ECH62:ECH63 ECP62:ECP63 ECX62:ECX63 EDF62:EDF63 EDN62:EDN63 EDV62:EDV63 EED62:EED63 EEL62:EEL63 EET62:EET63 EFB62:EFB63 EFJ62:EFJ63 EFR62:EFR63 EFZ62:EFZ63 EGH62:EGH63 EGP62:EGP63 EGX62:EGX63 EHF62:EHF63 EHN62:EHN63 EHV62:EHV63 EID62:EID63 EIL62:EIL63 EIT62:EIT63 EJB62:EJB63 EJJ62:EJJ63 EJR62:EJR63 EJZ62:EJZ63 EKH62:EKH63 EKP62:EKP63 EKX62:EKX63 ELF62:ELF63 ELN62:ELN63 ELV62:ELV63 EMD62:EMD63 EML62:EML63 EMT62:EMT63 ENB62:ENB63 ENJ62:ENJ63 ENR62:ENR63 ENZ62:ENZ63 EOH62:EOH63 EOP62:EOP63 EOX62:EOX63 EPF62:EPF63 EPN62:EPN63 EPV62:EPV63 EQD62:EQD63 EQL62:EQL63 EQT62:EQT63 ERB62:ERB63 ERJ62:ERJ63 ERR62:ERR63 ERZ62:ERZ63 ESH62:ESH63 ESP62:ESP63 ESX62:ESX63 ETF62:ETF63 ETN62:ETN63 ETV62:ETV63 EUD62:EUD63 EUL62:EUL63 EUT62:EUT63 EVB62:EVB63 EVJ62:EVJ63 EVR62:EVR63 EVZ62:EVZ63 EWH62:EWH63 EWP62:EWP63 EWX62:EWX63 EXF62:EXF63 EXN62:EXN63 EXV62:EXV63 EYD62:EYD63 EYL62:EYL63 EYT62:EYT63 EZB62:EZB63 EZJ62:EZJ63 EZR62:EZR63 EZZ62:EZZ63 FAH62:FAH63 FAP62:FAP63 FAX62:FAX63 FBF62:FBF63 FBN62:FBN63 FBV62:FBV63 FCD62:FCD63 FCL62:FCL63 FCT62:FCT63 FDB62:FDB63 FDJ62:FDJ63 FDR62:FDR63 FDZ62:FDZ63 FEH62:FEH63 FEP62:FEP63 FEX62:FEX63 FFF62:FFF63 FFN62:FFN63 FFV62:FFV63 FGD62:FGD63 FGL62:FGL63 FGT62:FGT63 FHB62:FHB63 FHJ62:FHJ63 FHR62:FHR63 FHZ62:FHZ63 FIH62:FIH63 FIP62:FIP63 FIX62:FIX63 FJF62:FJF63 FJN62:FJN63 FJV62:FJV63 FKD62:FKD63 FKL62:FKL63 FKT62:FKT63 FLB62:FLB63 FLJ62:FLJ63 FLR62:FLR63 FLZ62:FLZ63 FMH62:FMH63 FMP62:FMP63 FMX62:FMX63 FNF62:FNF63 FNN62:FNN63 FNV62:FNV63 FOD62:FOD63 FOL62:FOL63 FOT62:FOT63 FPB62:FPB63 FPJ62:FPJ63 FPR62:FPR63 FPZ62:FPZ63 FQH62:FQH63 FQP62:FQP63 FQX62:FQX63 FRF62:FRF63 FRN62:FRN63 FRV62:FRV63 FSD62:FSD63 FSL62:FSL63 FST62:FST63 FTB62:FTB63 FTJ62:FTJ63 FTR62:FTR63 FTZ62:FTZ63 FUH62:FUH63 FUP62:FUP63 FUX62:FUX63 FVF62:FVF63 FVN62:FVN63 FVV62:FVV63 FWD62:FWD63 FWL62:FWL63 FWT62:FWT63 FXB62:FXB63 FXJ62:FXJ63 FXR62:FXR63 FXZ62:FXZ63 FYH62:FYH63 FYP62:FYP63 FYX62:FYX63 FZF62:FZF63 FZN62:FZN63 FZV62:FZV63 GAD62:GAD63 GAL62:GAL63 GAT62:GAT63 GBB62:GBB63 GBJ62:GBJ63 GBR62:GBR63 GBZ62:GBZ63 GCH62:GCH63 GCP62:GCP63 GCX62:GCX63 GDF62:GDF63 GDN62:GDN63 GDV62:GDV63 GED62:GED63 GEL62:GEL63 GET62:GET63 GFB62:GFB63 GFJ62:GFJ63 GFR62:GFR63 GFZ62:GFZ63 GGH62:GGH63 GGP62:GGP63 GGX62:GGX63 GHF62:GHF63 GHN62:GHN63 GHV62:GHV63 GID62:GID63 GIL62:GIL63 GIT62:GIT63 GJB62:GJB63 GJJ62:GJJ63 GJR62:GJR63 GJZ62:GJZ63 GKH62:GKH63 GKP62:GKP63 GKX62:GKX63 GLF62:GLF63 GLN62:GLN63 GLV62:GLV63 GMD62:GMD63 GML62:GML63 GMT62:GMT63 GNB62:GNB63 GNJ62:GNJ63 GNR62:GNR63 GNZ62:GNZ63 GOH62:GOH63 GOP62:GOP63 GOX62:GOX63 GPF62:GPF63 GPN62:GPN63 GPV62:GPV63 GQD62:GQD63 GQL62:GQL63 GQT62:GQT63 GRB62:GRB63 GRJ62:GRJ63 GRR62:GRR63 GRZ62:GRZ63 GSH62:GSH63 GSP62:GSP63 GSX62:GSX63 GTF62:GTF63 GTN62:GTN63 GTV62:GTV63 GUD62:GUD63 GUL62:GUL63 GUT62:GUT63 GVB62:GVB63 GVJ62:GVJ63 GVR62:GVR63 GVZ62:GVZ63 GWH62:GWH63 GWP62:GWP63 GWX62:GWX63 GXF62:GXF63 GXN62:GXN63 GXV62:GXV63 GYD62:GYD63 GYL62:GYL63 GYT62:GYT63 GZB62:GZB63 GZJ62:GZJ63 GZR62:GZR63 GZZ62:GZZ63 HAH62:HAH63 HAP62:HAP63 HAX62:HAX63 HBF62:HBF63 HBN62:HBN63 HBV62:HBV63 HCD62:HCD63 HCL62:HCL63 HCT62:HCT63 HDB62:HDB63 HDJ62:HDJ63 HDR62:HDR63 HDZ62:HDZ63 HEH62:HEH63 HEP62:HEP63 HEX62:HEX63 HFF62:HFF63 HFN62:HFN63 HFV62:HFV63 HGD62:HGD63 HGL62:HGL63 HGT62:HGT63 HHB62:HHB63 HHJ62:HHJ63 HHR62:HHR63 HHZ62:HHZ63 HIH62:HIH63 HIP62:HIP63 HIX62:HIX63 HJF62:HJF63 HJN62:HJN63 HJV62:HJV63 HKD62:HKD63 HKL62:HKL63 HKT62:HKT63 HLB62:HLB63 HLJ62:HLJ63 HLR62:HLR63 HLZ62:HLZ63 HMH62:HMH63 HMP62:HMP63 HMX62:HMX63 HNF62:HNF63 HNN62:HNN63 HNV62:HNV63 HOD62:HOD63 HOL62:HOL63 HOT62:HOT63 HPB62:HPB63 HPJ62:HPJ63 HPR62:HPR63 HPZ62:HPZ63 HQH62:HQH63 HQP62:HQP63 HQX62:HQX63 HRF62:HRF63 HRN62:HRN63 HRV62:HRV63 HSD62:HSD63 HSL62:HSL63 HST62:HST63 HTB62:HTB63 HTJ62:HTJ63 HTR62:HTR63 HTZ62:HTZ63 HUH62:HUH63 HUP62:HUP63 HUX62:HUX63 HVF62:HVF63 HVN62:HVN63 HVV62:HVV63 HWD62:HWD63 HWL62:HWL63 HWT62:HWT63 HXB62:HXB63 HXJ62:HXJ63 HXR62:HXR63 HXZ62:HXZ63 HYH62:HYH63 HYP62:HYP63 HYX62:HYX63 HZF62:HZF63 HZN62:HZN63 HZV62:HZV63 IAD62:IAD63 IAL62:IAL63 IAT62:IAT63 IBB62:IBB63 IBJ62:IBJ63 IBR62:IBR63 IBZ62:IBZ63 ICH62:ICH63 ICP62:ICP63 ICX62:ICX63 IDF62:IDF63 IDN62:IDN63 IDV62:IDV63 IED62:IED63 IEL62:IEL63 IET62:IET63 IFB62:IFB63 IFJ62:IFJ63 IFR62:IFR63 IFZ62:IFZ63 IGH62:IGH63 IGP62:IGP63 IGX62:IGX63 IHF62:IHF63 IHN62:IHN63 IHV62:IHV63 IID62:IID63 IIL62:IIL63 IIT62:IIT63 IJB62:IJB63 IJJ62:IJJ63 IJR62:IJR63 IJZ62:IJZ63 IKH62:IKH63 IKP62:IKP63 IKX62:IKX63 ILF62:ILF63 ILN62:ILN63 ILV62:ILV63 IMD62:IMD63 IML62:IML63 IMT62:IMT63 INB62:INB63 INJ62:INJ63 INR62:INR63 INZ62:INZ63 IOH62:IOH63 IOP62:IOP63 IOX62:IOX63 IPF62:IPF63 IPN62:IPN63 IPV62:IPV63 IQD62:IQD63 IQL62:IQL63 IQT62:IQT63 IRB62:IRB63 IRJ62:IRJ63 IRR62:IRR63 IRZ62:IRZ63 ISH62:ISH63 ISP62:ISP63 ISX62:ISX63 ITF62:ITF63 ITN62:ITN63 ITV62:ITV63 IUD62:IUD63 IUL62:IUL63 IUT62:IUT63 IVB62:IVB63 IVJ62:IVJ63 IVR62:IVR63 IVZ62:IVZ63 IWH62:IWH63 IWP62:IWP63 IWX62:IWX63 IXF62:IXF63 IXN62:IXN63 IXV62:IXV63 IYD62:IYD63 IYL62:IYL63 IYT62:IYT63 IZB62:IZB63 IZJ62:IZJ63 IZR62:IZR63 IZZ62:IZZ63 JAH62:JAH63 JAP62:JAP63 JAX62:JAX63 JBF62:JBF63 JBN62:JBN63 JBV62:JBV63 JCD62:JCD63 JCL62:JCL63 JCT62:JCT63 JDB62:JDB63 JDJ62:JDJ63 JDR62:JDR63 JDZ62:JDZ63 JEH62:JEH63 JEP62:JEP63 JEX62:JEX63 JFF62:JFF63 JFN62:JFN63 JFV62:JFV63 JGD62:JGD63 JGL62:JGL63 JGT62:JGT63 JHB62:JHB63 JHJ62:JHJ63 JHR62:JHR63 JHZ62:JHZ63 JIH62:JIH63 JIP62:JIP63 JIX62:JIX63 JJF62:JJF63 JJN62:JJN63 JJV62:JJV63 JKD62:JKD63 JKL62:JKL63 JKT62:JKT63 JLB62:JLB63 JLJ62:JLJ63 JLR62:JLR63 JLZ62:JLZ63 JMH62:JMH63 JMP62:JMP63 JMX62:JMX63 JNF62:JNF63 JNN62:JNN63 JNV62:JNV63 JOD62:JOD63 JOL62:JOL63 JOT62:JOT63 JPB62:JPB63 JPJ62:JPJ63 JPR62:JPR63 JPZ62:JPZ63 JQH62:JQH63 JQP62:JQP63 JQX62:JQX63 JRF62:JRF63 JRN62:JRN63 JRV62:JRV63 JSD62:JSD63 JSL62:JSL63 JST62:JST63 JTB62:JTB63 JTJ62:JTJ63 JTR62:JTR63 JTZ62:JTZ63 JUH62:JUH63 JUP62:JUP63 JUX62:JUX63 JVF62:JVF63 JVN62:JVN63 JVV62:JVV63 JWD62:JWD63 JWL62:JWL63 JWT62:JWT63 JXB62:JXB63 JXJ62:JXJ63 JXR62:JXR63 JXZ62:JXZ63 JYH62:JYH63 JYP62:JYP63 JYX62:JYX63 JZF62:JZF63 JZN62:JZN63 JZV62:JZV63 KAD62:KAD63 KAL62:KAL63 KAT62:KAT63 KBB62:KBB63 KBJ62:KBJ63 KBR62:KBR63 KBZ62:KBZ63 KCH62:KCH63 KCP62:KCP63 KCX62:KCX63 KDF62:KDF63 KDN62:KDN63 KDV62:KDV63 KED62:KED63 KEL62:KEL63 KET62:KET63 KFB62:KFB63 KFJ62:KFJ63 KFR62:KFR63 KFZ62:KFZ63 KGH62:KGH63 KGP62:KGP63 KGX62:KGX63 KHF62:KHF63 KHN62:KHN63 KHV62:KHV63 KID62:KID63 KIL62:KIL63 KIT62:KIT63 KJB62:KJB63 KJJ62:KJJ63 KJR62:KJR63 KJZ62:KJZ63 KKH62:KKH63 KKP62:KKP63 KKX62:KKX63 KLF62:KLF63 KLN62:KLN63 KLV62:KLV63 KMD62:KMD63 KML62:KML63 KMT62:KMT63 KNB62:KNB63 KNJ62:KNJ63 KNR62:KNR63 KNZ62:KNZ63 KOH62:KOH63 KOP62:KOP63 KOX62:KOX63 KPF62:KPF63 KPN62:KPN63 KPV62:KPV63 KQD62:KQD63 KQL62:KQL63 KQT62:KQT63 KRB62:KRB63 KRJ62:KRJ63 KRR62:KRR63 KRZ62:KRZ63 KSH62:KSH63 KSP62:KSP63 KSX62:KSX63 KTF62:KTF63 KTN62:KTN63 KTV62:KTV63 KUD62:KUD63 KUL62:KUL63 KUT62:KUT63 KVB62:KVB63 KVJ62:KVJ63 KVR62:KVR63 KVZ62:KVZ63 KWH62:KWH63 KWP62:KWP63 KWX62:KWX63 KXF62:KXF63 KXN62:KXN63 KXV62:KXV63 KYD62:KYD63 KYL62:KYL63 KYT62:KYT63 KZB62:KZB63 KZJ62:KZJ63 KZR62:KZR63 KZZ62:KZZ63 LAH62:LAH63 LAP62:LAP63 LAX62:LAX63 LBF62:LBF63 LBN62:LBN63 LBV62:LBV63 LCD62:LCD63 LCL62:LCL63 LCT62:LCT63 LDB62:LDB63 LDJ62:LDJ63 LDR62:LDR63 LDZ62:LDZ63 LEH62:LEH63 LEP62:LEP63 LEX62:LEX63 LFF62:LFF63 LFN62:LFN63 LFV62:LFV63 LGD62:LGD63 LGL62:LGL63 LGT62:LGT63 LHB62:LHB63 LHJ62:LHJ63 LHR62:LHR63 LHZ62:LHZ63 LIH62:LIH63 LIP62:LIP63 LIX62:LIX63 LJF62:LJF63 LJN62:LJN63 LJV62:LJV63 LKD62:LKD63 LKL62:LKL63 LKT62:LKT63 LLB62:LLB63 LLJ62:LLJ63 LLR62:LLR63 LLZ62:LLZ63 LMH62:LMH63 LMP62:LMP63 LMX62:LMX63 LNF62:LNF63 LNN62:LNN63 LNV62:LNV63 LOD62:LOD63 LOL62:LOL63 LOT62:LOT63 LPB62:LPB63 LPJ62:LPJ63 LPR62:LPR63 LPZ62:LPZ63 LQH62:LQH63 LQP62:LQP63 LQX62:LQX63 LRF62:LRF63 LRN62:LRN63 LRV62:LRV63 LSD62:LSD63 LSL62:LSL63 LST62:LST63 LTB62:LTB63 LTJ62:LTJ63 LTR62:LTR63 LTZ62:LTZ63 LUH62:LUH63 LUP62:LUP63 LUX62:LUX63 LVF62:LVF63 LVN62:LVN63 LVV62:LVV63 LWD62:LWD63 LWL62:LWL63 LWT62:LWT63 LXB62:LXB63 LXJ62:LXJ63 LXR62:LXR63 LXZ62:LXZ63 LYH62:LYH63 LYP62:LYP63 LYX62:LYX63 LZF62:LZF63 LZN62:LZN63 LZV62:LZV63 MAD62:MAD63 MAL62:MAL63 MAT62:MAT63 MBB62:MBB63 MBJ62:MBJ63 MBR62:MBR63 MBZ62:MBZ63 MCH62:MCH63 MCP62:MCP63 MCX62:MCX63 MDF62:MDF63 MDN62:MDN63 MDV62:MDV63 MED62:MED63 MEL62:MEL63 MET62:MET63 MFB62:MFB63 MFJ62:MFJ63 MFR62:MFR63 MFZ62:MFZ63 MGH62:MGH63 MGP62:MGP63 MGX62:MGX63 MHF62:MHF63 MHN62:MHN63 MHV62:MHV63 MID62:MID63 MIL62:MIL63 MIT62:MIT63 MJB62:MJB63 MJJ62:MJJ63 MJR62:MJR63 MJZ62:MJZ63 MKH62:MKH63 MKP62:MKP63 MKX62:MKX63 MLF62:MLF63 MLN62:MLN63 MLV62:MLV63 MMD62:MMD63 MML62:MML63 MMT62:MMT63 MNB62:MNB63 MNJ62:MNJ63 MNR62:MNR63 MNZ62:MNZ63 MOH62:MOH63 MOP62:MOP63 MOX62:MOX63 MPF62:MPF63 MPN62:MPN63 MPV62:MPV63 MQD62:MQD63 MQL62:MQL63 MQT62:MQT63 MRB62:MRB63 MRJ62:MRJ63 MRR62:MRR63 MRZ62:MRZ63 MSH62:MSH63 MSP62:MSP63 MSX62:MSX63 MTF62:MTF63 MTN62:MTN63 MTV62:MTV63 MUD62:MUD63 MUL62:MUL63 MUT62:MUT63 MVB62:MVB63 MVJ62:MVJ63 MVR62:MVR63 MVZ62:MVZ63 MWH62:MWH63 MWP62:MWP63 MWX62:MWX63 MXF62:MXF63 MXN62:MXN63 MXV62:MXV63 MYD62:MYD63 MYL62:MYL63 MYT62:MYT63 MZB62:MZB63 MZJ62:MZJ63 MZR62:MZR63 MZZ62:MZZ63 NAH62:NAH63 NAP62:NAP63 NAX62:NAX63 NBF62:NBF63 NBN62:NBN63 NBV62:NBV63 NCD62:NCD63 NCL62:NCL63 NCT62:NCT63 NDB62:NDB63 NDJ62:NDJ63 NDR62:NDR63 NDZ62:NDZ63 NEH62:NEH63 NEP62:NEP63 NEX62:NEX63 NFF62:NFF63 NFN62:NFN63 NFV62:NFV63 NGD62:NGD63 NGL62:NGL63 NGT62:NGT63 NHB62:NHB63 NHJ62:NHJ63 NHR62:NHR63 NHZ62:NHZ63 NIH62:NIH63 NIP62:NIP63 NIX62:NIX63 NJF62:NJF63 NJN62:NJN63 NJV62:NJV63 NKD62:NKD63 NKL62:NKL63 NKT62:NKT63 NLB62:NLB63 NLJ62:NLJ63 NLR62:NLR63 NLZ62:NLZ63 NMH62:NMH63 NMP62:NMP63 NMX62:NMX63 NNF62:NNF63 NNN62:NNN63 NNV62:NNV63 NOD62:NOD63 NOL62:NOL63 NOT62:NOT63 NPB62:NPB63 NPJ62:NPJ63 NPR62:NPR63 NPZ62:NPZ63 NQH62:NQH63 NQP62:NQP63 NQX62:NQX63 NRF62:NRF63 NRN62:NRN63 NRV62:NRV63 NSD62:NSD63 NSL62:NSL63 NST62:NST63 NTB62:NTB63 NTJ62:NTJ63 NTR62:NTR63 NTZ62:NTZ63 NUH62:NUH63 NUP62:NUP63 NUX62:NUX63 NVF62:NVF63 NVN62:NVN63 NVV62:NVV63 NWD62:NWD63 NWL62:NWL63 NWT62:NWT63 NXB62:NXB63 NXJ62:NXJ63 NXR62:NXR63 NXZ62:NXZ63 NYH62:NYH63 NYP62:NYP63 NYX62:NYX63 NZF62:NZF63 NZN62:NZN63 NZV62:NZV63 OAD62:OAD63 OAL62:OAL63 OAT62:OAT63 OBB62:OBB63 OBJ62:OBJ63 OBR62:OBR63 OBZ62:OBZ63 OCH62:OCH63 OCP62:OCP63 OCX62:OCX63 ODF62:ODF63 ODN62:ODN63 ODV62:ODV63 OED62:OED63 OEL62:OEL63 OET62:OET63 OFB62:OFB63 OFJ62:OFJ63 OFR62:OFR63 OFZ62:OFZ63 OGH62:OGH63 OGP62:OGP63 OGX62:OGX63 OHF62:OHF63 OHN62:OHN63 OHV62:OHV63 OID62:OID63 OIL62:OIL63 OIT62:OIT63 OJB62:OJB63 OJJ62:OJJ63 OJR62:OJR63 OJZ62:OJZ63 OKH62:OKH63 OKP62:OKP63 OKX62:OKX63 OLF62:OLF63 OLN62:OLN63 OLV62:OLV63 OMD62:OMD63 OML62:OML63 OMT62:OMT63 ONB62:ONB63 ONJ62:ONJ63 ONR62:ONR63 ONZ62:ONZ63 OOH62:OOH63 OOP62:OOP63 OOX62:OOX63 OPF62:OPF63 OPN62:OPN63 OPV62:OPV63 OQD62:OQD63 OQL62:OQL63 OQT62:OQT63 ORB62:ORB63 ORJ62:ORJ63 ORR62:ORR63 ORZ62:ORZ63 OSH62:OSH63 OSP62:OSP63 OSX62:OSX63 OTF62:OTF63 OTN62:OTN63 OTV62:OTV63 OUD62:OUD63 OUL62:OUL63 OUT62:OUT63 OVB62:OVB63 OVJ62:OVJ63 OVR62:OVR63 OVZ62:OVZ63 OWH62:OWH63 OWP62:OWP63 OWX62:OWX63 OXF62:OXF63 OXN62:OXN63 OXV62:OXV63 OYD62:OYD63 OYL62:OYL63 OYT62:OYT63 OZB62:OZB63 OZJ62:OZJ63 OZR62:OZR63 OZZ62:OZZ63 PAH62:PAH63 PAP62:PAP63 PAX62:PAX63 PBF62:PBF63 PBN62:PBN63 PBV62:PBV63 PCD62:PCD63 PCL62:PCL63 PCT62:PCT63 PDB62:PDB63 PDJ62:PDJ63 PDR62:PDR63 PDZ62:PDZ63 PEH62:PEH63 PEP62:PEP63 PEX62:PEX63 PFF62:PFF63 PFN62:PFN63 PFV62:PFV63 PGD62:PGD63 PGL62:PGL63 PGT62:PGT63 PHB62:PHB63 PHJ62:PHJ63 PHR62:PHR63 PHZ62:PHZ63 PIH62:PIH63 PIP62:PIP63 PIX62:PIX63 PJF62:PJF63 PJN62:PJN63 PJV62:PJV63 PKD62:PKD63 PKL62:PKL63 PKT62:PKT63 PLB62:PLB63 PLJ62:PLJ63 PLR62:PLR63 PLZ62:PLZ63 PMH62:PMH63 PMP62:PMP63 PMX62:PMX63 PNF62:PNF63 PNN62:PNN63 PNV62:PNV63 POD62:POD63 POL62:POL63 POT62:POT63 PPB62:PPB63 PPJ62:PPJ63 PPR62:PPR63 PPZ62:PPZ63 PQH62:PQH63 PQP62:PQP63 PQX62:PQX63 PRF62:PRF63 PRN62:PRN63 PRV62:PRV63 PSD62:PSD63 PSL62:PSL63 PST62:PST63 PTB62:PTB63 PTJ62:PTJ63 PTR62:PTR63 PTZ62:PTZ63 PUH62:PUH63 PUP62:PUP63 PUX62:PUX63 PVF62:PVF63 PVN62:PVN63 PVV62:PVV63 PWD62:PWD63 PWL62:PWL63 PWT62:PWT63 PXB62:PXB63 PXJ62:PXJ63 PXR62:PXR63 PXZ62:PXZ63 PYH62:PYH63 PYP62:PYP63 PYX62:PYX63 PZF62:PZF63 PZN62:PZN63 PZV62:PZV63 QAD62:QAD63 QAL62:QAL63 QAT62:QAT63 QBB62:QBB63 QBJ62:QBJ63 QBR62:QBR63 QBZ62:QBZ63 QCH62:QCH63 QCP62:QCP63 QCX62:QCX63 QDF62:QDF63 QDN62:QDN63 QDV62:QDV63 QED62:QED63 QEL62:QEL63 QET62:QET63 QFB62:QFB63 QFJ62:QFJ63 QFR62:QFR63 QFZ62:QFZ63 QGH62:QGH63 QGP62:QGP63 QGX62:QGX63 QHF62:QHF63 QHN62:QHN63 QHV62:QHV63 QID62:QID63 QIL62:QIL63 QIT62:QIT63 QJB62:QJB63 QJJ62:QJJ63 QJR62:QJR63 QJZ62:QJZ63 QKH62:QKH63 QKP62:QKP63 QKX62:QKX63 QLF62:QLF63 QLN62:QLN63 QLV62:QLV63 QMD62:QMD63 QML62:QML63 QMT62:QMT63 QNB62:QNB63 QNJ62:QNJ63 QNR62:QNR63 QNZ62:QNZ63 QOH62:QOH63 QOP62:QOP63 QOX62:QOX63 QPF62:QPF63 QPN62:QPN63 QPV62:QPV63 QQD62:QQD63 QQL62:QQL63 QQT62:QQT63 QRB62:QRB63 QRJ62:QRJ63 QRR62:QRR63 QRZ62:QRZ63 QSH62:QSH63 QSP62:QSP63 QSX62:QSX63 QTF62:QTF63 QTN62:QTN63 QTV62:QTV63 QUD62:QUD63 QUL62:QUL63 QUT62:QUT63 QVB62:QVB63 QVJ62:QVJ63 QVR62:QVR63 QVZ62:QVZ63 QWH62:QWH63 QWP62:QWP63 QWX62:QWX63 QXF62:QXF63 QXN62:QXN63 QXV62:QXV63 QYD62:QYD63 QYL62:QYL63 QYT62:QYT63 QZB62:QZB63 QZJ62:QZJ63 QZR62:QZR63 QZZ62:QZZ63 RAH62:RAH63 RAP62:RAP63 RAX62:RAX63 RBF62:RBF63 RBN62:RBN63 RBV62:RBV63 RCD62:RCD63 RCL62:RCL63 RCT62:RCT63 RDB62:RDB63 RDJ62:RDJ63 RDR62:RDR63 RDZ62:RDZ63 REH62:REH63 REP62:REP63 REX62:REX63 RFF62:RFF63 RFN62:RFN63 RFV62:RFV63 RGD62:RGD63 RGL62:RGL63 RGT62:RGT63 RHB62:RHB63 RHJ62:RHJ63 RHR62:RHR63 RHZ62:RHZ63 RIH62:RIH63 RIP62:RIP63 RIX62:RIX63 RJF62:RJF63 RJN62:RJN63 RJV62:RJV63 RKD62:RKD63 RKL62:RKL63 RKT62:RKT63 RLB62:RLB63 RLJ62:RLJ63 RLR62:RLR63 RLZ62:RLZ63 RMH62:RMH63 RMP62:RMP63 RMX62:RMX63 RNF62:RNF63 RNN62:RNN63 RNV62:RNV63 ROD62:ROD63 ROL62:ROL63 ROT62:ROT63 RPB62:RPB63 RPJ62:RPJ63 RPR62:RPR63 RPZ62:RPZ63 RQH62:RQH63 RQP62:RQP63 RQX62:RQX63 RRF62:RRF63 RRN62:RRN63 RRV62:RRV63 RSD62:RSD63 RSL62:RSL63 RST62:RST63 RTB62:RTB63 RTJ62:RTJ63 RTR62:RTR63 RTZ62:RTZ63 RUH62:RUH63 RUP62:RUP63 RUX62:RUX63 RVF62:RVF63 RVN62:RVN63 RVV62:RVV63 RWD62:RWD63 RWL62:RWL63 RWT62:RWT63 RXB62:RXB63 RXJ62:RXJ63 RXR62:RXR63 RXZ62:RXZ63 RYH62:RYH63 RYP62:RYP63 RYX62:RYX63 RZF62:RZF63 RZN62:RZN63 RZV62:RZV63 SAD62:SAD63 SAL62:SAL63 SAT62:SAT63 SBB62:SBB63 SBJ62:SBJ63 SBR62:SBR63 SBZ62:SBZ63 SCH62:SCH63 SCP62:SCP63 SCX62:SCX63 SDF62:SDF63 SDN62:SDN63 SDV62:SDV63 SED62:SED63 SEL62:SEL63 SET62:SET63 SFB62:SFB63 SFJ62:SFJ63 SFR62:SFR63 SFZ62:SFZ63 SGH62:SGH63 SGP62:SGP63 SGX62:SGX63 SHF62:SHF63 SHN62:SHN63 SHV62:SHV63 SID62:SID63 SIL62:SIL63 SIT62:SIT63 SJB62:SJB63 SJJ62:SJJ63 SJR62:SJR63 SJZ62:SJZ63 SKH62:SKH63 SKP62:SKP63 SKX62:SKX63 SLF62:SLF63 SLN62:SLN63 SLV62:SLV63 SMD62:SMD63 SML62:SML63 SMT62:SMT63 SNB62:SNB63 SNJ62:SNJ63 SNR62:SNR63 SNZ62:SNZ63 SOH62:SOH63 SOP62:SOP63 SOX62:SOX63 SPF62:SPF63 SPN62:SPN63 SPV62:SPV63 SQD62:SQD63 SQL62:SQL63 SQT62:SQT63 SRB62:SRB63 SRJ62:SRJ63 SRR62:SRR63 SRZ62:SRZ63 SSH62:SSH63 SSP62:SSP63 SSX62:SSX63 STF62:STF63 STN62:STN63 STV62:STV63 SUD62:SUD63 SUL62:SUL63 SUT62:SUT63 SVB62:SVB63 SVJ62:SVJ63 SVR62:SVR63 SVZ62:SVZ63 SWH62:SWH63 SWP62:SWP63 SWX62:SWX63 SXF62:SXF63 SXN62:SXN63 SXV62:SXV63 SYD62:SYD63 SYL62:SYL63 SYT62:SYT63 SZB62:SZB63 SZJ62:SZJ63 SZR62:SZR63 SZZ62:SZZ63 TAH62:TAH63 TAP62:TAP63 TAX62:TAX63 TBF62:TBF63 TBN62:TBN63 TBV62:TBV63 TCD62:TCD63 TCL62:TCL63 TCT62:TCT63 TDB62:TDB63 TDJ62:TDJ63 TDR62:TDR63 TDZ62:TDZ63 TEH62:TEH63 TEP62:TEP63 TEX62:TEX63 TFF62:TFF63 TFN62:TFN63 TFV62:TFV63 TGD62:TGD63 TGL62:TGL63 TGT62:TGT63 THB62:THB63 THJ62:THJ63 THR62:THR63 THZ62:THZ63 TIH62:TIH63 TIP62:TIP63 TIX62:TIX63 TJF62:TJF63 TJN62:TJN63 TJV62:TJV63 TKD62:TKD63 TKL62:TKL63 TKT62:TKT63 TLB62:TLB63 TLJ62:TLJ63 TLR62:TLR63 TLZ62:TLZ63 TMH62:TMH63 TMP62:TMP63 TMX62:TMX63 TNF62:TNF63 TNN62:TNN63 TNV62:TNV63 TOD62:TOD63 TOL62:TOL63 TOT62:TOT63 TPB62:TPB63 TPJ62:TPJ63 TPR62:TPR63 TPZ62:TPZ63 TQH62:TQH63 TQP62:TQP63 TQX62:TQX63 TRF62:TRF63 TRN62:TRN63 TRV62:TRV63 TSD62:TSD63 TSL62:TSL63 TST62:TST63 TTB62:TTB63 TTJ62:TTJ63 TTR62:TTR63 TTZ62:TTZ63 TUH62:TUH63 TUP62:TUP63 TUX62:TUX63 TVF62:TVF63 TVN62:TVN63 TVV62:TVV63 TWD62:TWD63 TWL62:TWL63 TWT62:TWT63 TXB62:TXB63 TXJ62:TXJ63 TXR62:TXR63 TXZ62:TXZ63 TYH62:TYH63 TYP62:TYP63 TYX62:TYX63 TZF62:TZF63 TZN62:TZN63 TZV62:TZV63 UAD62:UAD63 UAL62:UAL63 UAT62:UAT63 UBB62:UBB63 UBJ62:UBJ63 UBR62:UBR63 UBZ62:UBZ63 UCH62:UCH63 UCP62:UCP63 UCX62:UCX63 UDF62:UDF63 UDN62:UDN63 UDV62:UDV63 UED62:UED63 UEL62:UEL63 UET62:UET63 UFB62:UFB63 UFJ62:UFJ63 UFR62:UFR63 UFZ62:UFZ63 UGH62:UGH63 UGP62:UGP63 UGX62:UGX63 UHF62:UHF63 UHN62:UHN63 UHV62:UHV63 UID62:UID63 UIL62:UIL63 UIT62:UIT63 UJB62:UJB63 UJJ62:UJJ63 UJR62:UJR63 UJZ62:UJZ63 UKH62:UKH63 UKP62:UKP63 UKX62:UKX63 ULF62:ULF63 ULN62:ULN63 ULV62:ULV63 UMD62:UMD63 UML62:UML63 UMT62:UMT63 UNB62:UNB63 UNJ62:UNJ63 UNR62:UNR63 UNZ62:UNZ63 UOH62:UOH63 UOP62:UOP63 UOX62:UOX63 UPF62:UPF63 UPN62:UPN63 UPV62:UPV63 UQD62:UQD63 UQL62:UQL63 UQT62:UQT63 URB62:URB63 URJ62:URJ63 URR62:URR63 URZ62:URZ63 USH62:USH63 USP62:USP63 USX62:USX63 UTF62:UTF63 UTN62:UTN63 UTV62:UTV63 UUD62:UUD63 UUL62:UUL63 UUT62:UUT63 UVB62:UVB63 UVJ62:UVJ63 UVR62:UVR63 UVZ62:UVZ63 UWH62:UWH63 UWP62:UWP63 UWX62:UWX63 UXF62:UXF63 UXN62:UXN63 UXV62:UXV63 UYD62:UYD63 UYL62:UYL63 UYT62:UYT63 UZB62:UZB63 UZJ62:UZJ63 UZR62:UZR63 UZZ62:UZZ63 VAH62:VAH63 VAP62:VAP63 VAX62:VAX63 VBF62:VBF63 VBN62:VBN63 VBV62:VBV63 VCD62:VCD63 VCL62:VCL63 VCT62:VCT63 VDB62:VDB63 VDJ62:VDJ63 VDR62:VDR63 VDZ62:VDZ63 VEH62:VEH63 VEP62:VEP63 VEX62:VEX63 VFF62:VFF63 VFN62:VFN63 VFV62:VFV63 VGD62:VGD63 VGL62:VGL63 VGT62:VGT63 VHB62:VHB63 VHJ62:VHJ63 VHR62:VHR63 VHZ62:VHZ63 VIH62:VIH63 VIP62:VIP63 VIX62:VIX63 VJF62:VJF63 VJN62:VJN63 VJV62:VJV63 VKD62:VKD63 VKL62:VKL63 VKT62:VKT63 VLB62:VLB63 VLJ62:VLJ63 VLR62:VLR63 VLZ62:VLZ63 VMH62:VMH63 VMP62:VMP63 VMX62:VMX63 VNF62:VNF63 VNN62:VNN63 VNV62:VNV63 VOD62:VOD63 VOL62:VOL63 VOT62:VOT63 VPB62:VPB63 VPJ62:VPJ63 VPR62:VPR63 VPZ62:VPZ63 VQH62:VQH63 VQP62:VQP63 VQX62:VQX63 VRF62:VRF63 VRN62:VRN63 VRV62:VRV63 VSD62:VSD63 VSL62:VSL63 VST62:VST63 VTB62:VTB63 VTJ62:VTJ63 VTR62:VTR63 VTZ62:VTZ63 VUH62:VUH63 VUP62:VUP63 VUX62:VUX63 VVF62:VVF63 VVN62:VVN63 VVV62:VVV63 VWD62:VWD63 VWL62:VWL63 VWT62:VWT63 VXB62:VXB63 VXJ62:VXJ63 VXR62:VXR63 VXZ62:VXZ63 VYH62:VYH63 VYP62:VYP63 VYX62:VYX63 VZF62:VZF63 VZN62:VZN63 VZV62:VZV63 WAD62:WAD63 WAL62:WAL63 WAT62:WAT63 WBB62:WBB63 WBJ62:WBJ63 WBR62:WBR63 WBZ62:WBZ63 WCH62:WCH63 WCP62:WCP63 WCX62:WCX63 WDF62:WDF63 WDN62:WDN63 WDV62:WDV63 WED62:WED63 WEL62:WEL63 WET62:WET63 WFB62:WFB63 WFJ62:WFJ63 WFR62:WFR63 WFZ62:WFZ63 WGH62:WGH63 WGP62:WGP63 WGX62:WGX63 WHF62:WHF63 WHN62:WHN63 WHV62:WHV63 WID62:WID63 WIL62:WIL63 WIT62:WIT63 WJB62:WJB63 WJJ62:WJJ63 WJR62:WJR63 WJZ62:WJZ63 WKH62:WKH63 WKP62:WKP63 WKX62:WKX63 WLF62:WLF63 WLN62:WLN63 WLV62:WLV63 WMD62:WMD63 WML62:WML63 WMT62:WMT63 WNB62:WNB63 WNJ62:WNJ63 WNR62:WNR63 WNZ62:WNZ63 WOH62:WOH63 WOP62:WOP63 WOX62:WOX63 WPF62:WPF63 WPN62:WPN63 WPV62:WPV63 WQD62:WQD63 WQL62:WQL63 WQT62:WQT63 WRB62:WRB63 WRJ62:WRJ63 WRR62:WRR63 WRZ62:WRZ63 WSH62:WSH63 WSP62:WSP63 WSX62:WSX63 WTF62:WTF63 WTN62:WTN63 WTV62:WTV63 WUD62:WUD63 WUL62:WUL63 WUT62:WUT63 WVB62:WVB63 WVJ62:WVJ63 WVR62:WVR63 WVZ62:WVZ63 WWH62:WWH63 WWP62:WWP63 WWX62:WWX63 WXF62:WXF63 WXN62:WXN63 WXV62:WXV63 WYD62:WYD63 WYL62:WYL63 WYT62:WYT63 WZB62:WZB63 WZJ62:WZJ63 WZR62:WZR63 WZZ62:WZZ63 XAH62:XAH63 XAP62:XAP63 XAX62:XAX63 XBF62:XBF63 XBN62:XBN63 XBV62:XBV63 XCD62:XCD63 XCL62:XCL63 XCT62:XCT63 XDB62:XDB63 XDJ62:XDJ63 XDR62:XDR63 XDZ62:XDZ63 XEH62:XEH63 XEP62:XEP63 XEX62:XEX63 B3:B67</xm:sqref>
+          <xm:sqref>B92:B1034 B80:B84 J72:J74 R72:R74 Z72:Z74 AH72:AH74 AP72:AP74 AX72:AX74 BF72:BF74 BN72:BN74 BV72:BV74 CD72:CD74 CL72:CL74 CT72:CT74 DB72:DB74 DJ72:DJ74 DR72:DR74 DZ72:DZ74 EH72:EH74 EP72:EP74 EX72:EX74 FF72:FF74 FN72:FN74 FV72:FV74 GD72:GD74 GL72:GL74 GT72:GT74 HB72:HB74 HJ72:HJ74 HR72:HR74 HZ72:HZ74 IH72:IH74 IP72:IP74 IX72:IX74 JF72:JF74 JN72:JN74 JV72:JV74 KD72:KD74 KL72:KL74 KT72:KT74 LB72:LB74 LJ72:LJ74 LR72:LR74 LZ72:LZ74 MH72:MH74 MP72:MP74 MX72:MX74 NF72:NF74 NN72:NN74 NV72:NV74 OD72:OD74 OL72:OL74 OT72:OT74 PB72:PB74 PJ72:PJ74 PR72:PR74 PZ72:PZ74 QH72:QH74 QP72:QP74 QX72:QX74 RF72:RF74 RN72:RN74 RV72:RV74 SD72:SD74 SL72:SL74 ST72:ST74 TB72:TB74 TJ72:TJ74 TR72:TR74 TZ72:TZ74 UH72:UH74 UP72:UP74 UX72:UX74 VF72:VF74 VN72:VN74 VV72:VV74 WD72:WD74 WL72:WL74 WT72:WT74 XB72:XB74 XJ72:XJ74 XR72:XR74 XZ72:XZ74 YH72:YH74 YP72:YP74 YX72:YX74 ZF72:ZF74 ZN72:ZN74 ZV72:ZV74 AAD72:AAD74 AAL72:AAL74 AAT72:AAT74 ABB72:ABB74 ABJ72:ABJ74 ABR72:ABR74 ABZ72:ABZ74 ACH72:ACH74 ACP72:ACP74 ACX72:ACX74 ADF72:ADF74 ADN72:ADN74 ADV72:ADV74 AED72:AED74 AEL72:AEL74 AET72:AET74 AFB72:AFB74 AFJ72:AFJ74 AFR72:AFR74 AFZ72:AFZ74 AGH72:AGH74 AGP72:AGP74 AGX72:AGX74 AHF72:AHF74 AHN72:AHN74 AHV72:AHV74 AID72:AID74 AIL72:AIL74 AIT72:AIT74 AJB72:AJB74 AJJ72:AJJ74 AJR72:AJR74 AJZ72:AJZ74 AKH72:AKH74 AKP72:AKP74 AKX72:AKX74 ALF72:ALF74 ALN72:ALN74 ALV72:ALV74 AMD72:AMD74 AML72:AML74 AMT72:AMT74 ANB72:ANB74 ANJ72:ANJ74 ANR72:ANR74 ANZ72:ANZ74 AOH72:AOH74 AOP72:AOP74 AOX72:AOX74 APF72:APF74 APN72:APN74 APV72:APV74 AQD72:AQD74 AQL72:AQL74 AQT72:AQT74 ARB72:ARB74 ARJ72:ARJ74 ARR72:ARR74 ARZ72:ARZ74 ASH72:ASH74 ASP72:ASP74 ASX72:ASX74 ATF72:ATF74 ATN72:ATN74 ATV72:ATV74 AUD72:AUD74 AUL72:AUL74 AUT72:AUT74 AVB72:AVB74 AVJ72:AVJ74 AVR72:AVR74 AVZ72:AVZ74 AWH72:AWH74 AWP72:AWP74 AWX72:AWX74 AXF72:AXF74 AXN72:AXN74 AXV72:AXV74 AYD72:AYD74 AYL72:AYL74 AYT72:AYT74 AZB72:AZB74 AZJ72:AZJ74 AZR72:AZR74 AZZ72:AZZ74 BAH72:BAH74 BAP72:BAP74 BAX72:BAX74 BBF72:BBF74 BBN72:BBN74 BBV72:BBV74 BCD72:BCD74 BCL72:BCL74 BCT72:BCT74 BDB72:BDB74 BDJ72:BDJ74 BDR72:BDR74 BDZ72:BDZ74 BEH72:BEH74 BEP72:BEP74 BEX72:BEX74 BFF72:BFF74 BFN72:BFN74 BFV72:BFV74 BGD72:BGD74 BGL72:BGL74 BGT72:BGT74 BHB72:BHB74 BHJ72:BHJ74 BHR72:BHR74 BHZ72:BHZ74 BIH72:BIH74 BIP72:BIP74 BIX72:BIX74 BJF72:BJF74 BJN72:BJN74 BJV72:BJV74 BKD72:BKD74 BKL72:BKL74 BKT72:BKT74 BLB72:BLB74 BLJ72:BLJ74 BLR72:BLR74 BLZ72:BLZ74 BMH72:BMH74 BMP72:BMP74 BMX72:BMX74 BNF72:BNF74 BNN72:BNN74 BNV72:BNV74 BOD72:BOD74 BOL72:BOL74 BOT72:BOT74 BPB72:BPB74 BPJ72:BPJ74 BPR72:BPR74 BPZ72:BPZ74 BQH72:BQH74 BQP72:BQP74 BQX72:BQX74 BRF72:BRF74 BRN72:BRN74 BRV72:BRV74 BSD72:BSD74 BSL72:BSL74 BST72:BST74 BTB72:BTB74 BTJ72:BTJ74 BTR72:BTR74 BTZ72:BTZ74 BUH72:BUH74 BUP72:BUP74 BUX72:BUX74 BVF72:BVF74 BVN72:BVN74 BVV72:BVV74 BWD72:BWD74 BWL72:BWL74 BWT72:BWT74 BXB72:BXB74 BXJ72:BXJ74 BXR72:BXR74 BXZ72:BXZ74 BYH72:BYH74 BYP72:BYP74 BYX72:BYX74 BZF72:BZF74 BZN72:BZN74 BZV72:BZV74 CAD72:CAD74 CAL72:CAL74 CAT72:CAT74 CBB72:CBB74 CBJ72:CBJ74 CBR72:CBR74 CBZ72:CBZ74 CCH72:CCH74 CCP72:CCP74 CCX72:CCX74 CDF72:CDF74 CDN72:CDN74 CDV72:CDV74 CED72:CED74 CEL72:CEL74 CET72:CET74 CFB72:CFB74 CFJ72:CFJ74 CFR72:CFR74 CFZ72:CFZ74 CGH72:CGH74 CGP72:CGP74 CGX72:CGX74 CHF72:CHF74 CHN72:CHN74 CHV72:CHV74 CID72:CID74 CIL72:CIL74 CIT72:CIT74 CJB72:CJB74 CJJ72:CJJ74 CJR72:CJR74 CJZ72:CJZ74 CKH72:CKH74 CKP72:CKP74 CKX72:CKX74 CLF72:CLF74 CLN72:CLN74 CLV72:CLV74 CMD72:CMD74 CML72:CML74 CMT72:CMT74 CNB72:CNB74 CNJ72:CNJ74 CNR72:CNR74 CNZ72:CNZ74 COH72:COH74 COP72:COP74 COX72:COX74 CPF72:CPF74 CPN72:CPN74 CPV72:CPV74 CQD72:CQD74 CQL72:CQL74 CQT72:CQT74 CRB72:CRB74 CRJ72:CRJ74 CRR72:CRR74 CRZ72:CRZ74 CSH72:CSH74 CSP72:CSP74 CSX72:CSX74 CTF72:CTF74 CTN72:CTN74 CTV72:CTV74 CUD72:CUD74 CUL72:CUL74 CUT72:CUT74 CVB72:CVB74 CVJ72:CVJ74 CVR72:CVR74 CVZ72:CVZ74 CWH72:CWH74 CWP72:CWP74 CWX72:CWX74 CXF72:CXF74 CXN72:CXN74 CXV72:CXV74 CYD72:CYD74 CYL72:CYL74 CYT72:CYT74 CZB72:CZB74 CZJ72:CZJ74 CZR72:CZR74 CZZ72:CZZ74 DAH72:DAH74 DAP72:DAP74 DAX72:DAX74 DBF72:DBF74 DBN72:DBN74 DBV72:DBV74 DCD72:DCD74 DCL72:DCL74 DCT72:DCT74 DDB72:DDB74 DDJ72:DDJ74 DDR72:DDR74 DDZ72:DDZ74 DEH72:DEH74 DEP72:DEP74 DEX72:DEX74 DFF72:DFF74 DFN72:DFN74 DFV72:DFV74 DGD72:DGD74 DGL72:DGL74 DGT72:DGT74 DHB72:DHB74 DHJ72:DHJ74 DHR72:DHR74 DHZ72:DHZ74 DIH72:DIH74 DIP72:DIP74 DIX72:DIX74 DJF72:DJF74 DJN72:DJN74 DJV72:DJV74 DKD72:DKD74 DKL72:DKL74 DKT72:DKT74 DLB72:DLB74 DLJ72:DLJ74 DLR72:DLR74 DLZ72:DLZ74 DMH72:DMH74 DMP72:DMP74 DMX72:DMX74 DNF72:DNF74 DNN72:DNN74 DNV72:DNV74 DOD72:DOD74 DOL72:DOL74 DOT72:DOT74 DPB72:DPB74 DPJ72:DPJ74 DPR72:DPR74 DPZ72:DPZ74 DQH72:DQH74 DQP72:DQP74 DQX72:DQX74 DRF72:DRF74 DRN72:DRN74 DRV72:DRV74 DSD72:DSD74 DSL72:DSL74 DST72:DST74 DTB72:DTB74 DTJ72:DTJ74 DTR72:DTR74 DTZ72:DTZ74 DUH72:DUH74 DUP72:DUP74 DUX72:DUX74 DVF72:DVF74 DVN72:DVN74 DVV72:DVV74 DWD72:DWD74 DWL72:DWL74 DWT72:DWT74 DXB72:DXB74 DXJ72:DXJ74 DXR72:DXR74 DXZ72:DXZ74 DYH72:DYH74 DYP72:DYP74 DYX72:DYX74 DZF72:DZF74 DZN72:DZN74 DZV72:DZV74 EAD72:EAD74 EAL72:EAL74 EAT72:EAT74 EBB72:EBB74 EBJ72:EBJ74 EBR72:EBR74 EBZ72:EBZ74 ECH72:ECH74 ECP72:ECP74 ECX72:ECX74 EDF72:EDF74 EDN72:EDN74 EDV72:EDV74 EED72:EED74 EEL72:EEL74 EET72:EET74 EFB72:EFB74 EFJ72:EFJ74 EFR72:EFR74 EFZ72:EFZ74 EGH72:EGH74 EGP72:EGP74 EGX72:EGX74 EHF72:EHF74 EHN72:EHN74 EHV72:EHV74 EID72:EID74 EIL72:EIL74 EIT72:EIT74 EJB72:EJB74 EJJ72:EJJ74 EJR72:EJR74 EJZ72:EJZ74 EKH72:EKH74 EKP72:EKP74 EKX72:EKX74 ELF72:ELF74 ELN72:ELN74 ELV72:ELV74 EMD72:EMD74 EML72:EML74 EMT72:EMT74 ENB72:ENB74 ENJ72:ENJ74 ENR72:ENR74 ENZ72:ENZ74 EOH72:EOH74 EOP72:EOP74 EOX72:EOX74 EPF72:EPF74 EPN72:EPN74 EPV72:EPV74 EQD72:EQD74 EQL72:EQL74 EQT72:EQT74 ERB72:ERB74 ERJ72:ERJ74 ERR72:ERR74 ERZ72:ERZ74 ESH72:ESH74 ESP72:ESP74 ESX72:ESX74 ETF72:ETF74 ETN72:ETN74 ETV72:ETV74 EUD72:EUD74 EUL72:EUL74 EUT72:EUT74 EVB72:EVB74 EVJ72:EVJ74 EVR72:EVR74 EVZ72:EVZ74 EWH72:EWH74 EWP72:EWP74 EWX72:EWX74 EXF72:EXF74 EXN72:EXN74 EXV72:EXV74 EYD72:EYD74 EYL72:EYL74 EYT72:EYT74 EZB72:EZB74 EZJ72:EZJ74 EZR72:EZR74 EZZ72:EZZ74 FAH72:FAH74 FAP72:FAP74 FAX72:FAX74 FBF72:FBF74 FBN72:FBN74 FBV72:FBV74 FCD72:FCD74 FCL72:FCL74 FCT72:FCT74 FDB72:FDB74 FDJ72:FDJ74 FDR72:FDR74 FDZ72:FDZ74 FEH72:FEH74 FEP72:FEP74 FEX72:FEX74 FFF72:FFF74 FFN72:FFN74 FFV72:FFV74 FGD72:FGD74 FGL72:FGL74 FGT72:FGT74 FHB72:FHB74 FHJ72:FHJ74 FHR72:FHR74 FHZ72:FHZ74 FIH72:FIH74 FIP72:FIP74 FIX72:FIX74 FJF72:FJF74 FJN72:FJN74 FJV72:FJV74 FKD72:FKD74 FKL72:FKL74 FKT72:FKT74 FLB72:FLB74 FLJ72:FLJ74 FLR72:FLR74 FLZ72:FLZ74 FMH72:FMH74 FMP72:FMP74 FMX72:FMX74 FNF72:FNF74 FNN72:FNN74 FNV72:FNV74 FOD72:FOD74 FOL72:FOL74 FOT72:FOT74 FPB72:FPB74 FPJ72:FPJ74 FPR72:FPR74 FPZ72:FPZ74 FQH72:FQH74 FQP72:FQP74 FQX72:FQX74 FRF72:FRF74 FRN72:FRN74 FRV72:FRV74 FSD72:FSD74 FSL72:FSL74 FST72:FST74 FTB72:FTB74 FTJ72:FTJ74 FTR72:FTR74 FTZ72:FTZ74 FUH72:FUH74 FUP72:FUP74 FUX72:FUX74 FVF72:FVF74 FVN72:FVN74 FVV72:FVV74 FWD72:FWD74 FWL72:FWL74 FWT72:FWT74 FXB72:FXB74 FXJ72:FXJ74 FXR72:FXR74 FXZ72:FXZ74 FYH72:FYH74 FYP72:FYP74 FYX72:FYX74 FZF72:FZF74 FZN72:FZN74 FZV72:FZV74 GAD72:GAD74 GAL72:GAL74 GAT72:GAT74 GBB72:GBB74 GBJ72:GBJ74 GBR72:GBR74 GBZ72:GBZ74 GCH72:GCH74 GCP72:GCP74 GCX72:GCX74 GDF72:GDF74 GDN72:GDN74 GDV72:GDV74 GED72:GED74 GEL72:GEL74 GET72:GET74 GFB72:GFB74 GFJ72:GFJ74 GFR72:GFR74 GFZ72:GFZ74 GGH72:GGH74 GGP72:GGP74 GGX72:GGX74 GHF72:GHF74 GHN72:GHN74 GHV72:GHV74 GID72:GID74 GIL72:GIL74 GIT72:GIT74 GJB72:GJB74 GJJ72:GJJ74 GJR72:GJR74 GJZ72:GJZ74 GKH72:GKH74 GKP72:GKP74 GKX72:GKX74 GLF72:GLF74 GLN72:GLN74 GLV72:GLV74 GMD72:GMD74 GML72:GML74 GMT72:GMT74 GNB72:GNB74 GNJ72:GNJ74 GNR72:GNR74 GNZ72:GNZ74 GOH72:GOH74 GOP72:GOP74 GOX72:GOX74 GPF72:GPF74 GPN72:GPN74 GPV72:GPV74 GQD72:GQD74 GQL72:GQL74 GQT72:GQT74 GRB72:GRB74 GRJ72:GRJ74 GRR72:GRR74 GRZ72:GRZ74 GSH72:GSH74 GSP72:GSP74 GSX72:GSX74 GTF72:GTF74 GTN72:GTN74 GTV72:GTV74 GUD72:GUD74 GUL72:GUL74 GUT72:GUT74 GVB72:GVB74 GVJ72:GVJ74 GVR72:GVR74 GVZ72:GVZ74 GWH72:GWH74 GWP72:GWP74 GWX72:GWX74 GXF72:GXF74 GXN72:GXN74 GXV72:GXV74 GYD72:GYD74 GYL72:GYL74 GYT72:GYT74 GZB72:GZB74 GZJ72:GZJ74 GZR72:GZR74 GZZ72:GZZ74 HAH72:HAH74 HAP72:HAP74 HAX72:HAX74 HBF72:HBF74 HBN72:HBN74 HBV72:HBV74 HCD72:HCD74 HCL72:HCL74 HCT72:HCT74 HDB72:HDB74 HDJ72:HDJ74 HDR72:HDR74 HDZ72:HDZ74 HEH72:HEH74 HEP72:HEP74 HEX72:HEX74 HFF72:HFF74 HFN72:HFN74 HFV72:HFV74 HGD72:HGD74 HGL72:HGL74 HGT72:HGT74 HHB72:HHB74 HHJ72:HHJ74 HHR72:HHR74 HHZ72:HHZ74 HIH72:HIH74 HIP72:HIP74 HIX72:HIX74 HJF72:HJF74 HJN72:HJN74 HJV72:HJV74 HKD72:HKD74 HKL72:HKL74 HKT72:HKT74 HLB72:HLB74 HLJ72:HLJ74 HLR72:HLR74 HLZ72:HLZ74 HMH72:HMH74 HMP72:HMP74 HMX72:HMX74 HNF72:HNF74 HNN72:HNN74 HNV72:HNV74 HOD72:HOD74 HOL72:HOL74 HOT72:HOT74 HPB72:HPB74 HPJ72:HPJ74 HPR72:HPR74 HPZ72:HPZ74 HQH72:HQH74 HQP72:HQP74 HQX72:HQX74 HRF72:HRF74 HRN72:HRN74 HRV72:HRV74 HSD72:HSD74 HSL72:HSL74 HST72:HST74 HTB72:HTB74 HTJ72:HTJ74 HTR72:HTR74 HTZ72:HTZ74 HUH72:HUH74 HUP72:HUP74 HUX72:HUX74 HVF72:HVF74 HVN72:HVN74 HVV72:HVV74 HWD72:HWD74 HWL72:HWL74 HWT72:HWT74 HXB72:HXB74 HXJ72:HXJ74 HXR72:HXR74 HXZ72:HXZ74 HYH72:HYH74 HYP72:HYP74 HYX72:HYX74 HZF72:HZF74 HZN72:HZN74 HZV72:HZV74 IAD72:IAD74 IAL72:IAL74 IAT72:IAT74 IBB72:IBB74 IBJ72:IBJ74 IBR72:IBR74 IBZ72:IBZ74 ICH72:ICH74 ICP72:ICP74 ICX72:ICX74 IDF72:IDF74 IDN72:IDN74 IDV72:IDV74 IED72:IED74 IEL72:IEL74 IET72:IET74 IFB72:IFB74 IFJ72:IFJ74 IFR72:IFR74 IFZ72:IFZ74 IGH72:IGH74 IGP72:IGP74 IGX72:IGX74 IHF72:IHF74 IHN72:IHN74 IHV72:IHV74 IID72:IID74 IIL72:IIL74 IIT72:IIT74 IJB72:IJB74 IJJ72:IJJ74 IJR72:IJR74 IJZ72:IJZ74 IKH72:IKH74 IKP72:IKP74 IKX72:IKX74 ILF72:ILF74 ILN72:ILN74 ILV72:ILV74 IMD72:IMD74 IML72:IML74 IMT72:IMT74 INB72:INB74 INJ72:INJ74 INR72:INR74 INZ72:INZ74 IOH72:IOH74 IOP72:IOP74 IOX72:IOX74 IPF72:IPF74 IPN72:IPN74 IPV72:IPV74 IQD72:IQD74 IQL72:IQL74 IQT72:IQT74 IRB72:IRB74 IRJ72:IRJ74 IRR72:IRR74 IRZ72:IRZ74 ISH72:ISH74 ISP72:ISP74 ISX72:ISX74 ITF72:ITF74 ITN72:ITN74 ITV72:ITV74 IUD72:IUD74 IUL72:IUL74 IUT72:IUT74 IVB72:IVB74 IVJ72:IVJ74 IVR72:IVR74 IVZ72:IVZ74 IWH72:IWH74 IWP72:IWP74 IWX72:IWX74 IXF72:IXF74 IXN72:IXN74 IXV72:IXV74 IYD72:IYD74 IYL72:IYL74 IYT72:IYT74 IZB72:IZB74 IZJ72:IZJ74 IZR72:IZR74 IZZ72:IZZ74 JAH72:JAH74 JAP72:JAP74 JAX72:JAX74 JBF72:JBF74 JBN72:JBN74 JBV72:JBV74 JCD72:JCD74 JCL72:JCL74 JCT72:JCT74 JDB72:JDB74 JDJ72:JDJ74 JDR72:JDR74 JDZ72:JDZ74 JEH72:JEH74 JEP72:JEP74 JEX72:JEX74 JFF72:JFF74 JFN72:JFN74 JFV72:JFV74 JGD72:JGD74 JGL72:JGL74 JGT72:JGT74 JHB72:JHB74 JHJ72:JHJ74 JHR72:JHR74 JHZ72:JHZ74 JIH72:JIH74 JIP72:JIP74 JIX72:JIX74 JJF72:JJF74 JJN72:JJN74 JJV72:JJV74 JKD72:JKD74 JKL72:JKL74 JKT72:JKT74 JLB72:JLB74 JLJ72:JLJ74 JLR72:JLR74 JLZ72:JLZ74 JMH72:JMH74 JMP72:JMP74 JMX72:JMX74 JNF72:JNF74 JNN72:JNN74 JNV72:JNV74 JOD72:JOD74 JOL72:JOL74 JOT72:JOT74 JPB72:JPB74 JPJ72:JPJ74 JPR72:JPR74 JPZ72:JPZ74 JQH72:JQH74 JQP72:JQP74 JQX72:JQX74 JRF72:JRF74 JRN72:JRN74 JRV72:JRV74 JSD72:JSD74 JSL72:JSL74 JST72:JST74 JTB72:JTB74 JTJ72:JTJ74 JTR72:JTR74 JTZ72:JTZ74 JUH72:JUH74 JUP72:JUP74 JUX72:JUX74 JVF72:JVF74 JVN72:JVN74 JVV72:JVV74 JWD72:JWD74 JWL72:JWL74 JWT72:JWT74 JXB72:JXB74 JXJ72:JXJ74 JXR72:JXR74 JXZ72:JXZ74 JYH72:JYH74 JYP72:JYP74 JYX72:JYX74 JZF72:JZF74 JZN72:JZN74 JZV72:JZV74 KAD72:KAD74 KAL72:KAL74 KAT72:KAT74 KBB72:KBB74 KBJ72:KBJ74 KBR72:KBR74 KBZ72:KBZ74 KCH72:KCH74 KCP72:KCP74 KCX72:KCX74 KDF72:KDF74 KDN72:KDN74 KDV72:KDV74 KED72:KED74 KEL72:KEL74 KET72:KET74 KFB72:KFB74 KFJ72:KFJ74 KFR72:KFR74 KFZ72:KFZ74 KGH72:KGH74 KGP72:KGP74 KGX72:KGX74 KHF72:KHF74 KHN72:KHN74 KHV72:KHV74 KID72:KID74 KIL72:KIL74 KIT72:KIT74 KJB72:KJB74 KJJ72:KJJ74 KJR72:KJR74 KJZ72:KJZ74 KKH72:KKH74 KKP72:KKP74 KKX72:KKX74 KLF72:KLF74 KLN72:KLN74 KLV72:KLV74 KMD72:KMD74 KML72:KML74 KMT72:KMT74 KNB72:KNB74 KNJ72:KNJ74 KNR72:KNR74 KNZ72:KNZ74 KOH72:KOH74 KOP72:KOP74 KOX72:KOX74 KPF72:KPF74 KPN72:KPN74 KPV72:KPV74 KQD72:KQD74 KQL72:KQL74 KQT72:KQT74 KRB72:KRB74 KRJ72:KRJ74 KRR72:KRR74 KRZ72:KRZ74 KSH72:KSH74 KSP72:KSP74 KSX72:KSX74 KTF72:KTF74 KTN72:KTN74 KTV72:KTV74 KUD72:KUD74 KUL72:KUL74 KUT72:KUT74 KVB72:KVB74 KVJ72:KVJ74 KVR72:KVR74 KVZ72:KVZ74 KWH72:KWH74 KWP72:KWP74 KWX72:KWX74 KXF72:KXF74 KXN72:KXN74 KXV72:KXV74 KYD72:KYD74 KYL72:KYL74 KYT72:KYT74 KZB72:KZB74 KZJ72:KZJ74 KZR72:KZR74 KZZ72:KZZ74 LAH72:LAH74 LAP72:LAP74 LAX72:LAX74 LBF72:LBF74 LBN72:LBN74 LBV72:LBV74 LCD72:LCD74 LCL72:LCL74 LCT72:LCT74 LDB72:LDB74 LDJ72:LDJ74 LDR72:LDR74 LDZ72:LDZ74 LEH72:LEH74 LEP72:LEP74 LEX72:LEX74 LFF72:LFF74 LFN72:LFN74 LFV72:LFV74 LGD72:LGD74 LGL72:LGL74 LGT72:LGT74 LHB72:LHB74 LHJ72:LHJ74 LHR72:LHR74 LHZ72:LHZ74 LIH72:LIH74 LIP72:LIP74 LIX72:LIX74 LJF72:LJF74 LJN72:LJN74 LJV72:LJV74 LKD72:LKD74 LKL72:LKL74 LKT72:LKT74 LLB72:LLB74 LLJ72:LLJ74 LLR72:LLR74 LLZ72:LLZ74 LMH72:LMH74 LMP72:LMP74 LMX72:LMX74 LNF72:LNF74 LNN72:LNN74 LNV72:LNV74 LOD72:LOD74 LOL72:LOL74 LOT72:LOT74 LPB72:LPB74 LPJ72:LPJ74 LPR72:LPR74 LPZ72:LPZ74 LQH72:LQH74 LQP72:LQP74 LQX72:LQX74 LRF72:LRF74 LRN72:LRN74 LRV72:LRV74 LSD72:LSD74 LSL72:LSL74 LST72:LST74 LTB72:LTB74 LTJ72:LTJ74 LTR72:LTR74 LTZ72:LTZ74 LUH72:LUH74 LUP72:LUP74 LUX72:LUX74 LVF72:LVF74 LVN72:LVN74 LVV72:LVV74 LWD72:LWD74 LWL72:LWL74 LWT72:LWT74 LXB72:LXB74 LXJ72:LXJ74 LXR72:LXR74 LXZ72:LXZ74 LYH72:LYH74 LYP72:LYP74 LYX72:LYX74 LZF72:LZF74 LZN72:LZN74 LZV72:LZV74 MAD72:MAD74 MAL72:MAL74 MAT72:MAT74 MBB72:MBB74 MBJ72:MBJ74 MBR72:MBR74 MBZ72:MBZ74 MCH72:MCH74 MCP72:MCP74 MCX72:MCX74 MDF72:MDF74 MDN72:MDN74 MDV72:MDV74 MED72:MED74 MEL72:MEL74 MET72:MET74 MFB72:MFB74 MFJ72:MFJ74 MFR72:MFR74 MFZ72:MFZ74 MGH72:MGH74 MGP72:MGP74 MGX72:MGX74 MHF72:MHF74 MHN72:MHN74 MHV72:MHV74 MID72:MID74 MIL72:MIL74 MIT72:MIT74 MJB72:MJB74 MJJ72:MJJ74 MJR72:MJR74 MJZ72:MJZ74 MKH72:MKH74 MKP72:MKP74 MKX72:MKX74 MLF72:MLF74 MLN72:MLN74 MLV72:MLV74 MMD72:MMD74 MML72:MML74 MMT72:MMT74 MNB72:MNB74 MNJ72:MNJ74 MNR72:MNR74 MNZ72:MNZ74 MOH72:MOH74 MOP72:MOP74 MOX72:MOX74 MPF72:MPF74 MPN72:MPN74 MPV72:MPV74 MQD72:MQD74 MQL72:MQL74 MQT72:MQT74 MRB72:MRB74 MRJ72:MRJ74 MRR72:MRR74 MRZ72:MRZ74 MSH72:MSH74 MSP72:MSP74 MSX72:MSX74 MTF72:MTF74 MTN72:MTN74 MTV72:MTV74 MUD72:MUD74 MUL72:MUL74 MUT72:MUT74 MVB72:MVB74 MVJ72:MVJ74 MVR72:MVR74 MVZ72:MVZ74 MWH72:MWH74 MWP72:MWP74 MWX72:MWX74 MXF72:MXF74 MXN72:MXN74 MXV72:MXV74 MYD72:MYD74 MYL72:MYL74 MYT72:MYT74 MZB72:MZB74 MZJ72:MZJ74 MZR72:MZR74 MZZ72:MZZ74 NAH72:NAH74 NAP72:NAP74 NAX72:NAX74 NBF72:NBF74 NBN72:NBN74 NBV72:NBV74 NCD72:NCD74 NCL72:NCL74 NCT72:NCT74 NDB72:NDB74 NDJ72:NDJ74 NDR72:NDR74 NDZ72:NDZ74 NEH72:NEH74 NEP72:NEP74 NEX72:NEX74 NFF72:NFF74 NFN72:NFN74 NFV72:NFV74 NGD72:NGD74 NGL72:NGL74 NGT72:NGT74 NHB72:NHB74 NHJ72:NHJ74 NHR72:NHR74 NHZ72:NHZ74 NIH72:NIH74 NIP72:NIP74 NIX72:NIX74 NJF72:NJF74 NJN72:NJN74 NJV72:NJV74 NKD72:NKD74 NKL72:NKL74 NKT72:NKT74 NLB72:NLB74 NLJ72:NLJ74 NLR72:NLR74 NLZ72:NLZ74 NMH72:NMH74 NMP72:NMP74 NMX72:NMX74 NNF72:NNF74 NNN72:NNN74 NNV72:NNV74 NOD72:NOD74 NOL72:NOL74 NOT72:NOT74 NPB72:NPB74 NPJ72:NPJ74 NPR72:NPR74 NPZ72:NPZ74 NQH72:NQH74 NQP72:NQP74 NQX72:NQX74 NRF72:NRF74 NRN72:NRN74 NRV72:NRV74 NSD72:NSD74 NSL72:NSL74 NST72:NST74 NTB72:NTB74 NTJ72:NTJ74 NTR72:NTR74 NTZ72:NTZ74 NUH72:NUH74 NUP72:NUP74 NUX72:NUX74 NVF72:NVF74 NVN72:NVN74 NVV72:NVV74 NWD72:NWD74 NWL72:NWL74 NWT72:NWT74 NXB72:NXB74 NXJ72:NXJ74 NXR72:NXR74 NXZ72:NXZ74 NYH72:NYH74 NYP72:NYP74 NYX72:NYX74 NZF72:NZF74 NZN72:NZN74 NZV72:NZV74 OAD72:OAD74 OAL72:OAL74 OAT72:OAT74 OBB72:OBB74 OBJ72:OBJ74 OBR72:OBR74 OBZ72:OBZ74 OCH72:OCH74 OCP72:OCP74 OCX72:OCX74 ODF72:ODF74 ODN72:ODN74 ODV72:ODV74 OED72:OED74 OEL72:OEL74 OET72:OET74 OFB72:OFB74 OFJ72:OFJ74 OFR72:OFR74 OFZ72:OFZ74 OGH72:OGH74 OGP72:OGP74 OGX72:OGX74 OHF72:OHF74 OHN72:OHN74 OHV72:OHV74 OID72:OID74 OIL72:OIL74 OIT72:OIT74 OJB72:OJB74 OJJ72:OJJ74 OJR72:OJR74 OJZ72:OJZ74 OKH72:OKH74 OKP72:OKP74 OKX72:OKX74 OLF72:OLF74 OLN72:OLN74 OLV72:OLV74 OMD72:OMD74 OML72:OML74 OMT72:OMT74 ONB72:ONB74 ONJ72:ONJ74 ONR72:ONR74 ONZ72:ONZ74 OOH72:OOH74 OOP72:OOP74 OOX72:OOX74 OPF72:OPF74 OPN72:OPN74 OPV72:OPV74 OQD72:OQD74 OQL72:OQL74 OQT72:OQT74 ORB72:ORB74 ORJ72:ORJ74 ORR72:ORR74 ORZ72:ORZ74 OSH72:OSH74 OSP72:OSP74 OSX72:OSX74 OTF72:OTF74 OTN72:OTN74 OTV72:OTV74 OUD72:OUD74 OUL72:OUL74 OUT72:OUT74 OVB72:OVB74 OVJ72:OVJ74 OVR72:OVR74 OVZ72:OVZ74 OWH72:OWH74 OWP72:OWP74 OWX72:OWX74 OXF72:OXF74 OXN72:OXN74 OXV72:OXV74 OYD72:OYD74 OYL72:OYL74 OYT72:OYT74 OZB72:OZB74 OZJ72:OZJ74 OZR72:OZR74 OZZ72:OZZ74 PAH72:PAH74 PAP72:PAP74 PAX72:PAX74 PBF72:PBF74 PBN72:PBN74 PBV72:PBV74 PCD72:PCD74 PCL72:PCL74 PCT72:PCT74 PDB72:PDB74 PDJ72:PDJ74 PDR72:PDR74 PDZ72:PDZ74 PEH72:PEH74 PEP72:PEP74 PEX72:PEX74 PFF72:PFF74 PFN72:PFN74 PFV72:PFV74 PGD72:PGD74 PGL72:PGL74 PGT72:PGT74 PHB72:PHB74 PHJ72:PHJ74 PHR72:PHR74 PHZ72:PHZ74 PIH72:PIH74 PIP72:PIP74 PIX72:PIX74 PJF72:PJF74 PJN72:PJN74 PJV72:PJV74 PKD72:PKD74 PKL72:PKL74 PKT72:PKT74 PLB72:PLB74 PLJ72:PLJ74 PLR72:PLR74 PLZ72:PLZ74 PMH72:PMH74 PMP72:PMP74 PMX72:PMX74 PNF72:PNF74 PNN72:PNN74 PNV72:PNV74 POD72:POD74 POL72:POL74 POT72:POT74 PPB72:PPB74 PPJ72:PPJ74 PPR72:PPR74 PPZ72:PPZ74 PQH72:PQH74 PQP72:PQP74 PQX72:PQX74 PRF72:PRF74 PRN72:PRN74 PRV72:PRV74 PSD72:PSD74 PSL72:PSL74 PST72:PST74 PTB72:PTB74 PTJ72:PTJ74 PTR72:PTR74 PTZ72:PTZ74 PUH72:PUH74 PUP72:PUP74 PUX72:PUX74 PVF72:PVF74 PVN72:PVN74 PVV72:PVV74 PWD72:PWD74 PWL72:PWL74 PWT72:PWT74 PXB72:PXB74 PXJ72:PXJ74 PXR72:PXR74 PXZ72:PXZ74 PYH72:PYH74 PYP72:PYP74 PYX72:PYX74 PZF72:PZF74 PZN72:PZN74 PZV72:PZV74 QAD72:QAD74 QAL72:QAL74 QAT72:QAT74 QBB72:QBB74 QBJ72:QBJ74 QBR72:QBR74 QBZ72:QBZ74 QCH72:QCH74 QCP72:QCP74 QCX72:QCX74 QDF72:QDF74 QDN72:QDN74 QDV72:QDV74 QED72:QED74 QEL72:QEL74 QET72:QET74 QFB72:QFB74 QFJ72:QFJ74 QFR72:QFR74 QFZ72:QFZ74 QGH72:QGH74 QGP72:QGP74 QGX72:QGX74 QHF72:QHF74 QHN72:QHN74 QHV72:QHV74 QID72:QID74 QIL72:QIL74 QIT72:QIT74 QJB72:QJB74 QJJ72:QJJ74 QJR72:QJR74 QJZ72:QJZ74 QKH72:QKH74 QKP72:QKP74 QKX72:QKX74 QLF72:QLF74 QLN72:QLN74 QLV72:QLV74 QMD72:QMD74 QML72:QML74 QMT72:QMT74 QNB72:QNB74 QNJ72:QNJ74 QNR72:QNR74 QNZ72:QNZ74 QOH72:QOH74 QOP72:QOP74 QOX72:QOX74 QPF72:QPF74 QPN72:QPN74 QPV72:QPV74 QQD72:QQD74 QQL72:QQL74 QQT72:QQT74 QRB72:QRB74 QRJ72:QRJ74 QRR72:QRR74 QRZ72:QRZ74 QSH72:QSH74 QSP72:QSP74 QSX72:QSX74 QTF72:QTF74 QTN72:QTN74 QTV72:QTV74 QUD72:QUD74 QUL72:QUL74 QUT72:QUT74 QVB72:QVB74 QVJ72:QVJ74 QVR72:QVR74 QVZ72:QVZ74 QWH72:QWH74 QWP72:QWP74 QWX72:QWX74 QXF72:QXF74 QXN72:QXN74 QXV72:QXV74 QYD72:QYD74 QYL72:QYL74 QYT72:QYT74 QZB72:QZB74 QZJ72:QZJ74 QZR72:QZR74 QZZ72:QZZ74 RAH72:RAH74 RAP72:RAP74 RAX72:RAX74 RBF72:RBF74 RBN72:RBN74 RBV72:RBV74 RCD72:RCD74 RCL72:RCL74 RCT72:RCT74 RDB72:RDB74 RDJ72:RDJ74 RDR72:RDR74 RDZ72:RDZ74 REH72:REH74 REP72:REP74 REX72:REX74 RFF72:RFF74 RFN72:RFN74 RFV72:RFV74 RGD72:RGD74 RGL72:RGL74 RGT72:RGT74 RHB72:RHB74 RHJ72:RHJ74 RHR72:RHR74 RHZ72:RHZ74 RIH72:RIH74 RIP72:RIP74 RIX72:RIX74 RJF72:RJF74 RJN72:RJN74 RJV72:RJV74 RKD72:RKD74 RKL72:RKL74 RKT72:RKT74 RLB72:RLB74 RLJ72:RLJ74 RLR72:RLR74 RLZ72:RLZ74 RMH72:RMH74 RMP72:RMP74 RMX72:RMX74 RNF72:RNF74 RNN72:RNN74 RNV72:RNV74 ROD72:ROD74 ROL72:ROL74 ROT72:ROT74 RPB72:RPB74 RPJ72:RPJ74 RPR72:RPR74 RPZ72:RPZ74 RQH72:RQH74 RQP72:RQP74 RQX72:RQX74 RRF72:RRF74 RRN72:RRN74 RRV72:RRV74 RSD72:RSD74 RSL72:RSL74 RST72:RST74 RTB72:RTB74 RTJ72:RTJ74 RTR72:RTR74 RTZ72:RTZ74 RUH72:RUH74 RUP72:RUP74 RUX72:RUX74 RVF72:RVF74 RVN72:RVN74 RVV72:RVV74 RWD72:RWD74 RWL72:RWL74 RWT72:RWT74 RXB72:RXB74 RXJ72:RXJ74 RXR72:RXR74 RXZ72:RXZ74 RYH72:RYH74 RYP72:RYP74 RYX72:RYX74 RZF72:RZF74 RZN72:RZN74 RZV72:RZV74 SAD72:SAD74 SAL72:SAL74 SAT72:SAT74 SBB72:SBB74 SBJ72:SBJ74 SBR72:SBR74 SBZ72:SBZ74 SCH72:SCH74 SCP72:SCP74 SCX72:SCX74 SDF72:SDF74 SDN72:SDN74 SDV72:SDV74 SED72:SED74 SEL72:SEL74 SET72:SET74 SFB72:SFB74 SFJ72:SFJ74 SFR72:SFR74 SFZ72:SFZ74 SGH72:SGH74 SGP72:SGP74 SGX72:SGX74 SHF72:SHF74 SHN72:SHN74 SHV72:SHV74 SID72:SID74 SIL72:SIL74 SIT72:SIT74 SJB72:SJB74 SJJ72:SJJ74 SJR72:SJR74 SJZ72:SJZ74 SKH72:SKH74 SKP72:SKP74 SKX72:SKX74 SLF72:SLF74 SLN72:SLN74 SLV72:SLV74 SMD72:SMD74 SML72:SML74 SMT72:SMT74 SNB72:SNB74 SNJ72:SNJ74 SNR72:SNR74 SNZ72:SNZ74 SOH72:SOH74 SOP72:SOP74 SOX72:SOX74 SPF72:SPF74 SPN72:SPN74 SPV72:SPV74 SQD72:SQD74 SQL72:SQL74 SQT72:SQT74 SRB72:SRB74 SRJ72:SRJ74 SRR72:SRR74 SRZ72:SRZ74 SSH72:SSH74 SSP72:SSP74 SSX72:SSX74 STF72:STF74 STN72:STN74 STV72:STV74 SUD72:SUD74 SUL72:SUL74 SUT72:SUT74 SVB72:SVB74 SVJ72:SVJ74 SVR72:SVR74 SVZ72:SVZ74 SWH72:SWH74 SWP72:SWP74 SWX72:SWX74 SXF72:SXF74 SXN72:SXN74 SXV72:SXV74 SYD72:SYD74 SYL72:SYL74 SYT72:SYT74 SZB72:SZB74 SZJ72:SZJ74 SZR72:SZR74 SZZ72:SZZ74 TAH72:TAH74 TAP72:TAP74 TAX72:TAX74 TBF72:TBF74 TBN72:TBN74 TBV72:TBV74 TCD72:TCD74 TCL72:TCL74 TCT72:TCT74 TDB72:TDB74 TDJ72:TDJ74 TDR72:TDR74 TDZ72:TDZ74 TEH72:TEH74 TEP72:TEP74 TEX72:TEX74 TFF72:TFF74 TFN72:TFN74 TFV72:TFV74 TGD72:TGD74 TGL72:TGL74 TGT72:TGT74 THB72:THB74 THJ72:THJ74 THR72:THR74 THZ72:THZ74 TIH72:TIH74 TIP72:TIP74 TIX72:TIX74 TJF72:TJF74 TJN72:TJN74 TJV72:TJV74 TKD72:TKD74 TKL72:TKL74 TKT72:TKT74 TLB72:TLB74 TLJ72:TLJ74 TLR72:TLR74 TLZ72:TLZ74 TMH72:TMH74 TMP72:TMP74 TMX72:TMX74 TNF72:TNF74 TNN72:TNN74 TNV72:TNV74 TOD72:TOD74 TOL72:TOL74 TOT72:TOT74 TPB72:TPB74 TPJ72:TPJ74 TPR72:TPR74 TPZ72:TPZ74 TQH72:TQH74 TQP72:TQP74 TQX72:TQX74 TRF72:TRF74 TRN72:TRN74 TRV72:TRV74 TSD72:TSD74 TSL72:TSL74 TST72:TST74 TTB72:TTB74 TTJ72:TTJ74 TTR72:TTR74 TTZ72:TTZ74 TUH72:TUH74 TUP72:TUP74 TUX72:TUX74 TVF72:TVF74 TVN72:TVN74 TVV72:TVV74 TWD72:TWD74 TWL72:TWL74 TWT72:TWT74 TXB72:TXB74 TXJ72:TXJ74 TXR72:TXR74 TXZ72:TXZ74 TYH72:TYH74 TYP72:TYP74 TYX72:TYX74 TZF72:TZF74 TZN72:TZN74 TZV72:TZV74 UAD72:UAD74 UAL72:UAL74 UAT72:UAT74 UBB72:UBB74 UBJ72:UBJ74 UBR72:UBR74 UBZ72:UBZ74 UCH72:UCH74 UCP72:UCP74 UCX72:UCX74 UDF72:UDF74 UDN72:UDN74 UDV72:UDV74 UED72:UED74 UEL72:UEL74 UET72:UET74 UFB72:UFB74 UFJ72:UFJ74 UFR72:UFR74 UFZ72:UFZ74 UGH72:UGH74 UGP72:UGP74 UGX72:UGX74 UHF72:UHF74 UHN72:UHN74 UHV72:UHV74 UID72:UID74 UIL72:UIL74 UIT72:UIT74 UJB72:UJB74 UJJ72:UJJ74 UJR72:UJR74 UJZ72:UJZ74 UKH72:UKH74 UKP72:UKP74 UKX72:UKX74 ULF72:ULF74 ULN72:ULN74 ULV72:ULV74 UMD72:UMD74 UML72:UML74 UMT72:UMT74 UNB72:UNB74 UNJ72:UNJ74 UNR72:UNR74 UNZ72:UNZ74 UOH72:UOH74 UOP72:UOP74 UOX72:UOX74 UPF72:UPF74 UPN72:UPN74 UPV72:UPV74 UQD72:UQD74 UQL72:UQL74 UQT72:UQT74 URB72:URB74 URJ72:URJ74 URR72:URR74 URZ72:URZ74 USH72:USH74 USP72:USP74 USX72:USX74 UTF72:UTF74 UTN72:UTN74 UTV72:UTV74 UUD72:UUD74 UUL72:UUL74 UUT72:UUT74 UVB72:UVB74 UVJ72:UVJ74 UVR72:UVR74 UVZ72:UVZ74 UWH72:UWH74 UWP72:UWP74 UWX72:UWX74 UXF72:UXF74 UXN72:UXN74 UXV72:UXV74 UYD72:UYD74 UYL72:UYL74 UYT72:UYT74 UZB72:UZB74 UZJ72:UZJ74 UZR72:UZR74 UZZ72:UZZ74 VAH72:VAH74 VAP72:VAP74 VAX72:VAX74 VBF72:VBF74 VBN72:VBN74 VBV72:VBV74 VCD72:VCD74 VCL72:VCL74 VCT72:VCT74 VDB72:VDB74 VDJ72:VDJ74 VDR72:VDR74 VDZ72:VDZ74 VEH72:VEH74 VEP72:VEP74 VEX72:VEX74 VFF72:VFF74 VFN72:VFN74 VFV72:VFV74 VGD72:VGD74 VGL72:VGL74 VGT72:VGT74 VHB72:VHB74 VHJ72:VHJ74 VHR72:VHR74 VHZ72:VHZ74 VIH72:VIH74 VIP72:VIP74 VIX72:VIX74 VJF72:VJF74 VJN72:VJN74 VJV72:VJV74 VKD72:VKD74 VKL72:VKL74 VKT72:VKT74 VLB72:VLB74 VLJ72:VLJ74 VLR72:VLR74 VLZ72:VLZ74 VMH72:VMH74 VMP72:VMP74 VMX72:VMX74 VNF72:VNF74 VNN72:VNN74 VNV72:VNV74 VOD72:VOD74 VOL72:VOL74 VOT72:VOT74 VPB72:VPB74 VPJ72:VPJ74 VPR72:VPR74 VPZ72:VPZ74 VQH72:VQH74 VQP72:VQP74 VQX72:VQX74 VRF72:VRF74 VRN72:VRN74 VRV72:VRV74 VSD72:VSD74 VSL72:VSL74 VST72:VST74 VTB72:VTB74 VTJ72:VTJ74 VTR72:VTR74 VTZ72:VTZ74 VUH72:VUH74 VUP72:VUP74 VUX72:VUX74 VVF72:VVF74 VVN72:VVN74 VVV72:VVV74 VWD72:VWD74 VWL72:VWL74 VWT72:VWT74 VXB72:VXB74 VXJ72:VXJ74 VXR72:VXR74 VXZ72:VXZ74 VYH72:VYH74 VYP72:VYP74 VYX72:VYX74 VZF72:VZF74 VZN72:VZN74 VZV72:VZV74 WAD72:WAD74 WAL72:WAL74 WAT72:WAT74 WBB72:WBB74 WBJ72:WBJ74 WBR72:WBR74 WBZ72:WBZ74 WCH72:WCH74 WCP72:WCP74 WCX72:WCX74 WDF72:WDF74 WDN72:WDN74 WDV72:WDV74 WED72:WED74 WEL72:WEL74 WET72:WET74 WFB72:WFB74 WFJ72:WFJ74 WFR72:WFR74 WFZ72:WFZ74 WGH72:WGH74 WGP72:WGP74 WGX72:WGX74 WHF72:WHF74 WHN72:WHN74 WHV72:WHV74 WID72:WID74 WIL72:WIL74 WIT72:WIT74 WJB72:WJB74 WJJ72:WJJ74 WJR72:WJR74 WJZ72:WJZ74 WKH72:WKH74 WKP72:WKP74 WKX72:WKX74 WLF72:WLF74 WLN72:WLN74 WLV72:WLV74 WMD72:WMD74 WML72:WML74 WMT72:WMT74 WNB72:WNB74 WNJ72:WNJ74 WNR72:WNR74 WNZ72:WNZ74 WOH72:WOH74 WOP72:WOP74 WOX72:WOX74 WPF72:WPF74 WPN72:WPN74 WPV72:WPV74 WQD72:WQD74 WQL72:WQL74 WQT72:WQT74 WRB72:WRB74 WRJ72:WRJ74 WRR72:WRR74 WRZ72:WRZ74 WSH72:WSH74 WSP72:WSP74 WSX72:WSX74 WTF72:WTF74 WTN72:WTN74 WTV72:WTV74 WUD72:WUD74 WUL72:WUL74 WUT72:WUT74 WVB72:WVB74 WVJ72:WVJ74 WVR72:WVR74 WVZ72:WVZ74 WWH72:WWH74 WWP72:WWP74 WWX72:WWX74 WXF72:WXF74 WXN72:WXN74 WXV72:WXV74 WYD72:WYD74 WYL72:WYL74 WYT72:WYT74 WZB72:WZB74 WZJ72:WZJ74 WZR72:WZR74 WZZ72:WZZ74 XAH72:XAH74 XAP72:XAP74 XAX72:XAX74 XBF72:XBF74 XBN72:XBN74 XBV72:XBV74 XCD72:XCD74 XCL72:XCL74 XCT72:XCT74 XDB72:XDB74 XDJ72:XDJ74 XDR72:XDR74 XDZ72:XDZ74 XEH72:XEH74 XEP72:XEP74 XEX72:XEX74 B5:B78</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>